<commit_message>
feat(script): add conditional activities support for BSB zones
Implement getKegiatanBersyarat function to handle B1, B2, B3 activities and their combinations
Update generateExcelBSB and previewZonaBSB to include conditional activities in column V
Add Excel character limit handling for conditional activities data
</commit_message>
<xml_diff>
--- a/app/data/uji titik/uji-titik-bsb.xlsx
+++ b/app/data/uji titik/uji-titik-bsb.xlsx
@@ -752,8 +752,165 @@
       <c r="U3" t="str">
         <v/>
       </c>
-      <c r="V3" t="str">
-        <v/>
+      <c r="V3" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Ekspedisi Muatan Kapal
+Aktivitas Kawasan Alam Lainnya
+Aktivitas Telekomunikasi Lainnya YTDL
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Aktivitas Wisata Air
+Analisis Dan Uji Teknis Lainnya
+Arung Jeram
+Badan Nasional Penanggulangan Bencana Dan Pemadam Kebakaran
+Budidaya Biota Air Laut Lainnya
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Laut
+Budidaya Ikan Hias Air Tawar
+Budidaya Karang
+Daya Tarik Wisata Alam Lainnya
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Internet Service Provider
+Jasa Instalasi Konstruksi Navigasi Laut, Sungai, dan Udara
+Jasa Pekerjaan Konstruksi Pelindung Pantai
+Kawasan Pariwisata
+Kolam Pemancingan
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Telekomunikasi Untuk Prasarana Transportasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Konstruksi Jaringan Irigasi, Komunikasi dan Limbah Lainnya
+Konstruksi Reservoir Pembangkit Listrik Tenaga Air
+Konstruksi Sentral Telekomunikasi
+Pemandian Alam
+Pembangkitan Tenaga Listrik
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembenihan Ikan Laut
+Pembesaran Crustacea Air Payau
+Pembesaran Crustacea Laut
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Kolam
+Pembesaran Ikan Air Tawar Di Sawah
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Mollusca Laut
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Pisces/Ikan Bersirip Laut
+Pembesaran Tumbuhan Air Laut
+Pembesaran Tumbuhan Air Payau
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Penangkapan Biota Air Lainnya Di Laut
+Penangkapan Biota Air Lainnya Di Perairan Darat
+Penangkapan Coelenterata Di Laut
+Penangkapan Crustacea Di Laut
+Penangkapan Crustacea Di Perairan Darat
+Penangkapan Echinodermata Di Laut
+Penangkapan Ikan Hias Laut
+Penangkapan Ikan Hias di Perairan Darat
+Penangkapan Mollusca Di Laut
+Penangkapan Mollusca Di Perairan Darat
+Penangkapan Pisces/Ikan Bersirip Di Laut
+Penangkapan Pisces/Ikan Bersirip Di Perairan Darat
+Penangkapan/Pengambilan Induk/Benih Ikan Di Laut
+Penangkapan/Pengambilan Induk/Benih Ikan Di Perairan darat
+Penangkapan/Pengambilan Tumbuhan Air Di Laut
+Penangkapan/Pengambilan Tumbuhan Air Di Perairan Darat
+Penangkaran Ikan dan Coral/Karang
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Sejarah/Cagar Budaya
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian dan Pengembangan Seni
+Pengembangbiakan Algae Dan Biota Perairan Lainnya Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Amphibia Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Coelenterata Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Crustacea Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Echinodermata Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Ikan Bersirip (Pisces) Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Mamalia Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Mollusca Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengembangbiakan Reptilia Yang Dilindungi Dan/Atau Termasuk Dalam Appendiks CITES
+Pengerukan
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Kerikil/Sirtu
+Penggalian Pasir
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Perbenihan Tanaman Pakan Ternak dan Pembibitan Bit
+Perkebunan Cengkeh
+Perkebunan Lada
+Perkebunan Tanaman Aromatik/Penyegar
+Pertanian Aneka Kacang Holtikultura
+Pertanian Aneka Umbi Palawija
+Pertanian Biji-Bijian Penghasil Bukan Minyak Makan
+Pertanian Biji-Bijian Penghasil Minyak Makan
+Pertanian Bit Gula Dan Tanaman Pemanis Bukan Tebu
+Pertanian Buah Anggur
+Pertanian Buah Apel dan Buah Batu
+Pertanian Buah Beri
+Pertanian Buah Biji Kacang-Kacangan
+Pertanian Buah Jeruk
+Pertanian Buah Semak Lainnya
+Pertanian Buah-Buahan Tropis dan Subtropis
+Pertanian Cabai
+Pertanian Gandum
+Pertanian Holtikultura Buah
+Pertanian Holtikultura Sayuran Buah
+Pertanian Holtikultura Sayuran Daun
+Pertanian Holtikultura Sayuran Umbi
+Pertanian Jagung
+Pertanian Jamur
+Pertanian Kacang Hijau
+Pertanian Kacang Tanah
+Pertanian Kedelai
+Pertanian Padi Hibrida
+Pertanian Padi Inbrida
+Pertanian Pembibitan Tanaman Bunga
+Pertanian Sayuran Tahunan
+Pertanian Sayuran, Buah dan Aneka Umbi Lainnya
+Pertanian Serealia Lainnya, Aneka Kacang dan Biji-Bijian Penghasil Minyak Lainnya
+Pertanian Tanaman Bunga
+Pertanian Tanaman Hias
+Pertanian Tanaman Obat Atau Biofarma Non Rimpang
+Pertanian Tanaman Obat atau Biofarma Rimpang
+Pertanian Tanaman Pakan Ternak
+Pertanian Tanaman Rempah-Rempah, Aromatik/Penyegar dan Obat Lainnya
+Pertanian Tanaman Semusim Lainnya ytdl
+Pertanian Tanaman Untuk Bahan Minuman
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Taman Rekreasi
+Taman Rekreasi/Taman Wisata
+Taman Wisata Alam
+Transmisi Tenaga Listrik
+Wisata Agro
+Wisata Memancing
+Wisata Petualangan Alam
+Wisata Tirta Lainnya</v>
       </c>
       <c r="W3" t="str">
         <v/>
@@ -911,8 +1068,26 @@
       <c r="U4" t="str">
         <v/>
       </c>
-      <c r="V4" t="str">
-        <v/>
+      <c r="V4" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Jalan Tol
+Aktivitas Perparkiran Di Badan Jalan
+Aktivitas Stasiun Kereta Api
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Aktivitas Terminal Darat
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Jalan Rel</v>
       </c>
       <c r="W4" t="str">
         <v/>
@@ -1060,8 +1235,19 @@
       <c r="U5" t="str">
         <v/>
       </c>
-      <c r="V5" t="str">
-        <v/>
+      <c r="V5" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Perekaman Suara
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W5" t="str">
         <v/>
@@ -1202,8 +1388,85 @@
       <c r="U6" t="str">
         <v/>
       </c>
-      <c r="V6" t="str">
-        <v/>
+      <c r="V6" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Cold Storage
+Budidaya Biota Air Laut Lainnya
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Laut
+Budidaya Ikan Hias Air Tawar
+Budidaya Karang
+Daya Tarik Wisata Alam Lainnya
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Telekomunikasi
+Jasa Instalasi Konstruksi Navigasi Laut, Sungai, dan Udara
+Kolam Pemancingan
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Telekomunikasi Untuk Prasarana Transportasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Konstruksi Jaringan Irigasi, Komunikasi dan Limbah Lainnya
+Konstruksi Reservoir Pembangkit Listrik Tenaga Air
+Konstruksi Sentral Telekomunikasi
+Pemanfaatan Hasil Hutan Bukan Kayu
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembenihan Ikan Laut
+Pembesaran Crustacea Air Payau
+Pembesaran Crustacea Laut
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Kolam
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Mollusca Laut
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Pisces/Ikan Bersirip Laut
+Pembesaran Tumbuhan Air Laut
+Pembesaran Tumbuhan Air Payau
+Penangkapan Biota Air Lainnya Di Laut
+Penangkapan Biota Air Lainnya Di Perairan Darat
+Penangkapan Coelenterata Di Laut
+Penangkapan Crustacea Di Laut
+Penangkapan Crustacea Di Perairan Darat
+Penangkapan Echinodermata Di Laut
+Penangkapan Ikan Hias Laut
+Penangkapan Ikan Hias di Perairan Darat
+Penangkapan Mollusca Di Laut
+Penangkapan Mollusca Di Perairan Darat
+Penangkapan Pisces/Ikan Bersirip Di Laut
+Penangkapan Pisces/Ikan Bersirip Di Perairan Darat
+Penangkapan/Pengambilan Induk/Benih Ikan Di Laut
+Penangkapan/Pengambilan Induk/Benih Ikan Di Perairan darat
+Penangkapan/Pengambilan Tumbuhan Air Di Laut
+Penangkapan/Pengambilan Tumbuhan Air Di Perairan Darat
+Penangkaran Ikan dan Coral/Karang
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Sejarah/Cagar Budaya
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian dan Pengembangan Seni
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Taman Rekreasi
+Taman Wisata Alam
+Transmisi Tenaga Listrik
+Wisata Memancing</v>
       </c>
       <c r="W6" t="str">
         <v/>
@@ -1403,8 +1666,27 @@
       <c r="U7" t="str">
         <v/>
       </c>
-      <c r="V7" t="str">
-        <v/>
+      <c r="V7" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Instalasi Elektronika
+Instalasi Konstruksi Lainnya YTDL
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Minyak dan Gas
+Instalasi Pemanas dan Geotermal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan</v>
       </c>
       <c r="W7" t="str">
         <v/>
@@ -1545,8 +1827,110 @@
       <c r="U8" t="str">
         <v/>
       </c>
-      <c r="V8" t="str">
-        <v/>
+      <c r="V8" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Kawasan Alam Lainnya
+Analisis Dan Uji Teknis Lainnya
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Badan Nasional Penanggulangan Bencana Dan Pemadam Kebakaran
+Daya Tarik Wisata Alam Lainnya
+Distribusi Tenaga Listrik
+Hutan Lindung
+Instalasi Listrik
+Instalasi Telekomunikasi
+Jasa Kehutanan Bidang Perencanaan Kehutanan
+Jasa Penggunaan Kawasan Hutan Di Luar Sektor Kehutanan
+Jasa Penunjang Kehutanan Lainnya
+Jasa Perlindungan Hutan dan Konservasi Alam
+Jasa Rehabilitasi Dan Restorasi Kehutanan Sosial
+Jurnalis Berita Independen
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pemandian Alam
+Pemanfaatan Hasil Hutan Bukan Kayu
+Pemungutan Bambu
+Pemungutan Bukan Kayu Lainnya
+Pemungutan Damar
+Pemungutan Daun Kayu Putih
+Pemungutan Getah Karet
+Pemungutan Getah Pinus
+Pemungutan Kokon/Kepompong Ulat Sutera
+Pemungutan Madu
+Pemungutan Rotan
+Penangkaran Burung
+Penangkaran Insekta
+Penangkaran Mamalia
+Penangkaran Primata
+Penangkaran Reptil
+Penangkaran Tumbuhan/Satwa Liar Lainnya
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Sejarah/Cagar Budaya
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian dan Pengembangan Seni
+Peninggalan Sejarah/Cagar Budaya Yang Dikelola Pemerintah
+Perbenihan Tanaman Pakan Ternak dan Pembibitan Bit
+Perburuan dan Penangkapan Burung
+Perburuan dan Penangkapan Insekta
+Perburuan dan Penangkapan Reptil
+Perburuan dan Penangkapan Satwa Liar Lainnya
+Perkebunan Cengkeh
+Perkebunan Lada
+Perkebunan Tanaman Aromatik/Penyegar
+Pertanian Aneka Kacang Holtikultura
+Pertanian Aneka Umbi Palawija
+Pertanian Biji-Bijian Penghasil Bukan Minyak Makan
+Pertanian Biji-Bijian Penghasil Minyak Makan
+Pertanian Bit Gula Dan Tanaman Pemanis Bukan Tebu
+Pertanian Buah Anggur
+Pertanian Buah Apel dan Buah Batu
+Pertanian Buah Beri
+Pertanian Buah Biji Kacang-Kacangan
+Pertanian Buah Jeruk
+Pertanian Buah Semak Lainnya
+Pertanian Buah-Buahan Tropis dan Subtropis
+Pertanian Cabai
+Pertanian Gandum
+Pertanian Holtikultura Buah
+Pertanian Holtikultura Sayuran Buah
+Pertanian Holtikultura Sayuran Daun
+Pertanian Holtikultura Sayuran Umbi
+Pertanian Jagung
+Pertanian Jamur
+Pertanian Kacang Hijau
+Pertanian Kacang Tanah
+Pertanian Kedelai
+Pertanian Padi Hibrida
+Pertanian Padi Inbrida
+Pertanian Pembibitan Tanaman Bunga
+Pertanian Sayuran Tahunan
+Pertanian Sayuran, Buah dan Aneka Umbi Lainnya
+Pertanian Serealia Lainnya, Aneka Kacang dan Biji-Bijian Penghasil Minyak Lainnya
+Pertanian Tanaman Bunga
+Pertanian Tanaman Hias
+Pertanian Tanaman Obat Atau Biofarma Non Rimpang
+Pertanian Tanaman Obat atau Biofarma Rimpang
+Pertanian Tanaman Pakan Ternak
+Pertanian Tanaman Rempah-Rempah, Aromatik/Penyegar dan Obat Lainnya
+Pertanian Tanaman Semusim Lainnya ytdl
+Pertanian Tanaman Untuk Bahan Minuman
+Suaka Margasatwa
+Taman Hutan Raya
+Taman Nasional
+Taman Wisata Alam
+Transmisi Tenaga Listrik
+Wisata Agro</v>
       </c>
       <c r="W8" t="str">
         <v/>
@@ -1687,8 +2071,173 @@
       <c r="U9" t="str">
         <v/>
       </c>
-      <c r="V9" t="str">
-        <v/>
+      <c r="V9" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Kawasan Alam Lainnya
+Aktivitas Perawatan Dan Pemeliharaan Taman
+Aktivitas Perburuan
+Aktivitas Telekomunikasi Tanpa Kabel
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Daya Tarik Wisata Alam Lainnya
+Distribusi Tenaga Listrik
+Distribusi, dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Hutan Lindung
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Kehutanan Bidang Perencanaan Kehutanan
+Jasa Pemanenan
+Jasa Pemupukan, Penanaman Bibit/Benih dan Pengendalian Hama dan Gulma
+Jasa Penggunaan Kawasan Hutan Di Luar Sektor Kehutanan
+Jasa Pengolahan Lahan
+Jasa Penunjang Kehutanan Lainnya
+Jasa Penunjang Pertanian Lainnya
+Jasa Penyemprotan dan Penyerbukan Melalui Udara
+Jasa Perlindungan Hutan dan Konservasi Alam
+Jasa Rehabilitasi Dan Restorasi Kehutanan Sosial
+Kawasan Buru
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Telekomunikasi Untuk Prasarana Transportasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Konstruksi Jaringan Irigasi, Komunikasi dan Limbah Lainnya
+Konstruksi Reservoir Pembangkit Listrik Tenaga Air
+Konstruksi Sentral Telekomunikasi
+Pemanenan Kayu
+Pemanfaatan Hasil Hutan Bukan Kayu
+Pemanfaatan Hutan Kayu Tanaman Hasil Rehabilitasi Pada Hutan Produksi
+Pemanfaatan Hutan Kayu Tanaman Lainnya
+Pemanfaatan Hutan Kayu Tanaman Pada Hutan Produksi
+Pemanfaatan Hutan Kayu Tanaman Rakyat
+Pemanfaatan Kayu Hasil Restorasi Ekosistem Pada Hutan Alam
+Pemanfaatan Kayu Hutan Alam
+Pembangkit, Distribusi, dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Pembangkit, Transmisi, Distribusi dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Pembangkit, Transmisi, dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Pembangkitan Tenaga Listrik
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Pembibitan dan Budidaya Burung Walet
+Pembibitan dan Budidaya Cacing
+Pembibitan dan Budidaya Kelinci
+Pembibitan dan Budidaya Lebah
+Pembibitan dan Budidaya Rusa
+Pemungutan Bambu
+Pemungutan Bukan Kayu Lainnya
+Pemungutan Damar
+Pemungutan Daun Kayu Putih
+Pemungutan Getah Karet
+Pemungutan Getah Pinus
+Pemungutan Kokon/Kepompong Ulat Sutera
+Pemungutan Madu
+Pemungutan Rotan
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Penangkaran Anggrek
+Penangkaran Burung
+Penangkaran Ikan dan Coral/Karang
+Penangkaran Insekta
+Penangkaran Mamalia
+Penangkaran Primata
+Penangkaran Reptil
+Penangkaran Tumbuhan/Satwa Liar Lainnya
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Sejarah/Cagar Budaya
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian dan Pengembangan Seni
+Pengerukan
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Kerikil/Sirtu
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengusahaan Perbenihan Tanaman Kehutanan
+Peninggalan Sejarah/Cagar Budaya Yang Dikelola Pemerintah
+Peninggalan Sejarah/Cagar Budaya Yang Dikelola Swasta
+Perbenihan Tanaman Pakan Ternak dan Pembibitan Bit
+Perkebunan Buah Kelapa
+Perkebunan Buah Kelapa Sawit
+Perkebunan Buah Oleaginous Lainnya
+Perkebunan Cengkeh
+Perkebunan Karet dan Tanaman Penghasil Getah Lainnya
+Perkebunan Lada
+Perkebunan Tanaman Aromatik/Penyegar
+Perkebunan Tebu
+Perkebunan Tembakau
+Pertanian Aneka Kacang Holtikultura
+Pertanian Aneka Umbi Palawija
+Pertanian Biji-Bijian Penghasil Bukan Minyak Makan
+Pertanian Biji-Bijian Penghasil Minyak Makan
+Pertanian Bit Gula Dan Tanaman Pemanis Bukan Tebu
+Pertanian Buah Anggur
+Pertanian Buah Apel dan Buah Batu
+Pertanian Buah Beri
+Pertanian Buah Biji Kacang-Kacangan
+Pertanian Buah Jeruk
+Pertanian Buah Semak Lainnya
+Pertanian Buah-Buahan Tropis dan Subtropis
+Pertanian Cabai
+Pertanian Cemara dan Tanaman Tahunan Lainnya
+Pertanian Gandum
+Pertanian Holtikultura Buah
+Pertanian Holtikultura Sayuran Buah
+Pertanian Holtikultura Sayuran Daun
+Pertanian Holtikultura Sayuran Umbi
+Pertanian Jagung
+Pertanian Jamur
+Pertanian Kacang Hijau
+Pertanian Kacang Tanah
+Pertanian Kedelai
+Pertanian Padi Hibrida
+Pertanian Padi Inbrida
+Pertanian Pembibitan Tanaman Bunga
+Pertanian Pengembangbiakan Tanaman
+Pertanian Sayuran Tahunan
+Pertanian Sayuran, Buah dan Aneka Umbi Lainnya
+Pertanian Serealia Lainnya, Aneka Kacang dan Biji-Bijian Penghasil Minyak Lainnya
+Pertanian Tanaman Berserat
+Pertanian Tanaman Bunga
+Pertanian Tanaman Hias
+Pertanian Tanaman Obat Atau Biofarma Non Rimpang
+Pertanian Tanaman Obat atau Biofarma Rimpang
+Pertanian Tanaman Pakan Ternak
+Pertanian Tanaman Rempah-Rempah, Aromatik/Penyegar dan Obat Lainnya
+Pertanian Tanaman Semusim Lainnya ytdl
+Pertanian Tanaman Untuk Bahan Minuman
+Suaka Margasatwa
+Taman Hutan Raya
+Taman Konservasi Di Luar Habitat Alami
+Taman Nasional
+Taman Wisata Alam
+Transmisi Tenaga Listrik
+Usaha Kehutanan Lainnya
+Usaha Pemungutan Kayu
+Wisata Agro
+Wisata Petualangan Alam</v>
       </c>
       <c r="W9" t="str">
         <v/>
@@ -1829,8 +2378,172 @@
       <c r="U10" t="str">
         <v/>
       </c>
-      <c r="V10" t="str">
-        <v/>
+      <c r="V10" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Kawasan Alam Lainnya
+Aktivitas Perburuan
+Aktivitas Telekomunikasi Tanpa Kabel
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Daya Tarik Wisata Alam Lainnya
+Distribusi Tenaga Listrik
+Distribusi, dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Hutan Lindung
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Kehutanan Bidang Perencanaan Kehutanan
+Jasa Pemanenan
+Jasa Pemupukan, Penanaman Bibit/Benih dan Pengendalian Hama dan Gulma
+Jasa Penggunaan Kawasan Hutan Di Luar Sektor Kehutanan
+Jasa Pengolahan Lahan
+Jasa Penunjang Kehutanan Lainnya
+Jasa Penunjang Pertanian Lainnya
+Jasa Penyemprotan dan Penyerbukan Melalui Udara
+Jasa Perlindungan Hutan dan Konservasi Alam
+Jasa Rehabilitasi Dan Restorasi Kehutanan Sosial
+Kawasan Buru
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Telekomunikasi Untuk Prasarana Transportasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Konstruksi Jaringan Irigasi, Komunikasi dan Limbah Lainnya
+Konstruksi Reservoir Pembangkit Listrik Tenaga Air
+Konstruksi Sentral Telekomunikasi
+Pemanenan Kayu
+Pemanfaatan Hasil Hutan Bukan Kayu
+Pemanfaatan Hutan Kayu Tanaman Hasil Rehabilitasi Pada Hutan Produksi
+Pemanfaatan Hutan Kayu Tanaman Lainnya
+Pemanfaatan Hutan Kayu Tanaman Pada Hutan Produksi
+Pemanfaatan Hutan Kayu Tanaman Rakyat
+Pemanfaatan Kayu Hasil Restorasi Ekosistem Pada Hutan Alam
+Pemanfaatan Kayu Hutan Alam
+Pembangkit, Distribusi, dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Pembangkit, Transmisi, Distribusi dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Pembangkit, Transmisi, dan Penjualan Tenaga Listrik Dalam Satu Kesatuan Usaha
+Pembangkitan Tenaga Listrik
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Pembibitan dan Budidaya Burung Walet
+Pembibitan dan Budidaya Cacing
+Pembibitan dan Budidaya Kelinci
+Pembibitan dan Budidaya Lebah
+Pembibitan dan Budidaya Rusa
+Pemungutan Bambu
+Pemungutan Bukan Kayu Lainnya
+Pemungutan Damar
+Pemungutan Daun Kayu Putih
+Pemungutan Getah Karet
+Pemungutan Getah Pinus
+Pemungutan Kokon/Kepompong Ulat Sutera
+Pemungutan Madu
+Pemungutan Rotan
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Penangkaran Anggrek
+Penangkaran Burung
+Penangkaran Ikan dan Coral/Karang
+Penangkaran Insekta
+Penangkaran Mamalia
+Penangkaran Primata
+Penangkaran Reptil
+Penangkaran Tumbuhan/Satwa Liar Lainnya
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Sejarah/Cagar Budaya
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian dan Pengembangan Seni
+Pengerukan
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Kerikil/Sirtu
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengusahaan Perbenihan Tanaman Kehutanan
+Perbenihan Tanaman Pakan Ternak dan Pembibitan Bit
+Perkebunan Buah Kelapa
+Perkebunan Buah Kelapa Sawit
+Perkebunan Buah Oleaginous Lainnya
+Perkebunan Cengkeh
+Perkebunan Karet dan Tanaman Penghasil Getah Lainnya
+Perkebunan Lada
+Perkebunan Tanaman Aromatik/Penyegar
+Perkebunan Tebu
+Perkebunan Tembakau
+Pertanian Aneka Kacang Holtikultura
+Pertanian Aneka Umbi Palawija
+Pertanian Biji-Bijian Penghasil Bukan Minyak Makan
+Pertanian Biji-Bijian Penghasil Minyak Makan
+Pertanian Bit Gula Dan Tanaman Pemanis Bukan Tebu
+Pertanian Buah Anggur
+Pertanian Buah Apel dan Buah Batu
+Pertanian Buah Beri
+Pertanian Buah Biji Kacang-Kacangan
+Pertanian Buah Jeruk
+Pertanian Buah Semak Lainnya
+Pertanian Buah-Buahan Tropis dan Subtropis
+Pertanian Cabai
+Pertanian Cemara dan Tanaman Tahunan Lainnya
+Pertanian Gandum
+Pertanian Holtikultura Buah
+Pertanian Holtikultura Sayuran Buah
+Pertanian Holtikultura Sayuran Daun
+Pertanian Holtikultura Sayuran Umbi
+Pertanian Jagung
+Pertanian Jamur
+Pertanian Kacang Hijau
+Pertanian Kacang Tanah
+Pertanian Kedelai
+Pertanian Padi Hibrida
+Pertanian Padi Inbrida
+Pertanian Pembibitan Tanaman Bunga
+Pertanian Pengembangbiakan Tanaman
+Pertanian Sayuran Tahunan
+Pertanian Sayuran, Buah dan Aneka Umbi Lainnya
+Pertanian Serealia Lainnya, Aneka Kacang dan Biji-Bijian Penghasil Minyak Lainnya
+Pertanian Tanaman Berserat
+Pertanian Tanaman Bunga
+Pertanian Tanaman Hias
+Pertanian Tanaman Obat Atau Biofarma Non Rimpang
+Pertanian Tanaman Obat atau Biofarma Rimpang
+Pertanian Tanaman Pakan Ternak
+Pertanian Tanaman Rempah-Rempah, Aromatik/Penyegar dan Obat Lainnya
+Pertanian Tanaman Semusim Lainnya ytdl
+Pertanian Tanaman Untuk Bahan Minuman
+Produksi Kompos Sampah Organik
+Suaka Margasatwa
+Taman Hutan Raya
+Taman Konservasi Di Luar Habitat Alami
+Taman Nasional
+Taman Wisata Alam
+Transmisi Tenaga Listrik
+Usaha Kehutanan Lainnya
+Usaha Pemungutan Kayu
+Wisata Agro
+Wisata Petualangan Alam</v>
       </c>
       <c r="W10" t="str">
         <v/>
@@ -1984,8 +2697,23 @@
       <c r="U11" t="str">
         <v/>
       </c>
-      <c r="V11" t="str">
-        <v/>
+      <c r="V11" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Perekaman Suara
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W11" t="str">
         <v/>
@@ -2652,8 +3380,119 @@
       <c r="U12" t="str">
         <v/>
       </c>
-      <c r="V12" t="str">
-        <v/>
+      <c r="V12" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Iindustri Pemberantas Hama
+Industri Air Minum Isi Ulang
+Industri Alat Kesehatan Dalam Subgolongan 2101
+Industri Alat Laboratorium Klinis Dari Kaca
+Industri Alat Laboratorium dan Alat Listrik/Teknik dari Porselen
+Industri Alat-Alat Laboratorium Non Klinis, Farmasi dan Kesehatan Dari Kaca
+Industri Bahan Amelioran
+Industri Bahan Bakar dari Pemurnian dan Pengilangan Minyak Bumi
+Industri Bahan Baku Pemberantas Hama
+Industri Bahan Bangunan Dari Tanah Liat/Keramik Bukan Batu Bata Dan Genteng
+Industri Bahan Farmasi Untuk Hewan
+Industri Bahan Farmasi Untuk Manusia
+Industri Barang Dari Karet Lainnya YTDL
+Industri Barang Dari Karet Untuk Keperluan Industri
+Industri Barang Dari Karet Untuk Keperluan Rumah Tangga
+Industri Barang Dari Karet Untuk Kesehatan
+Industri Barang Dari Plastik Untuk Bangunan
+Industri Barang Dari Plastik Untuk Pengemasan
+Industri Barang Kimia Lainnya YTDL
+Industri Barang Lainnya Dari Kaca
+Industri Barang Plastik Lainnya YTDL
+Industri Barang Plastik Lembaran
+Industri Barang Tahan Api dari Tanah Liat/Keramik Lainnya
+Industri Barang dan Peralatan Teknik/Industri Dari Plastik
+Industri Barang dari Karet Untuk Keperluan Infrastruktur
+Industri Bata, Mortar, Semen, Dan Sejenisnya Yang Tahan Api
+Industri Batu Bata dari Tanah Liat/Keramik
+Industri Briket Batu Bara
+Industri Bumbu Rokok Serta Kelengkapan Rokok Lainnya
+Industri Cat dan Tinta Cetak
+Industri Genteng Dari Tanah Liat/Keramik
+Industri Kaca Lainnya
+Industri Kaca Lembaran
+Industri Kaca Pengaman
+Industri Karet Buatan
+Industri Karet Remah
+Industri Kemacan Dari Kaca
+Industri Kendaraan Perang
+Industri Kimia Dasar Anorganik Gas Industri
+Industri Kimia Dasar Anorganik Khlor dan Alkali
+Industri Kimia Dasar Anorganik Lainnya
+Industri Kimia Dasar Anorganik Pigmen
+Industri Kimia Dasar Organik Lainnya
+Industri Kimia Dasar Organik Untuk Bahan Baku Zat Warna Dan Pigmen, Zat Warna dan Pigmen
+Industri Kimia Dasar Organik Yang Bersumber Dari Hasil Pertanian
+Industri Kimia Dasar Organik Yang Bersumber Dari Minyak Bumi, Gas Alam dan Batu Bara
+Industri Kimia Dasar Organik Yang Menghasilkan Bahan Kimia Khusus
+Industri Kopra
+Industri Lak
+Industri Lokomotif dan Gerbong Kereta
+Industri Malt
+Industri Margarine
+Industri Minuman Beralkohol Hasil Destilasi
+Industri Minuman Beralkohol Hasil Fermentasi Anggur dan Hasil Pertanian Lainnya
+Industri Minuman Beralkohol Hasil Fermentasi Malt
+Industri Minyak Goreng Bukan Minyak Kelapa dan Minyak Kelapa Sawit
+Industri Minyak Goreng Kelapa
+Industri Minyak Goreng Kelapa Sawit
+Industri Minyak Ikan
+Industri Minyak Mentah dan Lemak Hewani Selain Ikan
+Industri Minyak Mentah dan Lemak Nabati
+Industri Minyak Mentah dan Lemak Nabati dan Hewani Lainnya
+Industri Pelet Kelapa
+Industri Pembuatan Minyak Pelumas
+Industri Pengasapan Karet
+Industri Pengeringan dan Pengolahan Tembakau
+Industri Pengolahan Kembali Minyak Pelumas
+Industri Pengolahan Lainnya YTDL
+Industri Pengolahan Minyak Pelumas Bekas Menjadi Bahan Bakar
+Industri Peralatan Saniter Dari Porselen
+Industri Perlengkapan Dan Peralatan Rumah Tangga
+Industri Perlengkapan dan Peralatan Rumah Tangga Dari Kaca
+Industri Pernis
+Industri Pesawat Terbang dan Perlengkapannya
+Industri Pipa Plastik dan Perlengkapannya
+Industri Produk Dari Hasil Kilang Minyak Bumi
+Industri Produk Farmasi Untuk Hewan
+Industri Produk Farmasi Untuk Manusia
+Industri Produk dari Batu Bara
+Industri Remiling Karet
+Industri Rokok Lainnya
+Industri Rokok Putih
+Industri Sigaret Kretek Mesin
+Industri Sigaret Kretek Tangan
+Industri Vulkanisir Ban
+Industri Zat Pengatur Tumbuh
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Mekanikal
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Minyak dan Gas
+Instalasi Pemanas dan Geotermal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Konstruksi Jalan Rel
+Pengerukan
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Lokomotif dan Gerbong Kereta
+Reparasi Peralatan Lainnya
+Reparasi Pesawat Terbang</v>
       </c>
       <c r="W12" t="str">
         <v/>
@@ -2947,8 +3786,108 @@
       <c r="U13" t="str">
         <v/>
       </c>
-      <c r="V13" t="str">
-        <v/>
+      <c r="V13" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Badan Internasional dan badan Ekstra Internasional Lainnya
+Aktivitas Cold Storage
+Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Pelabuhan Perikanan
+Aktivitas Penunjang Angkutan Perairan Lainnya
+Aktivitas Produksi Film, Video dan Program Televisi Oleh Pemerintah
+Aktivitas Produksi Film, Video dan Program Televisi Oleh Swasta
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Wisata Air
+Angkutan Antarkota Dalam Provinsi (AKDP) Bukan Bus, Dalam Trayek
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Bus Antarkota Antar provinsi
+Angkutan Bus Antarkota Dalam Provinsi
+Angkutan Bus Dalam Trayek Lainnya
+Angkutan Bus Khusus
+Angkutan Bus Kota
+Angkutan Bus Pariwisata
+Angkutan Bus Perbatasan
+Angkutan Bus Tidak Dalam Trayek Lainnya
+Angkutan Darat Khusus Bukan Bus
+Angkutan Darat Lainnya Untuk Penumpang
+Angkutan Darat Wisata
+Angkutan Jalan Rel Wisata
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Barang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Barang Khusus
+Angkutan Laut Dalam Negeri Untuk Barang Umum
+Angkutan Laut Dalam Negeri Untuk Pelayaran Rakyat
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Luar Negeri Pelayaran Rakyat
+Angkutan Laut Luar Negeri Untuk Barang Khusus
+Angkutan Laut Luar Negeri Untuk Barang Umum
+Angkutan Laut Luar Negeri Untuk Wisata
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Barang
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Ojek Motor
+Angkutan Penyeberangan Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Dalam Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Lainnya Untuk Barang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Lainnya Untuk Penumpang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Perintis Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Perintis Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Umum Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Umum Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Umum Dalam Kabupaten/Kota Untuk Barang
+Angkutan Perkotaan Bukan Bus, Dalam Trayek
+Angkutan Sewa
+Angkutan Sewa Khusus
+Angkutan Sungai dan Danau Liner (Trayek Tetap dan Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Tramper (Trayek Tidak Tetap dan Tidak Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Untuk Barang Berbahaya
+Angkutan Sungai dan Danau Untuk Barang Khusus
+Angkutan Sungai dan Danau Untuk Barang Umum dan/atau Hewan
+Angkutan Sungai dan Danau Untuk Wisata dan YBDI
+Angkutan Taksi
+Angkutan Tidak Bermotor Untuk Barang Umum
+Angkutan Tidak Bermotor Untuk Penumpang
+Bangunan Pemerintahan
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Dermaga Marina
+Fasilitas Umum dan Fasilitas Sosial Pemerintahan
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Pemanas dan Geotermal
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Telekomunikasi
+Konstruksi Bangunan Pelabuhan Perikanan
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Fasilitas Olahraga
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Pemandian Alam
+Pembesaran Ikan Air Tawar Di Kolam
+Pembuatan/Pengeboran Sumur Air Tanah
+Pengerukan
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Perdagangan Eceran Barang Kerajinan Dari Kayu, Bambu, Rotan, Pandan, Rumput dan Sejenisnya
+Perdagangan Eceran Barang Kerajinan Dari Keramik
+Perdagangan Eceran Lukisan
+Pergudangan dan Penyimpanan
+Pergudangan dan Penyimpanan Lainnya
+Restoran dan Penyediaan Makanan Keliling Lainnya
+Wisata Gua
+Wisata Pantai
+Wisata Petualangan Alam
+Wisata Selam
+Wisata Tirta Lainnya</v>
       </c>
       <c r="W13" t="str">
         <v/>
@@ -3097,8 +4036,22 @@
       <c r="U14" t="str">
         <v/>
       </c>
-      <c r="V14" t="str">
-        <v/>
+      <c r="V14" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Perekaman Suara
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W14" t="str">
         <v/>
@@ -3955,8 +4908,117 @@
       <c r="U15" t="str">
         <v/>
       </c>
-      <c r="V15" t="str">
-        <v/>
+      <c r="V15" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Cold Storage
+Aktivitas Hiburan, Seni Dan Kreativitas Lainnya
+Aktivitas Impresariat Bidang Seni Dan Festival Seni
+Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Operasional Fasilitas Seni
+Aktivitas Pekerja Seni Dan Pekerja Kreatif Lainnya
+Aktivitas Pelaku Kreatif Seni Rupa
+Aktivitas Pemakaman Dan Kegiatan YBDI
+Aktivitas Penulis Dan Pekerja Sastra
+Aktivitas Penunjang Seni Pertunjukan
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Perparkiran Di Badan Jalan
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Seni Pertunjukan
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Lainnya YTDL
+Aktivitas Sosial Pengumpulan Dana Keislaman
+Aktivitas Sosial Pengumpulan Dana Lainnya
+Aktivitas Sosial Swasta Tanpa Akomodasi Lainnya YTDL
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Aktivitas Terminal Darat
+Angkutan Antarkota Dalam Provinsi (AKDP) Bukan Bus, Dalam Trayek
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Bus Antarkota Antar provinsi
+Angkutan Bus Antarkota Dalam Provinsi
+Angkutan Bus Dalam Trayek Lainnya
+Angkutan Bus Khusus
+Angkutan Bus Kota
+Angkutan Bus Lintas Batas Negara
+Angkutan Bus Pariwisata
+Angkutan Bus Perbatasan
+Angkutan Bus Tidak Dalam Trayek Lainnya
+Angkutan Darat Bukan Bus Untuk Penumpang Lainnya Dalam Trayek
+Angkutan Darat Khusus Bukan Bus
+Angkutan Darat Lainnya Untuk Penumpang
+Angkutan Darat Wisata
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Melalui Saluran Pipa
+Angkutan Ojek Motor
+Angkutan Perbatasan Bukan Bus Dalam Trayek
+Angkutan Perdesaan Bukan Bus, Dalam Trayek
+Angkutan Perkotaan Bukan Bus, Dalam Trayek
+Angkutan Sewa
+Angkutan Sewa Khusus
+Angkutan Taksi
+Angkutan Tidak Bermotor Untuk Barang Umum
+Angkutan Tidak Bermotor Untuk Penumpang
+Apartemen Hotel
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Hotel Bintang
+Hotel Melati
+Industri Air Minum Isi Ulang
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Kehutanan Bidang Perencanaan Kehutanan
+Jasa Pelayanan Kesehatan Ternak
+Jasa Pengetasan Telur
+Jasa Penunjang Kehutanan Lainnya
+Jasa Penunjang Peternakan Lainnya
+Jasa Perkawinan Ternak
+Jasa Perlindungan Hutan dan Konservasi Alam
+Jasa Rehabilitasi Dan Restorasi Kehutanan Sosial
+Jurnalis Berita Independen
+Kegiatan Rumah Potong dan Pengepakan Daging Bukan Unggas
+Kegiatan Rumah Potong dan Pengepakan Daging Unggas
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Lainnya YTDL
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Gedung Lainnya
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Konstruksi Jalan Rel
+Kontruksi Gedung Penginapan
+Pelaku Kreatif Seni Musik
+Pelaku Kreatif Seni Pertunjukan
+Pembuatan/Pengeboran Sumur Air Tanah
+Pengelola Gudang Sistem Resi Gudang
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Penyediaan Makanan Keliling/Tempat Tidak Tetap
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Penyimpanan Yang Termasuk Dalam Natturally Occuring Radioactive Material
+Pergudangan dan Penyimpanan Lainnya
+Pondok Wisata
+Restoran dan Penyediaan Makanan Keliling Lainnya
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Villa</v>
       </c>
       <c r="W15" t="str">
         <v/>
@@ -4163,7 +5225,7 @@
         <v/>
       </c>
       <c r="V16" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="W16" t="str">
         <v/>
@@ -4305,7 +5367,7 @@
         <v/>
       </c>
       <c r="V17" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="W17" t="str">
         <v/>
@@ -5162,8 +6224,117 @@
       <c r="U18" t="str">
         <v/>
       </c>
-      <c r="V18" t="str">
-        <v/>
+      <c r="V18" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Cold Storage
+Aktivitas Hiburan, Seni Dan Kreativitas Lainnya
+Aktivitas Impresariat Bidang Seni Dan Festival Seni
+Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Operasional Fasilitas Seni
+Aktivitas Pekerja Seni Dan Pekerja Kreatif Lainnya
+Aktivitas Pelaku Kreatif Seni Rupa
+Aktivitas Pemakaman Dan Kegiatan YBDI
+Aktivitas Penulis Dan Pekerja Sastra
+Aktivitas Penunjang Seni Pertunjukan
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Perparkiran Di Badan Jalan
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Seni Pertunjukan
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Lainnya YTDL
+Aktivitas Sosial Pengumpulan Dana Keislaman
+Aktivitas Sosial Pengumpulan Dana Lainnya
+Aktivitas Sosial Swasta Tanpa Akomodasi Lainnya YTDL
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Aktivitas Terminal Darat
+Angkutan Antarkota Dalam Provinsi (AKDP) Bukan Bus, Dalam Trayek
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Bus Antarkota Antar provinsi
+Angkutan Bus Antarkota Dalam Provinsi
+Angkutan Bus Dalam Trayek Lainnya
+Angkutan Bus Khusus
+Angkutan Bus Kota
+Angkutan Bus Lintas Batas Negara
+Angkutan Bus Pariwisata
+Angkutan Bus Perbatasan
+Angkutan Bus Tidak Dalam Trayek Lainnya
+Angkutan Darat Bukan Bus Untuk Penumpang Lainnya Dalam Trayek
+Angkutan Darat Khusus Bukan Bus
+Angkutan Darat Lainnya Untuk Penumpang
+Angkutan Darat Wisata
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Melalui Saluran Pipa
+Angkutan Ojek Motor
+Angkutan Perbatasan Bukan Bus Dalam Trayek
+Angkutan Perdesaan Bukan Bus, Dalam Trayek
+Angkutan Perkotaan Bukan Bus, Dalam Trayek
+Angkutan Sewa
+Angkutan Sewa Khusus
+Angkutan Taksi
+Angkutan Tidak Bermotor Untuk Barang Umum
+Angkutan Tidak Bermotor Untuk Penumpang
+Apartemen Hotel
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Hotel Bintang
+Hotel Melati
+Industri Air Minum Isi Ulang
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Kehutanan Bidang Perencanaan Kehutanan
+Jasa Pelayanan Kesehatan Ternak
+Jasa Pengetasan Telur
+Jasa Penunjang Kehutanan Lainnya
+Jasa Penunjang Peternakan Lainnya
+Jasa Perkawinan Ternak
+Jasa Perlindungan Hutan dan Konservasi Alam
+Jasa Rehabilitasi Dan Restorasi Kehutanan Sosial
+Jurnalis Berita Independen
+Kegiatan Rumah Potong dan Pengepakan Daging Bukan Unggas
+Kegiatan Rumah Potong dan Pengepakan Daging Unggas
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Lainnya YTDL
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Gedung Lainnya
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Konstruksi Jalan Rel
+Kontruksi Gedung Penginapan
+Pelaku Kreatif Seni Musik
+Pelaku Kreatif Seni Pertunjukan
+Pembuatan/Pengeboran Sumur Air Tanah
+Pengelola Gudang Sistem Resi Gudang
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Penyediaan Makanan Keliling/Tempat Tidak Tetap
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Penyimpanan Yang Termasuk Dalam Natturally Occuring Radioactive Material
+Pergudangan dan Penyimpanan Lainnya
+Pondok Wisata
+Restoran dan Penyediaan Makanan Keliling Lainnya
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Villa</v>
       </c>
       <c r="W18" t="str">
         <v/>
@@ -5370,7 +6541,7 @@
         <v/>
       </c>
       <c r="V19" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="W19" t="str">
         <v/>
@@ -5512,7 +6683,7 @@
         <v/>
       </c>
       <c r="V20" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="W20" t="str">
         <v/>
@@ -6107,8 +7278,52 @@
       <c r="U21" t="str">
         <v/>
       </c>
-      <c r="V21" t="str">
-        <v/>
+      <c r="V21" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Badan Internasional dan badan Ekstra Internasional Lainnya
+Aktivitas Lainnya Yang Berkaitan Dengan Olahraga
+Aktivitas Penunjang Tenaga Listrik Lainnya
+Angkutan Bus Khusus
+Angkutan Darat Lainnya Untuk Penumpang
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Fasilitas Lapangan
+Fasilitas Stadion
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Mekanikal
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Pemanas dan Geotermal
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Telekomunikasi
+Jasa Pendidikan Olahraga Dan Rekreasi
+Klub Sepak Bola
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Fasilitas Olahraga
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Bangunan Sipil Telekomunikasi Untuk Prasarana Transportasi
+Konstruksi Gedung Pendidikan
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Olahragawan, Juri Dan Wasit Profesional
+Pembuatan/Pengeboran Sumur Air Tanah
+Pendidikan Dasar/Ibtidaiyah Pemerintah
+Pendidikan Dasar/Ibtidaiyah Swasta
+Pendidikan Lainnya Pemerintah
+Pendidikan Menengah Atas/Aliyah Pemerintah
+Pendidikan Menengah Kejuruan Dan Teknis/Aliyah Kejuruan Pemerintah
+Pendidikan Menengah Kejuruan/Aliyah Kejuruan Swasta
+Pendidikan Menengah Pertama/Tsanawiyah Pemerintah
+Pendidikan Menengah Pertama/Tsanawiyah Swasta
+Pendidikan Menengah/Aliyah Swasta
+Pendidikan Taman Kanak-Kanak Pemerintah
+Pendidikan Taman Penitipan Anak
+Pendidikan Tinggi Akademik Pemerintah
+Pengelolaan Fasilitas Olah Raga Lainnya
+Pengerukan
+Penyediaan Akomodasi Lainnya
+Penyediaan Minuman Keliling/Tempat Tidak Tetap</v>
       </c>
       <c r="W21" t="str">
         <v/>
@@ -6307,8 +7522,29 @@
       <c r="U22" t="str">
         <v/>
       </c>
-      <c r="V22" t="str">
-        <v/>
+      <c r="V22" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel untuk Penumpang
+Instalasi Elektronika
+Instalasi Konstruksi Lainnya YTDL
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Minyak dan Gas
+Instalasi Pemanas dan Geotermal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan</v>
       </c>
       <c r="W22" t="str">
         <v/>
@@ -6450,8 +7686,140 @@
       <c r="U23" t="str">
         <v/>
       </c>
-      <c r="V23" t="str">
-        <v/>
+      <c r="V23" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Analisis Dan Uji Teknis Lainnya
+Badan Nasional Penanggulangan Bencana Dan Pemadam Kebakaran
+Budidaya Biota Air Laut Lainnya
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Laut
+Budidaya Ikan Hias Air Tawar
+Budidaya Karang
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Instalasi Konstruksi Navigasi Laut, Sungai, dan Udara
+Jasa Pekerjaan Konstruksi Pelindung Pantai
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Telekomunikasi Untuk Prasarana Transportasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Konstruksi Jaringan Irigasi, Komunikasi dan Limbah Lainnya
+Konstruksi Reservoir Pembangkit Listrik Tenaga Air
+Konstruksi Sentral Telekomunikasi
+Pembangkitan Tenaga Listrik
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembenihan Ikan Laut
+Pembesaran Crustacea Air Payau
+Pembesaran Crustacea Laut
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Kolam
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Mollusca Laut
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Pisces/Ikan Bersirip Laut
+Pembesaran Tumbuhan Air Laut
+Pembesaran Tumbuhan Air Payau
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Penangkapan Biota Air Lainnya Di Laut
+Penangkapan Biota Air Lainnya Di Perairan Darat
+Penangkapan Coelenterata Di Laut
+Penangkapan Crustacea Di Laut
+Penangkapan Crustacea Di Perairan Darat
+Penangkapan Echinodermata Di Laut
+Penangkapan Ikan Hias Laut
+Penangkapan Ikan Hias di Perairan Darat
+Penangkapan Mollusca Di Laut
+Penangkapan Mollusca Di Perairan Darat
+Penangkapan Pisces/Ikan Bersirip Di Laut
+Penangkapan Pisces/Ikan Bersirip Di Perairan Darat
+Penangkapan/Pengambilan Induk/Benih Ikan Di Laut
+Penangkapan/Pengambilan Induk/Benih Ikan Di Perairan darat
+Penangkapan/Pengambilan Tumbuhan Air Di Laut
+Penangkapan/Pengambilan Tumbuhan Air Di Perairan Darat
+Penangkaran Anggrek
+Penangkaran Ikan dan Coral/Karang
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Sejarah/Cagar Budaya
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian dan Pengembangan Seni
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Perbenihan Tanaman Pakan Ternak dan Pembibitan Bit
+Perkebunan Buah Kelapa
+Perkebunan Buah Kelapa Sawit
+Perkebunan Buah Oleaginous Lainnya
+Perkebunan Cengkeh
+Perkebunan Lada
+Perkebunan Tanaman Aromatik/Penyegar
+Perkebunan Tebu
+Perkebunan Tembakau
+Pertanian Aneka Kacang Holtikultura
+Pertanian Aneka Umbi Palawija
+Pertanian Biji-Bijian Penghasil Bukan Minyak Makan
+Pertanian Biji-Bijian Penghasil Minyak Makan
+Pertanian Bit Gula Dan Tanaman Pemanis Bukan Tebu
+Pertanian Buah Anggur
+Pertanian Buah Apel dan Buah Batu
+Pertanian Buah Beri
+Pertanian Buah Biji Kacang-Kacangan
+Pertanian Buah Jeruk
+Pertanian Buah Semak Lainnya
+Pertanian Buah-Buahan Tropis dan Subtropis
+Pertanian Cabai
+Pertanian Cemara dan Tanaman Tahunan Lainnya
+Pertanian Gandum
+Pertanian Holtikultura Buah
+Pertanian Holtikultura Sayuran Buah
+Pertanian Holtikultura Sayuran Daun
+Pertanian Holtikultura Sayuran Umbi
+Pertanian Jagung
+Pertanian Jamur
+Pertanian Kacang Hijau
+Pertanian Kacang Tanah
+Pertanian Kedelai
+Pertanian Padi Hibrida
+Pertanian Padi Inbrida
+Pertanian Pembibitan Tanaman Bunga
+Pertanian Pengembangbiakan Tanaman
+Pertanian Sayuran Tahunan
+Pertanian Sayuran, Buah dan Aneka Umbi Lainnya
+Pertanian Serealia Lainnya, Aneka Kacang dan Biji-Bijian Penghasil Minyak Lainnya
+Pertanian Tanaman Berserat
+Pertanian Tanaman Bunga
+Pertanian Tanaman Hias
+Pertanian Tanaman Obat Atau Biofarma Non Rimpang
+Pertanian Tanaman Obat atau Biofarma Rimpang
+Pertanian Tanaman Pakan Ternak
+Pertanian Tanaman Rempah-Rempah, Aromatik/Penyegar dan Obat Lainnya
+Pertanian Tanaman Semusim Lainnya ytdl
+Pertanian Tanaman Untuk Bahan Minuman
+Taman Rekreasi
+Taman Wisata Alam
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W23" t="str">
         <v/>
@@ -6627,8 +7995,22 @@
       <c r="U24" t="str">
         <v/>
       </c>
-      <c r="V24" t="str">
-        <v/>
+      <c r="V24" t="str" xml:space="preserve">
+        <v xml:space="preserve">Instalasi Elektronika
+Instalasi Listrik
+Instalasi Mekanikal
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Pemanas dan Geotermal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Telekomunikasi
+Jasa Instalasi Konstruksi Navigasi Laut, Sungai, dan Udara
+Konstruksi Bangunan Sipil Telekomunikasi Untuk Prasarana Transportasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Pengerukan
+Penyediaan Jasa Boga Periode Tertentu</v>
       </c>
       <c r="W24" t="str">
         <v/>
@@ -7526,8 +8908,95 @@
       <c r="U25" t="str">
         <v/>
       </c>
-      <c r="V25" t="str">
-        <v/>
+      <c r="V25" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Cold Storage
+Aktivitas Hiburan, Seni Dan Kreativitas Lainnya
+Aktivitas Impresariat Bidang Seni Dan Festival Seni
+Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Operasional Fasilitas Seni
+Aktivitas Pekerja Seni Dan Pekerja Kreatif Lainnya
+Aktivitas Pelaku Kreatif Seni Rupa
+Aktivitas Pemakaman Dan Kegiatan YBDI
+Aktivitas Penulis Dan Pekerja Sastra
+Aktivitas Penunjang Seni Pertunjukan
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Seni Pertunjukan
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Lainnya YTDL
+Aktivitas Sosial Pengumpulan Dana Keislaman
+Aktivitas Sosial Pengumpulan Dana Lainnya
+Aktivitas Sosial Swasta Tanpa Akomodasi Lainnya YTDL
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Bangunan Pemerintahan
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Fasilitas Stadion
+Fasilitas Umum dan Fasilitas Sosial Pemerintahan
+Instalasi Konstruksi Lainnya YTDL
+Instalasi Listrik
+Instalasi Mekanikal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Kehutanan Bidang Perencanaan Kehutanan
+Jasa Pekerjaan Konstruksi Pelindung Pantai
+Jasa Pekerjaan Konstruksi Prapabrikasi Bangunan Gedung
+Jasa Pengurusan Transportasi
+Jasa Penunjang Kehutanan Lainnya
+Jasa Perlindungan Hutan dan Konservasi Alam
+Jasa Rehabilitasi Dan Restorasi Kehutanan Sosial
+Jurnalis Berita Independen
+Kegiatan Rumah Potong dan Pengepakan Daging Bukan Unggas
+Kegiatan Rumah Potong dan Pengepakan Daging Unggas
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Fasilitas Olahraga
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Lainnya YTDL
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Gedung Lainnya
+Konstruksi Jalan Rel
+Kontruksi Gedung Penginapan
+Pelaku Kreatif Seni Musik
+Pelaku Kreatif Seni Pertunjukan
+Pembongkaran
+Pembuatan/Pengeboran Sumur Air Tanah
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Pengelola Gudang Sistem Resi Gudang
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Peninggalan Sejarah/Cagar Budaya Yang Dikelola Pemerintah
+Peninggalan Sejarah/Cagar Budaya Yang Dikelola Swasta
+Penjualan Tenaga Listrik
+Penyediaan Jasa Boga Periode Tertentu
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Penyiapan Lahan
+Pergudangan dan Penyimpanan
+Pergudangan dan Penyimpanan Lainnya
+Restoran dan Penyediaan Makanan Keliling Lainnya
+Tempat Peribadatan
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya</v>
       </c>
       <c r="W25" t="str">
         <v/>
@@ -8423,8 +9892,93 @@
       <c r="U26" t="str">
         <v/>
       </c>
-      <c r="V26" t="str">
-        <v/>
+      <c r="V26" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Cold Storage
+Aktivitas Hiburan, Seni Dan Kreativitas Lainnya
+Aktivitas Impresariat Bidang Seni Dan Festival Seni
+Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Operasional Fasilitas Seni
+Aktivitas Pekerja Seni Dan Pekerja Kreatif Lainnya
+Aktivitas Pelaku Kreatif Seni Rupa
+Aktivitas Pemakaman Dan Kegiatan YBDI
+Aktivitas Penulis Dan Pekerja Sastra
+Aktivitas Penunjang Seni Pertunjukan
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Seni Pertunjukan
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Lainnya YTDL
+Aktivitas Sosial Pengumpulan Dana Keislaman
+Aktivitas Sosial Pengumpulan Dana Lainnya
+Aktivitas Sosial Swasta Tanpa Akomodasi Lainnya YTDL
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Bangunan Pemerintahan
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Fasilitas Stadion
+Fasilitas Umum dan Fasilitas Sosial Pemerintahan
+Instalasi Konstruksi Lainnya YTDL
+Instalasi Listrik
+Instalasi Mekanikal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Kehutanan Bidang Perencanaan Kehutanan
+Jasa Pekerjaan Konstruksi Pelindung Pantai
+Jasa Pekerjaan Konstruksi Prapabrikasi Bangunan Gedung
+Jasa Pengurusan Transportasi
+Jasa Penunjang Kehutanan Lainnya
+Jasa Perlindungan Hutan dan Konservasi Alam
+Jasa Rehabilitasi Dan Restorasi Kehutanan Sosial
+Jurnalis Berita Independen
+Kegiatan Rumah Potong dan Pengepakan Daging Bukan Unggas
+Kegiatan Rumah Potong dan Pengepakan Daging Unggas
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Fasilitas Olahraga
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Lainnya YTDL
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Gedung Lainnya
+Konstruksi Jalan Rel
+Kontruksi Gedung Penginapan
+Pelaku Kreatif Seni Musik
+Pelaku Kreatif Seni Pertunjukan
+Pembongkaran
+Pembuatan/Pengeboran Sumur Air Tanah
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Pengelola Gudang Sistem Resi Gudang
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Penyediaan Jasa Boga Periode Tertentu
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Penyiapan Lahan
+Pergudangan dan Penyimpanan
+Pergudangan dan Penyimpanan Lainnya
+Restoran dan Penyediaan Makanan Keliling Lainnya
+Tempat Peribadatan
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya</v>
       </c>
       <c r="W26" t="str">
         <v/>
@@ -9273,8 +10827,89 @@
       <c r="U27" t="str">
         <v/>
       </c>
-      <c r="V27" t="str">
-        <v/>
+      <c r="V27" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Cold Storage
+Aktivitas Hiburan, Seni Dan Kreativitas Lainnya
+Aktivitas Impresariat Bidang Seni Dan Festival Seni
+Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Operasional Fasilitas Seni
+Aktivitas Pekerja Seni Dan Pekerja Kreatif Lainnya
+Aktivitas Pelaku Kreatif Seni Rupa
+Aktivitas Pemakaman Dan Kegiatan YBDI
+Aktivitas Penulis Dan Pekerja Sastra
+Aktivitas Penunjang Seni Pertunjukan
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Seni Pertunjukan
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Lainnya YTDL
+Aktivitas Sosial Pengumpulan Dana Keislaman
+Aktivitas Sosial Pengumpulan Dana Lainnya
+Aktivitas Sosial Swasta Tanpa Akomodasi Lainnya YTDL
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Bangunan Pemerintahan
+Daya Tarik Wisata Buatan/Binaan Manusia Lainnya
+Fasilitas Stadion
+Fasilitas Umum dan Fasilitas Sosial Pemerintahan
+Instalasi Konstruksi Lainnya YTDL
+Instalasi Listrik
+Instalasi Mekanikal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Jasa Pekerjaan Konstruksi Pelindung Pantai
+Jasa Pekerjaan Konstruksi Prapabrikasi Bangunan Gedung
+Jasa Pengurusan Transportasi
+Jurnalis Berita Independen
+Kegiatan Rumah Potong dan Pengepakan Daging Bukan Unggas
+Kegiatan Rumah Potong dan Pengepakan Daging Unggas
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Fasilitas Olahraga
+Konstruksi Bangunan Sipil Jembatan, Jalan Layang, Fly Over dan Underpass
+Konstruksi Bangunan Sipil Lainnya YTDL
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Gedung Lainnya
+Konstruksi Jalan Rel
+Kontruksi Gedung Penginapan
+Pelaku Kreatif Seni Musik
+Pelaku Kreatif Seni Pertunjukan
+Pembongkaran
+Pembuatan/Pengeboran Sumur Air Tanah
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Pengelola Gudang Sistem Resi Gudang
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Penyediaan Jasa Boga Periode Tertentu
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Penyiapan Lahan
+Pergudangan dan Penyimpanan
+Pergudangan dan Penyimpanan Lainnya
+Restoran dan Penyediaan Makanan Keliling Lainnya
+Tempat Peribadatan
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya</v>
       </c>
       <c r="W27" t="str">
         <v/>
@@ -9440,8 +11075,21 @@
       <c r="U28" t="str">
         <v/>
       </c>
-      <c r="V28" t="str">
-        <v/>
+      <c r="V28" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penyiaran dan Pemrograman Televisi Oleh Pemerintah
+Aktivitas Penyiaran dan Pemrograman Televisi Oleh Swasta
+Aktivitas Produksi Film, Video dan Program Televisi Oleh Pemerintah
+Aktivitas Produksi Film, Video dan Program Televisi Oleh Swasta
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Pemanas dan Geotermal
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Telekomunikasi
+Jasa Instalasi Konstruksi Navigasi Laut, Sungai, dan Udara
+Konstruksi Bangunan Sipil Panas Bumi
+Konstruksi Jalan Rel</v>
       </c>
       <c r="W28" t="str">
         <v/>
@@ -9939,8 +11587,49 @@
       <c r="U29" t="str">
         <v/>
       </c>
-      <c r="V29" t="str">
-        <v/>
+      <c r="V29" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Pembuatan/Pengeboran Sumur Air Tanah
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya</v>
       </c>
       <c r="W29" t="str">
         <v/>
@@ -10438,8 +12127,49 @@
       <c r="U30" t="str">
         <v/>
       </c>
-      <c r="V30" t="str">
-        <v/>
+      <c r="V30" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Pembuatan/Pengeboran Sumur Air Tanah
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya</v>
       </c>
       <c r="W30" t="str">
         <v/>
@@ -10937,8 +12667,50 @@
       <c r="U31" t="str">
         <v/>
       </c>
-      <c r="V31" t="str">
-        <v/>
+      <c r="V31" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Industri Peralatan Iradiasi/Sinar X, Perlengkapan dan Sejenisnya
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Pembuatan/Pengeboran Sumur Air Tanah
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya</v>
       </c>
       <c r="W31" t="str">
         <v/>
@@ -11432,8 +13204,48 @@
       <c r="U32" t="str">
         <v/>
       </c>
-      <c r="V32" t="str">
-        <v/>
+      <c r="V32" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Klinik Pemerintah
+Aktivitas Klinik Swasta
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyimpanan B3
+Aktivitas Puskesmas
+Aktivitas Rumah Sakit Lainnya
+Aktivitas Rumah Sakit Pemerintah
+Aktivitas Rumah Sakit Swasta
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Angkutan Jalan Rel Lainnya
+Angkutan Jalan Rel Perkotaan
+Angkutan Jalan Rel Untuk Barang
+Angkutan Jalan Rel Wisata
+Angkutan Jalan Rel untuk Penumpang
+Instalasi Elektronika
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Saluran Air
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Bangunan Prasarana Sumber Daya Air
+Konstruksi Bangunan Sipil Elektrikal
+Konstruksi Bangunan Sipil Pengolahan Air Bersih
+Konstruksi Bangunan Sipil Prasarana dan Sarana Sistem Pengolahan Limbah Padat, Cair dan Gas
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Pembuatan/Pengeboran Sumur Air Tanah
+Penampungan dan Penyaluran Air Baku
+Penampungan, Penjernihan dan Penyaluran Air Minum
+Pengerukan
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Pengumpulan Air Limbah Tidak Berbahaya
+Penjualan Tenaga Listrik
+Treatment dan Pembuangan Air Limbah Tidak Berbahaya</v>
       </c>
       <c r="W32" t="str">
         <v/>
@@ -11620,8 +13432,27 @@
       <c r="U33" t="str">
         <v/>
       </c>
-      <c r="V33" t="str">
-        <v/>
+      <c r="V33" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Pemutaran Film
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Rekreasi Dan Olahraga
+Aktivitas Perekaman Suara
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Penyediaan Jasa Boga Periode Tertentu
+Penyediaan Makanan Keliling/Tempat Tidak Tetap
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W33" t="str">
         <v/>
@@ -11807,8 +13638,27 @@
       <c r="U34" t="str">
         <v/>
       </c>
-      <c r="V34" t="str">
-        <v/>
+      <c r="V34" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Pemutaran Film
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Rekreasi Dan Olahraga
+Aktivitas Perekaman Suara
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Penyediaan Jasa Boga Periode Tertentu
+Penyediaan Makanan Keliling/Tempat Tidak Tetap
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W34" t="str">
         <v/>
@@ -11995,8 +13845,27 @@
       <c r="U35" t="str">
         <v/>
       </c>
-      <c r="V35" t="str">
-        <v/>
+      <c r="V35" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Pemutaran Film
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Rekreasi Dan Olahraga
+Aktivitas Perekaman Suara
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Penyediaan Jasa Boga Periode Tertentu
+Penyediaan Makanan Keliling/Tempat Tidak Tetap
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W35" t="str">
         <v/>
@@ -12149,8 +14018,22 @@
       <c r="U36" t="str">
         <v/>
       </c>
-      <c r="V36" t="str">
-        <v/>
+      <c r="V36" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Perekaman Suara
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W36" t="str">
         <v/>
@@ -12327,8 +14210,25 @@
       <c r="U37" t="str">
         <v/>
       </c>
-      <c r="V37" t="str">
-        <v/>
+      <c r="V37" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Aktivitas Perekaman Suara
+Aktivitas Telekomunikasi Satelit
+Aktivitas Telekomunikasi Tanpa Kabel
+Aktivitas Telekomunikasi dengan Kabel
+Distribusi Tenaga Listrik
+Instalasi Listrik
+Instalasi Saluran Air
+Instalasi Telekomunikasi
+Konstruksi Bangunan Sipil Jalan
+Konstruksi Jalan Rel
+Konstruksi Sentral Telekomunikasi
+Pengoperasian Instalasi Pemanfaatan Tenaga Listrik
+Pengoperasian Instalasi Penyediaan Tenaga Listrik
+Penyediaan Jasa Boga Periode Tertentu
+Penyediaan Makanan Keliling/Tempat Tidak Tetap
+Penyediaan Minuman Keliling/Tempat Tidak Tetap
+Transmisi Tenaga Listrik</v>
       </c>
       <c r="W37" t="str">
         <v/>
@@ -12488,8 +14388,29 @@
       <c r="U38" t="str">
         <v/>
       </c>
-      <c r="V38" t="str">
-        <v/>
+      <c r="V38" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Angkutan Udara Khusus Pemotretan, Survei Dan Pemetaan
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Industri Penggilingan Padi dan Penyosohan Beras
+Instalasi Elektronika
+Instalasi Konstruksi Lainnya YTDL
+Instalasi Listrik
+Instalasi Meteorologi, Klimatologi dan Geofisika
+Instalasi Minyak dan Gas
+Instalasi Pemanas dan Geotermal
+Instalasi Pendingin dan Ventilasi Udara
+Instalasi Saluran Air
+Instalasi Sinyal dan Rambu-rambu Jalan Raya
+Instalasi Sinyal dan Telekomunikasi Kereta Api
+Instalasi Telekomunikasi
+Konstruksi Jalan Rel
+Konstruksi Jaringan Irigasi dan Drainase
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Wisata Agro</v>
       </c>
       <c r="W38" t="str">
         <v/>

</xml_diff>

<commit_message>
feat(intensitas): add arteri road support and kegiatan bersyarat terbatas
- Add new fields for arteri road in intensitas data processing
- Implement kegiatan bersyarat terbatas (T+B combinations) in BSB Excel generation
- Update UI components to display arteri road data for BSB source
- Adjust path references in process-intensitas-separate.js
</commit_message>
<xml_diff>
--- a/app/data/uji titik/uji-titik-bsb.xlsx
+++ b/app/data/uji titik/uji-titik-bsb.xlsx
@@ -924,8 +924,49 @@
       <c r="Z3" t="str">
         <v/>
       </c>
-      <c r="AA3" t="str">
-        <v/>
+      <c r="AA3" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Pelabuhan Perikanan
+Aktivitas Pelayanan Kepelabuhanan Laut
+Aktivitas Pelayanan Kepelabuhanan Penyeberangan
+Aktivitas Pelayanan Kepelabuhanan Sungai dan Danau
+Aktivitas Pengelolaan Kapal
+Aktivitas Penunjang Angkutan Perairan Lainnya
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Barang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Barang Khusus
+Angkutan Laut Dalam Negeri Untuk Barang Umum
+Angkutan Laut Dalam Negeri Untuk Pelayaran Rakyat
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Luar Negeri Pelayaran Rakyat
+Angkutan Laut Luar Negeri Untuk Barang Khusus
+Angkutan Laut Luar Negeri Untuk Barang Umum
+Angkutan Laut Luar Negeri Untuk Wisata
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Barang
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Penyeberangan Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Dalam Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Lainnya Untuk Barang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Lainnya Untuk Penumpang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Perintis Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Perintis Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Umum Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Umum Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Umum Dalam Kabupaten/Kota Untuk Barang
+Angkutan Sungai dan Danau Liner (Trayek Tetap dan Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Tramper (Trayek Tidak Tetap dan Tidak Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Untuk Barang Berbahaya
+Angkutan Sungai dan Danau Untuk Barang Khusus
+Angkutan Sungai dan Danau Untuk Barang Umum dan/atau Hewan
+Angkutan Sungai dan Danau Untuk Wisata dan YBDI
+Jasa Pengurusan Transportasi
+Konstruksi Bangunan Pelabuhan Bukan Perikanan
+Konstruksi Bangunan Pelabuhan Perikanan
+Penanganan Kargo</v>
       </c>
       <c r="AB3" t="str">
         <v/>
@@ -1101,8 +1142,10 @@
       <c r="Z4" t="str">
         <v/>
       </c>
-      <c r="AA4" t="str">
-        <v/>
+      <c r="AA4" t="str" xml:space="preserve">
+        <v xml:space="preserve">Konstruksi Bangunan Pelabuhan Bukan Perikanan
+Konstruksi Bangunan Pelabuhan Perikanan
+Periklanan</v>
       </c>
       <c r="AB4" t="str">
         <v/>
@@ -1262,7 +1305,7 @@
         <v/>
       </c>
       <c r="AA5" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB5" t="str">
         <v/>
@@ -1481,7 +1524,7 @@
         <v/>
       </c>
       <c r="AA6" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB6" t="str">
         <v/>
@@ -1700,8 +1743,91 @@
       <c r="Z7" t="str">
         <v/>
       </c>
-      <c r="AA7" t="str">
-        <v/>
+      <c r="AA7" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Budidaya Biota Air Laut Lainnya
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Tawar
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Fasilitas Umum dan Fasilitas Sosial Pemerintahan
+Jasa Pasca Panen
+Jasa Pasca Panen Budidaya Ikan Air Payau
+Jasa Pasca Panen Budidaya Ikan Air Tawar
+Jasa Pasca Panen Budidaya Ikan Laut
+Jasa Pelayanan Kesehatan Ternak
+Jasa Pemanenan
+Jasa Pemupukan, Penanaman Bibit/Benih dan Pengendalian Hama dan Gulma
+Jasa Pengetasan Telur
+Jasa Pengolahan Lahan
+Jasa Penunjang Pertanian Lainnya
+Jasa Penunjang Peternakan Lainnya
+Jasa Penyemprotan dan Penyerbukan Melalui Udara
+Jasa Perkawinan Ternak
+Jasa Produksi Budidaya Ikan Air Payau
+Jasa Produksi Budidaya Ikan Air Tawar
+Jasa Produksi Budidaya Ikan Laut
+Jasa Sarana Produksi Budidaya Ikan Air Payau
+Jasa Sarana Produksi Budidaya Ikan Air Tawar
+Jasa Sarana Produksi Budidaya Ikan Laut
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembesaran Crustacea Air Payau
+Pembesaran Crustacea Laut
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Kolam
+Pembesaran Ikan Air Tawar Di Sawah
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Tumbuhan Air Laut
+Pembesaran Tumbuhan Air Payau
+Pembibitan dan Budidaya Burung Walet
+Pembibitan dan Budidaya Lebah
+Pemilihan Benih Tanaman Untuk Pengembangbiakan
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Rumah Tinggal
+Tempat Peribadatan</v>
       </c>
       <c r="AB7" t="str">
         <v/>
@@ -1945,7 +2071,7 @@
         <v/>
       </c>
       <c r="AA8" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB8" t="str">
         <v/>
@@ -2251,8 +2377,45 @@
       <c r="Z9" t="str">
         <v/>
       </c>
-      <c r="AA9" t="str">
-        <v/>
+      <c r="AA9" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Instalasi Elektronika
+Konstruksi Bangunan Pelabuhan Bukan Perikanan
+Konstruksi Bangunan Pelabuhan Perikanan
+Penggalian Asbes
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium</v>
       </c>
       <c r="AB9" t="str">
         <v/>
@@ -2557,8 +2720,51 @@
       <c r="Z10" t="str">
         <v/>
       </c>
-      <c r="AA10" t="str">
-        <v/>
+      <c r="AA10" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Pelabuhan Perikanan
+Aktivitas Pelayanan Kepelabuhanan Laut
+Aktivitas Pelayanan Kepelabuhanan Penyeberangan
+Aktivitas Pelayanan Kepelabuhanan Sungai dan Danau
+Aktivitas Penunjang Angkutan Perairan Lainnya
+Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Instalasi Elektronika
+Konstruksi Bangunan Pelabuhan Bukan Perikanan
+Konstruksi Bangunan Pelabuhan Perikanan
+Penggalian Asbes
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Tras
+Pengumpulan Limbah dan Sampah Tidak Berbahaya
+Pengusahaaan Tenaga Panas Bumi
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium</v>
       </c>
       <c r="AB10" t="str">
         <v/>
@@ -2727,8 +2933,9 @@
       <c r="Z11" t="str">
         <v/>
       </c>
-      <c r="AA11" t="str">
-        <v/>
+      <c r="AA11" t="str" xml:space="preserve">
+        <v xml:space="preserve">Periklanan
+Taman Rekreasi</v>
       </c>
       <c r="AB11" t="str">
         <v/>
@@ -3506,8 +3713,264 @@
       <c r="Z12" t="str">
         <v/>
       </c>
-      <c r="AA12" t="str">
-        <v/>
+      <c r="AA12" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Agen Perjalanan Ibadah Umroh Dan Haji Khusus
+Aktivitas Agen Perjalanan Lainnya
+Aktivitas Agen Perjalanan Wisata
+Aktivitas Akuntansi, Pembukuan Dan Pemeriksa
+Aktivitas Arsitektur
+Aktivitas Biro Perjalanan Ibadah Umroh Dan Haji Khusus
+Aktivitas Biro Perjalanan Lainnya
+Aktivitas Biro Perjalanan Wisata
+Aktivitas Desain Alat Komunikasi Dan Elektronika
+Aktivitas Desain Alat Transportasi Dan Permesinan
+Aktivitas Desain Industri Lainnya
+Aktivitas Desain Industri Strategis Dan Pertahanan
+Aktivitas Desain Interior
+Aktivitas Desain Khusus Film, Video, Program Tv, Animasi Dan Komik
+Aktivitas Desain Komunikasi Visual/ Desain Grafis
+Aktivitas Desain Konten Game
+Aktivitas Desain Konten Kreatif Lainya
+Aktivitas Desain Pengemasan
+Aktivitas Desain Peralatan Olahraga Dan Permainan
+Aktivitas Desain Peralatan Rumah Tangga Dan Furnitur
+Aktivitas Desain Produk Kesehatan, Kosmetik Dan Perlengkapan Laboratorium
+Aktivitas Desain Tekstil, Fashion Dan Apparel
+Aktivitas Fotografi
+Aktivitas Fotokopi, Penyiapan Dokumen Dan Aktivitas Khusus Penunjang Kantor Lainnya
+Aktivitas Hukum Lainnya
+Aktivitas Jasa Sistem Keamanan
+Aktivitas Kantor Berita Oleh Pemerintah
+Aktivitas Kantor Berita Oleh Swasta
+Aktivitas Kantor Pusat
+Aktivitas Keamanan Swasta
+Aktivitas Kebersihan Bangunan Dan Industri Lainnya
+Aktivitas Kebersihan Umum Bangunan
+Aktivitas Kehumasan
+Aktivitas Keinsinyuran Dan Konsultasi Teknis Ybdi
+Aktivitas Kesehatan Hewan
+Aktivitas Konsultan Hukum
+Aktivitas Konsultan Kekayaan Intelektual
+Aktivitas Konsultansi Manajemen Industri
+Aktivitas Konsultansi Pariwisata
+Aktivitas Konsultansi Transportasi
+Aktivitas Konsultasi Bisnis Dan Broker Bisnis
+Aktivitas Konsultasi Manajemen Lainnya
+Aktivitas Konsultasi Pajak
+Aktivitas Lainnya Yang Berkaitan Dengan Olahraga
+Aktivitas Notaris Dan Pejabat Pembuat Akta Tanah
+Aktivitas Olahraga Tradisional
+Aktivitas Organisasi Ilmu Pengetahuan Sosial Dan Masyarakat
+Aktivitas Penempatan Pekerja Rumah Tangga
+Aktivitas Penempatan Tenaga Kerja Daring
+Aktivitas Penerjemah Atau Interpreter
+Aktivitas Pengacara
+Aktivitas Pengujian Dan Atau Kalibrasi Alat Kesehatan Dan Inspeksi Sarana Prasarana Kesehatan
+Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Penyedia Gabungan Jasa Administrasi Kantor
+Aktivitas Penyedia Gabungan Jasa Penunjang Fasilitas
+Aktivitas Penyediaan Tenaga Kerja Waktu Tertentu
+Aktivitas Penyeleksian Dan Penempatan Tenaga Kerja Dalam Negeri
+Aktivitas Penyeleksian Dan Penempatan Tenaga Kerja Luar Negeri
+Aktivitas Penyelidikan
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Alat Alat Bantu Teknologi Digital
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Alat Kebutuhan MICE
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Alat Perekaman Gambar &amp; Editing
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Dan Peralatan Industri Kreatif Lainnya
+Aktivitas Penyewaan Dan Sewa Guna Tanpa Hak Opsi Mesin Pertambangan Dan Energi Serta Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Musik
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Pesta
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Rekreasi Dan Olahraga
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Air
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Darat Bukan Kendaraan Bermotor Roda Empat Atau Lebih
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Lainnya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Alat Transportasi Udara
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Barang Hasil Pencetakan Dan Penerbitan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Barang Keperluan Rumah Tangga Dan Pribadi
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Barang Keperluan Rumah Tangga Dan Pribadi Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Bunga Dan Tanaman Hias
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Industri Pengolahan
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Dan Peralatan Konstruksi Dan Teknik Sipil
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Kantor Dan Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin Pertanian Dan Peralatannya
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mesin, Peralatan Dan Barang Berwujud Lainnya YTDL
+Aktivitas Penyewaan Dan Sewa Guna Usaha Tanpa Hak Opsi Mobil, Bus, Truk Dan Sejenisnya
+Aktivitas Penyewaan Kaset Video, Cd, Vcd/Dvd Dan Sejenisnya
+Aktivitas Perawatan Dan Pemeliharaan Taman
+Aktivitas Profesional, Ilmiah Dan Teknis Lainnya YTDL
+Aktivitas Puskesmas
+Aktivitas Sertifikasi Personel Independen
+Aktivitas Sertifikasi Profesi Pihak 1
+Aktivitas Sertifikasi Profesi Pihak 2
+Aktivitas Sertifikasi Profesi Pihak 3
+Analisis Dan Uji Teknis Lainnya
+Angkutan Bus Khusus
+Apartemen Hotel
+Badan Regulasi Dan Liga Olahraga
+Bank Pembiayaan Rakyat Syariah
+Bank Perkreditan Rakyat
+Bank Sentral
+Bank Umum Konvensional
+Bank Umum Syariah
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Fasilitas Gelanggang/Arena
+Fasilitas Lapangan
+Fasilitas Olahraga Beladiri
+Fasilitas Pusat Kebugaran/ Fitness Center
+Fasilitas Umum dan Fasilitas Sosial Pemerintahan
+Hotel Bintang
+Hotel Melati
+Industri Minyak Mentah Inti Kelapa Sawit
+Industri Minyak Mentah Kelapa
+Industri Minyak Mentah Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Kelapa Sawit
+Industri Pemurnian Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Jajak Pendapat Masyarakat
+Jasa Commissioning Proses Industrial, Quality Assurance (Qa), Dan Quality Control
+Jasa Informasi Daya Tarik Wisata
+Jasa Informasi Pariwisata
+Jasa Inspeksi Periodik
+Jasa Inspeksi Teknik Instalasi
+Jasa Interpreter Wisata
+Jasa Kalibrasi/Metrologi
+Jasa Klasifikasi Kapal
+Jasa Pendidikan Komputer (Teknologi Informasi Dan Komunikasi) Swasta
+Jasa Pendidikan Manajemen Dan Perbankan
+Jasa Pendidikan Olahraga Dan Rekreasi
+Jasa Pramuwisata
+Jasa Reservasi Lainnya YBDI YTDL
+Jasa Sertifikasi
+Kegiatan Penunjang Pendidikan
+Klub Bela Diri
+Klub Bowling
+Klub Golf
+Klub Kebugaran/Fitness Dan Binaraga
+Klub Olahraga Lainnya
+Klub Renang
+Klub Sepak Bola
+Klub Tenis Lapangan
+Klub Tinju
+Konstruksi Gedung Hunian
+Konstruksi Gedung Perbelanjaan
+Konstruksi Gedung Perkantoran
+Koperasi Simpan Pinjam Primer
+Koperasi Simpan Pinjam Sekunder
+Koperasi Simpan Pinjam dan Pembiayaan Syariah Primer
+Koperasi Simpan Pinjam dan Pembiayaan Syariah Sekunder
+Lembaga Keuangan Mikro Konvensional
+Lembaga Keuangan Mikro Syariah
+Pelatihan Kerja Bisnis Dan Manajemen Pemerintah
+Pelatihan Kerja Bisnis Dan Manajemen Perusahaan
+Pelatihan Kerja Bisnis Dan Manajemen Swasta
+Pelatihan Kerja Industri Kreatif Pemerintah
+Pelatihan Kerja Industri Kreatif Perusahaan
+Pelatihan Kerja Industri Kreatif Swasta
+Pelatihan Kerja Pariwisata Dan Perhotelan Pemerintah
+Pelatihan Kerja Pariwisata Dan Perhotelan Perusahaan
+Pelatihan Kerja Pariwisata Dan Perhotelan Swasta
+Pelatihan Kerja Pekerjaan Domestik Pemerintah
+Pelatihan Kerja Pekerjaan Domestik Perusahaan
+Pelatihan Kerja Pekerjaan Domestik Swasta
+Pelatihan Kerja Pemerintah Lainnya
+Pelatihan Kerja Pertanian Dan Perikanan Pemerintah
+Pelatihan Kerja Pertanian Dan Perikanan Perusahaan
+Pelatihan Kerja Pertanian Dan Perikanan Swasta
+Pelatihan Kerja Perusahaan Lainnya
+Pelatihan Kerja Swasta Lainnya
+Pelatihan Kerja Teknik Pemerintah
+Pelatihan Kerja Teknik Perusahaan
+Pelatihan Kerja Teknik Swasta
+Pelatihan Kerja Teknologi Informasi Dan Komunikasi Pemerintah
+Pelatihan Kerja Teknologi Informasi Dan Komunikasi Perusahaan
+Pelatihan Kerja Teknologi Informasi Dan Komunikasi Swasta
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Pembibitan dan Budidaya Burung Walet
+Pendidikan Awak Pesawat Dan Jasa Angkutan Udara Khusus
+Pendidikan Bahasa Swasta
+Pendidikan Bimbingan Belajar Dan Konseling Swasta
+Pendidikan Keagamaan Islam Non Formal
+Pendidikan Keagamaan Lainnya YTDL
+Pendidikan Kebudayaan
+Pendidikan Kerajinan Dan Industri
+Pendidikan Kesehatan Swasta
+Pendidikan Lainnya Pemerintah
+Pendidikan Lainnya Swasta
+Pendidikan Pesantren Lainnya
+Pendidikan Pesantren Tinggi
+Pendidikan Teknik Swasta
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Sejarah/Cagar Budaya
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian Pasar
+Penelitian dan Pengembangan Seni
+Pengelolaan Fasilitas Olah Raga Lainnya
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Penginapan Remaja
+Pengusahaaan Tenaga Panas Bumi
+Penyediaan Sumber Daya Manusia Dan Manajemen Fungsi Sumber Daya Manusia
+Perdagangan Besar Buah Yang Mengandung Minyak
+Periklanan
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Pondok Wisata
+Rumah Tinggal
+Satuan Pendidikan Kerjasama Pendidikan Nonformal
+Sewa Guna Usaha Tanpa Hak Opsi Intelektual Properti, Bukan Karya Hak Cipta
+Tempat Peribadatan
+Unit Simpan Pinjam Koperasi Primer
+Unit Simpan Pinjam Koperasi Sekunder
+Unit Simpan Pinjam dan Pembiayaan Syariah Koperasi Primer
+Unit Simpan Pinjam dan Pembiayaan Syariah Koperasi Sekunder
+Unit Usaha Syariah Bank Umum
+Villa</v>
       </c>
       <c r="AB12" t="str">
         <v/>
@@ -3901,8 +4364,362 @@
       <c r="Z13" t="str">
         <v/>
       </c>
-      <c r="AA13" t="str">
-        <v/>
+      <c r="AA13" t="str" xml:space="preserve">
+        <v xml:space="preserve">Agen Penjual Efek Reksa Dana
+Agen Perantara Pedagang Efek
+Ahli Syariah Pasar Modal
+Aktivitas Agen Asuransi
+Aktivitas Agen Penjamin
+Aktivitas Akuntansi, Pembukuan Dan Pemeriksa
+Aktivitas Arsitektur
+Aktivitas Broker Penjaminan
+Aktivitas Broker Penjaminan Ulang
+Aktivitas Hiburan dan Rekreasi Lainnya YTDL
+Aktivitas Hukum Lainnya
+Aktivitas Jasa Keuangan Lainnya YDTL, Bukan Asuransi dan Dana Pensiun
+Aktivitas Kantor Pusat
+Aktivitas Kehumasan
+Aktivitas Keinsinyuran Dan Konsultasi Teknis Ybdi
+Aktivitas Konsultan Aktuaria
+Aktivitas Konsultan Hukum
+Aktivitas Konsultan Kekayaan Intelektual
+Aktivitas Konsultansi Manajemen Industri
+Aktivitas Konsultansi Pariwisata
+Aktivitas Konsultansi Transportasi
+Aktivitas Konsultasi Manajemen Lainnya
+Aktivitas Konsultasi Pajak
+Aktivitas Lainnya Yang Berkaitan Dengan Olahraga
+Aktivitas Manajemen Dana Lainnya
+Aktivitas Notaris Dan Pejabat Pembuat Akta Tanah
+Aktivitas Olahraga Tradisional
+Aktivitas Pelayanan Kepelabuhanan Laut
+Aktivitas Pelayanan Kesehatan Tradisional
+Aktivitas Pelayanan Kesehatan yang Dilakukan Oleh Tenaga Kesehatan Selain Dokter dan Dokter Gigi
+Aktivitas Pelayanan Penunjang Kesehatan
+Aktivitas Pemeringkat Usaha Mikro, Kecil, Menengah dan Koperasi
+Aktivitas Pengacara
+Aktivitas Penilai Kerugian Asuransi
+Aktivitas Penilaian Risiko Asuransi
+Aktivitas Penunjang Asuransi, dan Dana Pensiun Lainnya
+Aktivitas Penunjang Jasa Keuangan Lainnya YTDL
+Aktivitas Penunjang Perdagangan Berjangka Komoditi Lainnya
+Aktivitas Perancangan Khusus
+Aktivitas Perusahaan Holding
+Aktivitas Pialang Asuransi
+Aktivitas Pialang Reasuransi
+Aktivitas Praktik Dokter
+Aktivitas Praktik Dokter Gigi
+Aktivitas Praktik Dokter Spesialis
+Angkutan Udara Untuk Wisata
+Asuransi Jiwa Konvensional
+Asuransi Jiwa Syariah
+Asuransi Umum Konvensional
+Asuransi Umum Syariah
+Bank Pembiayaan Rakyat Syariah
+Bank Perkreditan Rakyat
+Bank Sentral
+Bank Umum Konvensional
+Bank Umum Syariah
+Biro Administrasi Efek
+Budidaya Biota Air Laut Lainnya
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Tawar
+Bursa Berjangka
+Bursa Berjangka Penyelenggara Pasar Fisik
+Bursa Efek
+Central Counterparty Transaksi Derivatif Suku Bunga dan Nilai Tukar
+Dana Pensiun Lembaga Keuangan Konvensional
+Dana Pensiun Lembaga Keuangan Syariah
+Dana Pensiun Pemberi Kerja Konvensional
+Dana Pensiun Pemberi Kerja Syariah
+Diskotek
+Fasilitas Gelanggang/Arena
+Fasilitas Lapangan
+Fasilitas Olahraga Beladiri
+Fasilitas Pusat Kebugaran/ Fitness Center
+Fasilitas Stadion
+Gerai Penjualan Efek Reksa Dana
+Industri Air Kemasan
+Industri Air Minum Isi Ulang
+Industri Berbagai Macam Pati Palma
+Industri Berbasis Daging Lumatan Surimi
+Industri Berbasis Lumatan Biota Air Lainnya
+Industri Bumbu Masak dan Penyedap Masakan
+Industri Dodol
+Industri Glukosa dan Sejenisnya
+Industri Gula Merah
+Industri Gula Pasir
+Industri Kakao
+Industri Kecap
+Industri Kembang Gula
+Industri Kembang Gula Lainnya
+Industri Kerupuk, Keripik, Peyek dan Sejenisnya
+Industri Krimer Nabati
+Industri Kue Basah
+Industri Makanan Bayi
+Industri Makanan Dari Cokelat dan Kembang Gula dari Coklat
+Industri Makanan Dari Kedelai dan Kacang-Kacangan Lainnya Bukan Kecap, Tempe dan Tahu
+Industri Makanan Sereal
+Industri Makanan dan Masakan Olahan
+Industri Makaroni, Mie dan Produk Sejenisnya
+Industri Manisan Buah-Buahan dan Sayuran Kering
+Industri Minuman Lainnya
+Industri Minuman Ringan
+Industri Minyak Dari Jagung dan Beras
+Industri Pati Beras dan Jagung
+Industri Pati Ubi Kayu
+Industri Pati dan Produk Pati Lainnya
+Industri Pelumatan Buah-buahan dan Sayuran
+Industri Pemanis Dari Beras dan Jagung
+Industri Pembekuan Biota Air Lainnya
+Industri Pembekuan Buah-Buahan dan Sayuran
+Industri Pembekuan Ikan
+Industri Pemindangan Biota Air Lainnya
+Industri Pemindangan Ikan
+Industri Pendinginan/Pengesan Biota Air Lainnya
+Industri Pendinginan/Pengesan Ikan
+Industri Pengasapan/Pemanggangan Biota Air Lainnya
+Industri Pengasapan/Pemanggangan Ikan
+Industri Pengasinan Buah-Buahan dan Sayuran
+Industri Pengeringan Buah-Buahan dan Sayuran
+Industri Penggaraman/Pengeringan Biota Air Lainnya
+Industri Penggaraman/Pengeringan Ikan
+Industri Penggilingan Aneka Kacang
+Industri Penggilingan Aneka Umbi dan Sayuran
+Industri Penggilingan Gandum dan Serelia Lainnya
+Industri Penggilingan Padi dan Penyosohan Beras
+Industri Penggilingan dan Pembersihan Jagung
+Industri Pengolahan Es Krim
+Industri Pengolahan Es Sejenisnya Yang Dapat Dimakan
+Industri Pengolahan Garam
+Industri Pengolahan Gula Lainnya Bukan Sirop
+Industri Pengolahan Herbal
+Industri Pengolahan Kopi
+Industri Pengolahan Produk Dari Susu Lainnya
+Industri Pengolahan Rumput Laut
+Industri Pengolahan Sari Buah dan Sayuran
+Industri Pengolahan Susu Bubuk dan Susu Kental
+Industri Pengolahan Susu Segar dan Krim
+Industri Pengolahan Tea
+Industri Pengolahan dan Pengawetan Buah-Buahan dan Sayuran Dalam Kaleng
+Industri Pengolahan dan Pengawetan Ikan dan Biota Air (Bukan Udang) Dalam Kaleng
+Industri Pengolahan dan Pengawetan Kedelai dan Kacang-Kacangan Lainnya Selain Tahu dan Tempe
+Industri Pengolahan dan Pengawetan Lainnya Buah-Buahan dan Sayuran Bukan Kacang-Kacangan
+Industri Pengolahan dan Pengawetan Lainnya Untuk Biota Air Lainnya
+Industri Pengolahan dan Pengawetan Lainnya Untuk Ikan
+Industri Pengolahan dan Pengawetan Produk Daging dan Daging Unggas
+Industri Pengolahan dan Pengawetan Udang Dalam Kaleng
+Industri Peragian/Fermentasi Biota Air Lainnya
+Industri Peragian/Fermentasi Ikan
+Industri Produk Makanan Lainnya
+Industri Produk Masak Lainnya
+Industri Produk Masak dari Kelapa
+Industri Produk Roti dan Kue
+Industri Sirop
+Industri Tahu Kedelai
+Industri Tempe Kedelai
+Industri Tepung Beras dan Tepung Jagung
+Industri Tepung Campuran dan Adonan Tepung
+Industri Tepung Terigu
+Jasa Pasca Panen Budidaya Ikan Air Payau
+Jasa Pasca Panen Budidaya Ikan Air Tawar
+Jasa Pasca Panen Budidaya Ikan Laut
+Jasa Pendidikan Komputer (Teknologi Informasi Dan Komunikasi) Swasta
+Jasa Pendidikan Manajemen Dan Perbankan
+Jasa Pendidikan Olahraga Dan Rekreasi
+Jasa Produksi Budidaya Ikan Air Payau
+Jasa Produksi Budidaya Ikan Air Tawar
+Jasa Produksi Budidaya Ikan Laut
+Jasa Sarana Produksi Budidaya Ikan Air Payau
+Jasa Sarana Produksi Budidaya Ikan Air Tawar
+Jasa Sarana Produksi Budidaya Ikan Laut
+Kegiatan Penukaran Valuta Asing
+Kegiatan Penunjang Pendidikan
+Kegiatan Rumah Potong dan Pengepakan Daging Bukan Unggas
+Kegiatan Rumah Potong dan Pengepakan Daging Unggas
+Klub Bela Diri
+Klub Bowling
+Klub Golf
+Klub Kebugaran/Fitness Dan Binaraga
+Klub Malam
+Klub Olahraga Lainnya
+Klub Renang
+Klub Sepak Bola
+Klub Tenis Lapangan
+Klub Tinju
+Konstruksi Gedung Hunian
+Konstruksi Gedung Industri
+Konstruksi Gedung Perkantoran
+Koperasi Simpan Pinjam Primer
+Koperasi Simpan Pinjam Sekunder
+Koperasi Simpan Pinjam dan Pembiayaan Syariah Primer
+Koperasi Simpan Pinjam dan Pembiayaan Syariah Sekunder
+Kustodian
+Layanan Pinjam Meminjam Uang Berbasis Teknologi Informasi (Fintech P2P Lending) Konvensional
+Layanan Pinjam Meminjam Uang Berbasis Teknologi Informasi (Fintech P2P Lending) Syariah
+Lembaga Keuangan Mikro Konvensional
+Lembaga Keuangan Mikro Syariah
+Lembaga Kliring dan Penjaminan Berjangka
+Lembaga Kliring dan Penjaminan Berjangka Penyelenggara Pasar Fisik
+Lembaga Kliring dan Penjaminan Efek
+Lembaga Pendanaan Efek
+Lembaga Penilaian Harga Efek
+Lembaga Penjamin Simpanan
+Lembaga Penyimpanan dan Penyelesaian
+Lembagan Pembiayaan Ekspor Indonesia
+Manajer Investasi
+Manajer Investasi Syariah
+Olahragawan, Juri Dan Wasit Profesional
+Otoritas Jasa Keuangan
+Pedagang Berjangka
+Pedagang Fisik Komoditi
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembesaran Crustacea Air Payau
+Pembesaran Crustacea Laut
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Sawah
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Mollusca Laut
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Tumbuhan Air Laut
+Pembesaran Tumbuhan Air Payau
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Pembibitan dan Budidaya Burung Walet
+Pembibitan dan Budidaya Lebah
+Penasihat Berjangka
+Penasihat Investasi Berbentuk Perusahaan
+Penasihat Investasi Perorangan
+Pendidikan Anak Usia Dini Sejenis Lainnya
+Pendidikan Awak Pesawat Dan Jasa Angkutan Udara Khusus
+Pendidikan Bahasa Swasta
+Pendidikan Bimbingan Belajar Dan Konseling Swasta
+Pendidikan Dasar/Ibtidaiyah Pemerintah
+Pendidikan Dasar/Ibtidaiyah Swasta
+Pendidikan Keagamaan Islam Non Formal
+Pendidikan Keagamaan Lainnya YTDL
+Pendidikan Kebudayaan
+Pendidikan Kelompok Bermain
+Pendidikan Kerajinan Dan Industri
+Pendidikan Kesehatan Swasta
+Pendidikan Lainnya Pemerintah
+Pendidikan Lainnya Swasta
+Pendidikan Menengah Atas/Aliyah Pemerintah
+Pendidikan Menengah Kejuruan Dan Teknis/Aliyah Kejuruan Pemerintah
+Pendidikan Menengah Kejuruan/Aliyah Kejuruan Swasta
+Pendidikan Menengah Pertama/Tsanawiyah Pemerintah
+Pendidikan Menengah Pertama/Tsanawiyah Swasta
+Pendidikan Menengah/Aliyah Swasta
+Pendidikan Pesantren Lainnya
+Pendidikan Taman Kanak-Kanak Luar Biasa
+Pendidikan Taman Kanak-Kanak Pemerintah
+Pendidikan Taman Kanak-Kanak Swasta/Raudatul Athfal/Bustanul Athfal
+Pendidikan Taman Penitipan Anak
+Pendidikan Teknik Swasta
+Penelitian Dan Pengembangan Agama
+Penelitian Dan Pengembangan Bioteknologi
+Penelitian Dan Pengembangan Ilmu Kedokteran
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam
+Penelitian Dan Pengembangan Ilmu Pengetahuan Alam Dan Teknologi Rekayasa Lainnya
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial
+Penelitian Dan Pengembangan Ilmu Pengetahuan Sosial Dan Humaniora Lainnya
+Penelitian Dan Pengembangan Ilmu Perikanan Dan Kelautan
+Penelitian Dan Pengembangan Ilmu Pertanian, Peternakan, Dan Kehutanan
+Penelitian Dan Pengembangan Linguistik Dan Sastra
+Penelitian Dan Pengembangan Psikologi
+Penelitian Dan Pengembangan Teknologi Dan Rekayasa
+Penelitian dan Pengembangan Seni
+Pengelola Sentra Dana Berjangka
+Pengelola Tempat Penyimpanan Fisik Komoditi
+Pengelolaan Fasilitas Olah Raga Lainnya
+Pengusahaan Kokon/Kepompong Ulat Sutra
+Penjamin Emisi efek
+Penyedia Jasa Pembayaran
+Penyediaan Jasa Boga Periode Tertentu
+Penyelenggara Dana Perlindungan Pemodal
+Penyelenggara Infrastruktur Perdagangan Di Pasar Modal Lainnya
+Penyelenggara Infrastruktur Sistem Pembayaran
+Penyelenggara Kegiatan Jasa Pengolahan Uang Rupiah
+Penyelenggara Pasar Alternatif
+Penyelenggara Penawaran Efek Melalui Layanan Urun Dana Berbasis Teknologi Informasi
+Penyelenggara Penunjang Sistem Pembayaran
+Penyelenggara Sarana Pelaksanaan Transaksi Di Pasar Uang dan Pasar Valuta Asing
+Penyelenggara Sistem Perdagangan Alternatif
+Penyelenggaraan Infrastruktur Pasar Uang dan Pasar Valuta Asing
+Perantara Moneter Lainnya
+Perantara Pedagang Efek
+Perantara Pedagang Efek Bersifat Utang dan Suku
+Perantara Perdagangan Berjangka Komoditi Lainnya
+Perantara Perdagangan Fisik Komoditi
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) Selain di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Pergadaian Konvensional
+Pergadaian Syariah
+Periklanan
+Pertanian Holtikultura Buah
+Pertanian Holtikultura Sayuran Daun
+Pertanian Pengembangbiakan Tanaman
+Pertanian Tanaman Hias
+Perusahaan Efek Daerah
+Perusahaan Efek Selain Manajemen Investasi Lainnya
+Perusahaan Modal Ventura Konvensional
+Perusahaan Modal Ventura Syariah
+Perusahaan Pembiayaan Infrastruktur Konvensional
+Perusahaan Pembiayaan Infrastruktur Syariah
+Perusahaan Pembiayaan Konvensional
+Perusahaan Pembiayaan Sekunder Perumahan
+Perusahaan Pembiayaan Syariah
+Perusahaan Pemeringkat Efek
+Perusahaan Penjamin Konvensional
+Perusahaan Penjaminan Syariah
+Perusahaan Penjaminan Ulang Konvensional
+Perusahaan Penjaminan Ulang Syariah
+Pialang Perdagangan Berjangka
+Promotor Kegiatan Olahraga
+Real Estat Atas Dasar Balas Jasa (Fee) atau Kontrak
+Real Estat Yang Dimiliki Sendiri Atau Disewa
+Reasuransi Konvensional
+Reasuransi Syariah
+Satuan Pendidikan Anak Usia Dini/Paud Al-Quran
+Satuan Pendidikan Keagamaan Anak Usia Dini
+Satuan Pendidikan Keagamaan Dasar
+Satuan Pendidikan Keagamaan Menengah
+Satuan Pendidikan Keagamaan Menengah Pertama
+Satuan Pendidikan Kerjasama Kelompok Bermain
+Satuan Pendidikan Kerjasama Pendidikan Dasar
+Satuan Pendidikan Kerjasama Pendidikan Menengah Atas
+Satuan Pendidikan Kerjasama Pendidikan Menengah Kejuruan
+Satuan Pendidikan Kerjasama Pendidikan Menengah Pertama
+Satuan Pendidikan Kerjasama Pendidikan Nonformal
+Satuan Pendidikan Kerjasama Taman Kanak-Kanak
+Satuan Pendidikan Muadalah Wustha Dan Ulya Berkesinambungan
+Satuan Pendidikan Muadalah/ Pendidikan Diniyah Formal Ulya
+Satuan Pendidikan Muadalah/Pendidikan Diniyah Formal Ula
+Satuan Pendidikan Muadalah/Pendidikan Diniyah Formal Wustha
+Satuan Pendidikan Pesantren Pengkajian Kitab Kuning Ula
+Satuan Pendidikan Pesantren Pengkajian Kitab Kuning Ulya
+Satuan Pendidikan Pesantren Pengkajian Kitab Kuning Wustha
+Trust, Pendanaan dan Entitas Keuangan Sejenis
+Unit Simpan Pinjam Koperasi Primer
+Unit Simpan Pinjam Koperasi Sekunder
+Unit Simpan Pinjam dan Pembiayaan Syariah Koperasi Primer
+Unit Simpan Pinjam dan Pembiayaan Syariah Koperasi Sekunder
+Unit Syariah Asuransi Jiwa
+Unit Syariah Asuransi Umum
+Unit Syariah Dana Pensiun Pemberi Kerja
+Unit Syariah Perusahaan Penjaminan
+Unit Syariah Reasuransi
+Unit Usaha Syariah Bank Umum
+Unit Usaha Syariah Layanan Pinjam Meminjam Uang Berbasis Teknologi Informasi
+Unit Usaha Syariah Modal Ventura
+Unit Usaha Syariah Pegadaian
+Unit Usaha Syariah Perusahaan Pembiayaan
+Unit Usaha Syariah Perusahaan Pembiayaan Infrastruktur
+Usaha Arena Permainan
+Wali Amanat</v>
       </c>
       <c r="AB13" t="str">
         <v/>
@@ -4066,7 +4883,7 @@
         <v/>
       </c>
       <c r="AA14" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB14" t="str">
         <v/>
@@ -5032,8 +5849,389 @@
       <c r="Z15" t="str">
         <v/>
       </c>
-      <c r="AA15" t="str">
-        <v/>
+      <c r="AA15" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Panti Asuhan Pemerintah
+Aktivitas Panti Asuhan Swasta
+Aktivitas Pelabuhan Perikanan
+Aktivitas Pelayanan Kepelabuhanan Laut
+Aktivitas Pelayanan Kepelabuhanan Penyeberangan
+Aktivitas Pelayanan Kepelabuhanan Sungai dan Danau
+Aktivitas Pengelolaan Kapal
+Aktivitas Penunjang Angkutan Perairan Lainnya
+Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Perancangan Khusus
+Aktivitas Sosial Di Dalam Panti Gelandangan Dan Pengemis
+Aktivitas Sosial Di Dalam Panti Lainnya YTDL
+Aktivitas Sosial Di Dalam Panti Sosial Karya Wanita
+Aktivitas Sosial Di Dalam Panti Untuk Anak Yang Berhadapan Dengan Hukum
+Aktivitas Sosial Di Dalam Panti Untuk Bina Remaja
+Aktivitas Sosial Di Dalam Panti Untuk Korban Penyalahgunaan Narkotika, Alkohol , Psikotropika Dan Zat Adiktif
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Daksa
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Grahita
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Laras
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Netra
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Rungu Wicara
+Aktivitas Sosial Di Dalam Panti Untuk Petirahan Anak
+Aktivitas Sosial Pemerintah Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial Swasta Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Swasta Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial di Dalam Panti untuk Perawatan dan Pemulihan Kesehatan
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Barang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Barang Khusus
+Angkutan Laut Dalam Negeri Untuk Barang Umum
+Angkutan Laut Dalam Negeri Untuk Pelayaran Rakyat
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Luar Negeri Pelayaran Rakyat
+Angkutan Laut Luar Negeri Untuk Barang Khusus
+Angkutan Laut Luar Negeri Untuk Barang Umum
+Angkutan Laut Luar Negeri Untuk Wisata
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Barang
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Penyeberangan Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Dalam Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Lainnya Untuk Barang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Lainnya Untuk Penumpang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Perintis Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Perintis Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Umum Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Umum Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Umum Dalam Kabupaten/Kota Untuk Barang
+Angkutan Sungai dan Danau Liner (Trayek Tetap dan Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Tramper (Trayek Tidak Tetap dan Tidak Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Untuk Barang Berbahaya
+Angkutan Sungai dan Danau Untuk Barang Khusus
+Angkutan Sungai dan Danau Untuk Barang Umum dan/atau Hewan
+Angkutan Sungai dan Danau Untuk Wisata dan YBDI
+Bar
+Diskotek
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Iindustri Kain Tenun Ikat
+Industri Air Kemasan
+Industri Air Minum dan Air Mineral
+Industri Alas Kaki Lainnya
+Industri Alas Kaki Untuk Keperluan Sehari-hari
+Industri Alat Dapur dari Kayu, Rotan dan Bambu
+Industri Alat Musik Bukan Tradisional
+Industri Alat Musik Tradisional
+Industri Alat Olahraga
+Industri Alat Pengangkat dan Pemindah
+Industri Alat Permainan
+Industri Alat Potong dan Perkakas Tangan Pertukangan
+Industri Alat Potong dan Perkakas Tangan Untuk Pertanian
+Industri Alat Potong dan Perkakas Tangan Yang Digunakan Dalam Rumah Tangga
+Industri Alat Tulis dan Gambar Termasuk Perlengkapannya
+Industri Alat Uji Dalam Proses Industri
+Industri Alat Ukur Waktu
+Industri Alat Ukur dan Alat Uji Elektrik
+Industri Alat Ukur dan Alat Uji Elektronik
+Industri Alat Ukur dan Alat Uji Manual
+Industri Bahan Bangunan Dari Tanah Liat/Keramik Bukan Batu Bata Dan Genteng
+Industri Bangunan Prafabrikasi dari Kayu
+Industri Bantal Dan Sejenisnya
+Industri Barang Anyaman dari Rotan dan Bambu
+Industri Barang Anyaman dari Tanaman Bukan Rotan dan Bambu
+Industri Barang Bangunan dari Kayu
+Industri Barang Dari Kawat
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Hewan
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Lainnya
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Pribadi
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Teknik Industri
+Industri Barang Dari Tali
+Industri Barang Jadi Rajutan dan Sulaman
+Industri Barang Jadi Tekstil Lainnya
+Industri Barang Jadi Tekstil Sulaman
+Industri Barang Jadi Tekstil Untuk Keperluan Rumah Tangga
+Industri Barang Lainnya dari Logam Mulia
+Industri Barang Logam Lainnya YTDL
+Industri Barang Perhiasan Dari Logam Mulia Bukan Untuk Keperluan Pribadi
+Industri Barang Perhiasan Dari Logam Mulia Untuk Keperluan Pribadi
+Industri Barang Tahan Api dari Tanah Liat/Keramik Lainnya
+Industri Barang dari Kayu, Rotan, Gabus Lainnya YTDL
+Industri Barang dari Logam Mulia Untuk Keperluan Teknik dan Atau Laboratorium
+Industri Bata, Mortar, Semen, Dan Sejenisnya Yang Tahan Api
+Industri Batik
+Industri Batu Bata dari Tanah Liat/Keramik
+Industri Berbagai Macam Pati Palma
+Industri Berbasis Daging Lumatan Surimi
+Industri Berbasis Lumatan Biota Air Lainnya
+Industri Brankas, Filling Kantor dan Sejenisnya
+Industri Bulu Tiruan Rajutan
+Industri Bulu Tiruan Tenunan
+Industri Bumbu Masak dan Penyedap Masakan
+Industri Dodol
+Industri Ember, Kaleng, Drum dan Wadah Sejenis Dari Logam
+Industri Furnitur Lainnya
+Industri Furnitur dari Kayu
+Industri Furnitur dari Logam
+Industri Furnitur dari Plastik
+Industri Furnitur dari Rotan dan atau Bambu
+Industri Genteng Dari Tanah Liat/Keramik
+Industri Glukosa dan Sejenisnya
+Industri Gula Merah
+Industri Gula Pasir
+Industri Jarum Mesin Jahit, Rajut, Bordir dan Sejenisnya
+Industri Kabinet Mesin Jahit
+Industri Kaca Mata
+Industri Kain Ban
+Industri Kain Pita
+Industri Kain Rajutan
+Industri Kain Sulaman
+Industri Kain Tulle Dan Kain Jaring
+Industri Kakao
+Industri Kamera Cinematografi Proyektor dan Perlengkapannya
+Industri Kapuk
+Industri Karpet dan Permadani
+Industri Kartu Cerdas
+Industri Karung Bukan Goni
+Industri Karung Goni
+Industri Kayu Bakar dan Pelet Kayu
+Industri Kayu Laminasi
+Industri Kayu Lapis
+Industri Kayu Lapis Laminasi, Termasuk Decorative Plywood
+Industri Kecap
+Industri Kembang Gula
+Industri Kembang Gula Lainnya
+Industri Keperluan Rumah Tangga Dari Logam Bukan Peralatan Dapur dan Peralatan Meja
+Industri Kerajinan Ukiran dari Kayu Bukan Mebeller
+Industri Kerajinan YTDL
+Industri Kerupuk, Keripik, Peyek dan Sejenisnya
+Industri Komponen dan Perlengkapan Sepeda Motor Roda Dua dan Tiga
+Industri Komputer dan/atau Perakitan Komputer
+Industri Krimer Nabati
+Industri Kue Basah
+Industri Kulit Komposisi
+Industri Lampu Dari Logam
+Industri Mainan Anak-anak
+Industri Makanan Bayi
+Industri Makanan Dari Cokelat dan Kembang Gula dari Coklat
+Industri Makanan Dari Kedelai dan Kacang-Kacangan Lainnya Bukan Kecap, Tempe dan Tahu
+Industri Makanan Sereal
+Industri Makanan dan Masakan Olahan
+Industri Makaroni, Mie dan Produk Sejenisnya
+Industri Malt
+Industri Manisan Buah-Buahan dan Sayuran Kering
+Industri Media Magnetik dan Media Optik
+Industri Mesin Fotocopi
+Industri Mesin Jahit Serta Mesin Cuci dan Mesin Pengering Untuk Keperluan Niaga
+Industri Mesin Kantor dan Akuntansi Elektrik
+Industri Mesin Kantor dan Akuntansi Elektronik
+Industri Mesin Kantor dan Akuntansi Manual
+Industri Mesin Pabrik Kertas
+Industri Mesin Pengolahan Makanan, Minuman, dan Tembakau
+Industri Mesin Penyiapan dan Pembuatan Produk Kulit
+Industri Mesin Percetakan
+Industri Mesin Tekstil
+Industri Mesin dan Peralatan Kantor Lainnya
+Industri Minuman Lainnya
+Industri Minuman Ringan
+Industri Minyak Dari Jagung dan Beras
+Industri Minyak Mentah dan Lemak Nabati dan Hewani Lainnya
+Industri Mortar atau Beton Siap Pakai
+Industri Non Woven
+Industri Oven, Perapian dan Tungku Pembakar Sejenis Yang Tidak Menggunakan Arus Listrik
+Industri Oven, Perapian dan Tungku Pembakar Sejenis yang Menggunakan Arus Listrik
+Industri Pakaian Jadi (Konveksi) Dari Kulit
+Industri Pakaian Jadi (Konveksi) Dari Tekstil
+Industri Pakaian Jadi Sulaman/Bordir
+Industri Pakaian Jadi dan Barang Dari Kulit Berbulu
+Industri Pakaian Rajutan
+Industri Paku, Mur dan Baut
+Industri Panel Kayu Lainnya
+Industri Partikel Kayu dan Sejenisnya
+Industri Pati Beras dan Jagung
+Industri Pati Ubi Kayu
+Industri Pati dan Produk Pati Lainnya
+Industri Pelumatan Buah-buahan dan Sayuran
+Industri Pemanis Dari Beras dan Jagung
+Industri Pembekuan Biota Air Lainnya
+Industri Pembekuan Buah-Buahan dan Sayuran
+Industri Pembekuan Ikan
+Industri Pembuatan Profil
+Industri Pemindangan Biota Air Lainnya
+Industri Pemindangan Ikan
+Industri Pemintalan Benang
+Industri Pemintalan Benang Jahit
+Industri Pencelupan Kulit Bulu
+Industri Pencetakan 3D Printing
+Industri Pencetakan Khusus
+Industri Pencetakan Umum
+Industri Pendinginan/Pengesan Biota Air Lainnya
+Industri Pendinginan/Pengesan Ikan
+Industri Pengasapan/Pemanggangan Biota Air Lainnya
+Industri Pengasapan/Pemanggangan Ikan
+Industri Pengasinan Buah-Buahan dan Sayuran
+Industri Pengawetan Kayu
+Industri Pengawetan Kotak, Bambu dan Sejenisnya
+Industri Pengawetan Kulit
+Industri Pengeringan Buah-Buahan dan Sayuran
+Industri Penggaraman/Pengeringan Biota Air Lainnya
+Industri Penggaraman/Pengeringan Ikan
+Industri Penggergajian Kayu
+Industri Penggilingan Aneka Kacang
+Industri Penggilingan Aneka Umbi dan Sayuran
+Industri Penggilingan Gandum dan Serelia Lainnya
+Industri Penggilingan Padi dan Penyosohan Beras
+Industri Penggilingan dan Pembersihan Jagung
+Industri Pengolahan Es Krim
+Industri Pengolahan Es Sejenisnya Yang Dapat Dimakan
+Industri Pengolahan Garam
+Industri Pengolahan Gula Lainnya Bukan Sirop
+Industri Pengolahan Herbal
+Industri Pengolahan Kopi
+Industri Pengolahan Produk Dari Susu Lainnya
+Industri Pengolahan Rotan
+Industri Pengolahan Rumput Laut
+Industri Pengolahan Sari Buah dan Sayuran
+Industri Pengolahan Susu Bubuk dan Susu Kental
+Industri Pengolahan Susu Segar dan Krim
+Industri Pengolahan Tea
+Industri Pengolahan dan Pengawetan Buah-Buahan dan Sayuran Dalam Kaleng
+Industri Pengolahan dan Pengawetan Ikan dan Biota Air (Bukan Udang) Dalam Kaleng
+Industri Pengolahan dan Pengawetan Kedelai dan Kacang-Kacangan Lainnya Selain Tahu dan Tempe
+Industri Pengolahan dan Pengawetan Lainnya Buah-Buahan dan Sayuran Bukan Kacang-Kacangan
+Industri Pengolahan dan Pengawetan Lainnya Untuk Biota Air Lainnya
+Industri Pengolahan dan Pengawetan Lainnya Untuk Ikan
+Industri Pengolahan dan Pengawetan Produk Daging dan Daging Unggas
+Industri Pengolahan dan Pengawetan Udang Dalam Kaleng
+Industri Penyamakan Kulit
+Industri Penyempurnaan Benang
+Industri Penyempurnaan Kain
+Industri Peragian/Fermentasi Biota Air Lainnya
+Industri Peragian/Fermentasi Ikan
+Industri Peralatan Audio dan Video Elektronik Lainnya
+Industri Peralatan Dapur dan Peralatan Meja Dari Logam
+Industri Peralatan Fotografi
+Industri Peralatan Kedokteran dan Kedokteran Gigi Serta Perlengkapan Lainnya
+Industri Peralatan Komunikasi Lainnya
+Industri Peralatan Komunikasi Tanpa Kabel
+Industri Peralatan Saniter Dari Porselen
+Industri Peralatan Telepon dan Faksimili
+Industri Peralatan Terekam, Penerima dan Pengganda Audio dan Video, Bukan Industri Televisi
+Industri Peralatan Umum
+Industri Peralatan Untuk Pelindung Keselamatan
+Industri Percetakan Kain
+Industri Perhiasan Imitasi dan Barang Sejenis
+Industri Perhiasan Mutiara
+Industri Perlengkapan Komputer
+Industri Perlengkapan Pakaian Dari Kulit
+Industri Perlengkapan Pakaian Dari Tekstil
+Industri Perlengkapan Rumah Tangga Dari Porselen
+Industri Perlengkapan Rumah Tangga Dari Tanah Liat/Keramik
+Industri Perlengkapan Sepeda dan Kursi Roda Termasuk Becak
+Industri Permata
+Industri Persiapan Serat Tekstil
+Industri Pertenunan
+Industri Pita Mesin Tulis/Gambar
+Industri Produk Makanan Lainnya
+Industri Produk Masak Lainnya
+Industri Produk Masak dari Kelapa
+Industri Produk Roti dan Kue
+Industri Rajutan Kaos Kaki dan Sejenisnya
+Industri Semi Konduktor Dan Komponen Elektronik Lainnya
+Industri Sepatu Olahraga
+Industri Sepatu Teknik Lapangan/Keperluan Industri
+Industri Sepeda dan Kursi Roda Termasuk Becak
+Industri Serat Sabut Kelapa
+Industri Sirop
+Industri Tabung Elektron dan Konektor Elektronik
+Industri Tahu Kedelai
+Industri Tali
+Industri Tekstil Lainnya YTDL
+Industri Televisi dan/atau Perakitan Televisi
+Industri Tempe Kedelai
+Industri Tepung Beras dan Tepung Jagung
+Industri Tepung Campuran dan Adonan Tepung
+Industri Tepung Terigu
+Industri Teropong dan Instrumen Optik Bukan Kacamata
+Industri Veneer
+Industri Wadah dari Kayu
+Industri Yang Menghasilkan Kain Keperluan Industri
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Jasa Industri Untuk Berbagai Pengerjaan Khusus Logam dan Barang dari Logam
+Jasa Pengurusan Transportasi
+Karaoke
+Kegiatan Jasa Penunjang Pencetakkan
+Klub Malam
+Konstruksi Bangunan Pelabuhan Bukan Perikanan
+Konstruksi Bangunan Pelabuhan Perikanan
+Konstruksi Bangunan Sipil Fasilitas Olahraga
+Konstruksi Gedung Industri
+Konstruksi Gedung Kesehatan
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Penjahitan dan Pembuatan Pakaian Sesuai Pesanan
+Perdagangan Besar Bahan Bakar Padat, Cair dan Gas dan Produk YBDI
+Perdagangan Besar Barang Bekas dan Sisa-sisa Tak Terpakai
+Perdagangan Besar Logam dan Bijih Logam
+Pergudangan dan Penyimpanan
+Periklanan
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Produksi Es
+Real Estat Yang Dimiliki Sendiri Atau Disewa
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Lainnya
+Reparasi Peralatan Listrik Lainnya
+Reparasi Produk Logam Pabrikasi Lainnya
+Reparasi Produk Logam Siap Pasang Untuk Bangunan, Tangki, Tandon Air dan Generator Uap
+Reproduksi Media Rekaman Film dan Video
+Reproduksi Media Rekaman Suara dan Piranti Lunak
+Tempat Peribadatan
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Pendidikan
+Yayasan Sosial</v>
       </c>
       <c r="AB15" t="str">
         <v/>
@@ -5240,7 +6438,7 @@
         <v/>
       </c>
       <c r="AA16" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB16" t="str">
         <v/>
@@ -5382,7 +6580,7 @@
         <v/>
       </c>
       <c r="AA17" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB17" t="str">
         <v/>
@@ -6348,8 +7546,389 @@
       <c r="Z18" t="str">
         <v/>
       </c>
-      <c r="AA18" t="str">
-        <v/>
+      <c r="AA18" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Panti Asuhan Pemerintah
+Aktivitas Panti Asuhan Swasta
+Aktivitas Pelabuhan Perikanan
+Aktivitas Pelayanan Kepelabuhanan Laut
+Aktivitas Pelayanan Kepelabuhanan Penyeberangan
+Aktivitas Pelayanan Kepelabuhanan Sungai dan Danau
+Aktivitas Pengelolaan Kapal
+Aktivitas Penunjang Angkutan Perairan Lainnya
+Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Perancangan Khusus
+Aktivitas Sosial Di Dalam Panti Gelandangan Dan Pengemis
+Aktivitas Sosial Di Dalam Panti Lainnya YTDL
+Aktivitas Sosial Di Dalam Panti Sosial Karya Wanita
+Aktivitas Sosial Di Dalam Panti Untuk Anak Yang Berhadapan Dengan Hukum
+Aktivitas Sosial Di Dalam Panti Untuk Bina Remaja
+Aktivitas Sosial Di Dalam Panti Untuk Korban Penyalahgunaan Narkotika, Alkohol , Psikotropika Dan Zat Adiktif
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Daksa
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Grahita
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Laras
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Netra
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Rungu Wicara
+Aktivitas Sosial Di Dalam Panti Untuk Petirahan Anak
+Aktivitas Sosial Pemerintah Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial Swasta Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Swasta Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial di Dalam Panti untuk Perawatan dan Pemulihan Kesehatan
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Barang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Barang Khusus
+Angkutan Laut Dalam Negeri Untuk Barang Umum
+Angkutan Laut Dalam Negeri Untuk Pelayaran Rakyat
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Luar Negeri Pelayaran Rakyat
+Angkutan Laut Luar Negeri Untuk Barang Khusus
+Angkutan Laut Luar Negeri Untuk Barang Umum
+Angkutan Laut Luar Negeri Untuk Wisata
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Barang
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Penyeberangan Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Dalam Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Lainnya Untuk Barang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Lainnya Untuk Penumpang Termasuk Penyeberangan Antar Negara
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Perintis Antar Kabupaten/Kota Untuk Penumpang
+Angkutan Penyeberangan Perintis Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Perintis Antarprovinsi Untuk Penumpang
+Angkutan Penyeberangan Umum Antar Kabupaten/Kota Untuk Barang
+Angkutan Penyeberangan Umum Antar Provinsi Untuk Barang
+Angkutan Penyeberangan Umum Dalam Kabupaten/Kota Untuk Barang
+Angkutan Sungai dan Danau Liner (Trayek Tetap dan Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Tramper (Trayek Tidak Tetap dan Tidak Teratur) Untuk Penumpang
+Angkutan Sungai dan Danau Untuk Barang Berbahaya
+Angkutan Sungai dan Danau Untuk Barang Khusus
+Angkutan Sungai dan Danau Untuk Barang Umum dan/atau Hewan
+Angkutan Sungai dan Danau Untuk Wisata dan YBDI
+Bar
+Diskotek
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Iindustri Kain Tenun Ikat
+Industri Air Kemasan
+Industri Air Minum dan Air Mineral
+Industri Alas Kaki Lainnya
+Industri Alas Kaki Untuk Keperluan Sehari-hari
+Industri Alat Dapur dari Kayu, Rotan dan Bambu
+Industri Alat Musik Bukan Tradisional
+Industri Alat Musik Tradisional
+Industri Alat Olahraga
+Industri Alat Pengangkat dan Pemindah
+Industri Alat Permainan
+Industri Alat Potong dan Perkakas Tangan Pertukangan
+Industri Alat Potong dan Perkakas Tangan Untuk Pertanian
+Industri Alat Potong dan Perkakas Tangan Yang Digunakan Dalam Rumah Tangga
+Industri Alat Tulis dan Gambar Termasuk Perlengkapannya
+Industri Alat Uji Dalam Proses Industri
+Industri Alat Ukur Waktu
+Industri Alat Ukur dan Alat Uji Elektrik
+Industri Alat Ukur dan Alat Uji Elektronik
+Industri Alat Ukur dan Alat Uji Manual
+Industri Bahan Bangunan Dari Tanah Liat/Keramik Bukan Batu Bata Dan Genteng
+Industri Bangunan Prafabrikasi dari Kayu
+Industri Bantal Dan Sejenisnya
+Industri Barang Anyaman dari Rotan dan Bambu
+Industri Barang Anyaman dari Tanaman Bukan Rotan dan Bambu
+Industri Barang Bangunan dari Kayu
+Industri Barang Dari Kawat
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Hewan
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Lainnya
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Pribadi
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Teknik Industri
+Industri Barang Dari Tali
+Industri Barang Jadi Rajutan dan Sulaman
+Industri Barang Jadi Tekstil Lainnya
+Industri Barang Jadi Tekstil Sulaman
+Industri Barang Jadi Tekstil Untuk Keperluan Rumah Tangga
+Industri Barang Lainnya dari Logam Mulia
+Industri Barang Logam Lainnya YTDL
+Industri Barang Perhiasan Dari Logam Mulia Bukan Untuk Keperluan Pribadi
+Industri Barang Perhiasan Dari Logam Mulia Untuk Keperluan Pribadi
+Industri Barang Tahan Api dari Tanah Liat/Keramik Lainnya
+Industri Barang dari Kayu, Rotan, Gabus Lainnya YTDL
+Industri Barang dari Logam Mulia Untuk Keperluan Teknik dan Atau Laboratorium
+Industri Bata, Mortar, Semen, Dan Sejenisnya Yang Tahan Api
+Industri Batik
+Industri Batu Bata dari Tanah Liat/Keramik
+Industri Berbagai Macam Pati Palma
+Industri Berbasis Daging Lumatan Surimi
+Industri Berbasis Lumatan Biota Air Lainnya
+Industri Brankas, Filling Kantor dan Sejenisnya
+Industri Bulu Tiruan Rajutan
+Industri Bulu Tiruan Tenunan
+Industri Bumbu Masak dan Penyedap Masakan
+Industri Dodol
+Industri Ember, Kaleng, Drum dan Wadah Sejenis Dari Logam
+Industri Furnitur Lainnya
+Industri Furnitur dari Kayu
+Industri Furnitur dari Logam
+Industri Furnitur dari Plastik
+Industri Furnitur dari Rotan dan atau Bambu
+Industri Genteng Dari Tanah Liat/Keramik
+Industri Glukosa dan Sejenisnya
+Industri Gula Merah
+Industri Gula Pasir
+Industri Jarum Mesin Jahit, Rajut, Bordir dan Sejenisnya
+Industri Kabinet Mesin Jahit
+Industri Kaca Mata
+Industri Kain Ban
+Industri Kain Pita
+Industri Kain Rajutan
+Industri Kain Sulaman
+Industri Kain Tulle Dan Kain Jaring
+Industri Kakao
+Industri Kamera Cinematografi Proyektor dan Perlengkapannya
+Industri Kapuk
+Industri Karpet dan Permadani
+Industri Kartu Cerdas
+Industri Karung Bukan Goni
+Industri Karung Goni
+Industri Kayu Bakar dan Pelet Kayu
+Industri Kayu Laminasi
+Industri Kayu Lapis
+Industri Kayu Lapis Laminasi, Termasuk Decorative Plywood
+Industri Kecap
+Industri Kembang Gula
+Industri Kembang Gula Lainnya
+Industri Keperluan Rumah Tangga Dari Logam Bukan Peralatan Dapur dan Peralatan Meja
+Industri Kerajinan Ukiran dari Kayu Bukan Mebeller
+Industri Kerajinan YTDL
+Industri Kerupuk, Keripik, Peyek dan Sejenisnya
+Industri Komponen dan Perlengkapan Sepeda Motor Roda Dua dan Tiga
+Industri Komputer dan/atau Perakitan Komputer
+Industri Krimer Nabati
+Industri Kue Basah
+Industri Kulit Komposisi
+Industri Lampu Dari Logam
+Industri Mainan Anak-anak
+Industri Makanan Bayi
+Industri Makanan Dari Cokelat dan Kembang Gula dari Coklat
+Industri Makanan Dari Kedelai dan Kacang-Kacangan Lainnya Bukan Kecap, Tempe dan Tahu
+Industri Makanan Sereal
+Industri Makanan dan Masakan Olahan
+Industri Makaroni, Mie dan Produk Sejenisnya
+Industri Malt
+Industri Manisan Buah-Buahan dan Sayuran Kering
+Industri Media Magnetik dan Media Optik
+Industri Mesin Fotocopi
+Industri Mesin Jahit Serta Mesin Cuci dan Mesin Pengering Untuk Keperluan Niaga
+Industri Mesin Kantor dan Akuntansi Elektrik
+Industri Mesin Kantor dan Akuntansi Elektronik
+Industri Mesin Kantor dan Akuntansi Manual
+Industri Mesin Pabrik Kertas
+Industri Mesin Pengolahan Makanan, Minuman, dan Tembakau
+Industri Mesin Penyiapan dan Pembuatan Produk Kulit
+Industri Mesin Percetakan
+Industri Mesin Tekstil
+Industri Mesin dan Peralatan Kantor Lainnya
+Industri Minuman Lainnya
+Industri Minuman Ringan
+Industri Minyak Dari Jagung dan Beras
+Industri Minyak Mentah dan Lemak Nabati dan Hewani Lainnya
+Industri Mortar atau Beton Siap Pakai
+Industri Non Woven
+Industri Oven, Perapian dan Tungku Pembakar Sejenis Yang Tidak Menggunakan Arus Listrik
+Industri Oven, Perapian dan Tungku Pembakar Sejenis yang Menggunakan Arus Listrik
+Industri Pakaian Jadi (Konveksi) Dari Kulit
+Industri Pakaian Jadi (Konveksi) Dari Tekstil
+Industri Pakaian Jadi Sulaman/Bordir
+Industri Pakaian Jadi dan Barang Dari Kulit Berbulu
+Industri Pakaian Rajutan
+Industri Paku, Mur dan Baut
+Industri Panel Kayu Lainnya
+Industri Partikel Kayu dan Sejenisnya
+Industri Pati Beras dan Jagung
+Industri Pati Ubi Kayu
+Industri Pati dan Produk Pati Lainnya
+Industri Pelumatan Buah-buahan dan Sayuran
+Industri Pemanis Dari Beras dan Jagung
+Industri Pembekuan Biota Air Lainnya
+Industri Pembekuan Buah-Buahan dan Sayuran
+Industri Pembekuan Ikan
+Industri Pembuatan Profil
+Industri Pemindangan Biota Air Lainnya
+Industri Pemindangan Ikan
+Industri Pemintalan Benang
+Industri Pemintalan Benang Jahit
+Industri Pencelupan Kulit Bulu
+Industri Pencetakan 3D Printing
+Industri Pencetakan Khusus
+Industri Pencetakan Umum
+Industri Pendinginan/Pengesan Biota Air Lainnya
+Industri Pendinginan/Pengesan Ikan
+Industri Pengasapan/Pemanggangan Biota Air Lainnya
+Industri Pengasapan/Pemanggangan Ikan
+Industri Pengasinan Buah-Buahan dan Sayuran
+Industri Pengawetan Kayu
+Industri Pengawetan Kotak, Bambu dan Sejenisnya
+Industri Pengawetan Kulit
+Industri Pengeringan Buah-Buahan dan Sayuran
+Industri Penggaraman/Pengeringan Biota Air Lainnya
+Industri Penggaraman/Pengeringan Ikan
+Industri Penggergajian Kayu
+Industri Penggilingan Aneka Kacang
+Industri Penggilingan Aneka Umbi dan Sayuran
+Industri Penggilingan Gandum dan Serelia Lainnya
+Industri Penggilingan Padi dan Penyosohan Beras
+Industri Penggilingan dan Pembersihan Jagung
+Industri Pengolahan Es Krim
+Industri Pengolahan Es Sejenisnya Yang Dapat Dimakan
+Industri Pengolahan Garam
+Industri Pengolahan Gula Lainnya Bukan Sirop
+Industri Pengolahan Herbal
+Industri Pengolahan Kopi
+Industri Pengolahan Produk Dari Susu Lainnya
+Industri Pengolahan Rotan
+Industri Pengolahan Rumput Laut
+Industri Pengolahan Sari Buah dan Sayuran
+Industri Pengolahan Susu Bubuk dan Susu Kental
+Industri Pengolahan Susu Segar dan Krim
+Industri Pengolahan Tea
+Industri Pengolahan dan Pengawetan Buah-Buahan dan Sayuran Dalam Kaleng
+Industri Pengolahan dan Pengawetan Ikan dan Biota Air (Bukan Udang) Dalam Kaleng
+Industri Pengolahan dan Pengawetan Kedelai dan Kacang-Kacangan Lainnya Selain Tahu dan Tempe
+Industri Pengolahan dan Pengawetan Lainnya Buah-Buahan dan Sayuran Bukan Kacang-Kacangan
+Industri Pengolahan dan Pengawetan Lainnya Untuk Biota Air Lainnya
+Industri Pengolahan dan Pengawetan Lainnya Untuk Ikan
+Industri Pengolahan dan Pengawetan Produk Daging dan Daging Unggas
+Industri Pengolahan dan Pengawetan Udang Dalam Kaleng
+Industri Penyamakan Kulit
+Industri Penyempurnaan Benang
+Industri Penyempurnaan Kain
+Industri Peragian/Fermentasi Biota Air Lainnya
+Industri Peragian/Fermentasi Ikan
+Industri Peralatan Audio dan Video Elektronik Lainnya
+Industri Peralatan Dapur dan Peralatan Meja Dari Logam
+Industri Peralatan Fotografi
+Industri Peralatan Kedokteran dan Kedokteran Gigi Serta Perlengkapan Lainnya
+Industri Peralatan Komunikasi Lainnya
+Industri Peralatan Komunikasi Tanpa Kabel
+Industri Peralatan Saniter Dari Porselen
+Industri Peralatan Telepon dan Faksimili
+Industri Peralatan Terekam, Penerima dan Pengganda Audio dan Video, Bukan Industri Televisi
+Industri Peralatan Umum
+Industri Peralatan Untuk Pelindung Keselamatan
+Industri Percetakan Kain
+Industri Perhiasan Imitasi dan Barang Sejenis
+Industri Perhiasan Mutiara
+Industri Perlengkapan Komputer
+Industri Perlengkapan Pakaian Dari Kulit
+Industri Perlengkapan Pakaian Dari Tekstil
+Industri Perlengkapan Rumah Tangga Dari Porselen
+Industri Perlengkapan Rumah Tangga Dari Tanah Liat/Keramik
+Industri Perlengkapan Sepeda dan Kursi Roda Termasuk Becak
+Industri Permata
+Industri Persiapan Serat Tekstil
+Industri Pertenunan
+Industri Pita Mesin Tulis/Gambar
+Industri Produk Makanan Lainnya
+Industri Produk Masak Lainnya
+Industri Produk Masak dari Kelapa
+Industri Produk Roti dan Kue
+Industri Rajutan Kaos Kaki dan Sejenisnya
+Industri Semi Konduktor Dan Komponen Elektronik Lainnya
+Industri Sepatu Olahraga
+Industri Sepatu Teknik Lapangan/Keperluan Industri
+Industri Sepeda dan Kursi Roda Termasuk Becak
+Industri Serat Sabut Kelapa
+Industri Sirop
+Industri Tabung Elektron dan Konektor Elektronik
+Industri Tahu Kedelai
+Industri Tali
+Industri Tekstil Lainnya YTDL
+Industri Televisi dan/atau Perakitan Televisi
+Industri Tempe Kedelai
+Industri Tepung Beras dan Tepung Jagung
+Industri Tepung Campuran dan Adonan Tepung
+Industri Tepung Terigu
+Industri Teropong dan Instrumen Optik Bukan Kacamata
+Industri Veneer
+Industri Wadah dari Kayu
+Industri Yang Menghasilkan Kain Keperluan Industri
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Jasa Industri Untuk Berbagai Pengerjaan Khusus Logam dan Barang dari Logam
+Jasa Pengurusan Transportasi
+Karaoke
+Kegiatan Jasa Penunjang Pencetakkan
+Klub Malam
+Konstruksi Bangunan Pelabuhan Bukan Perikanan
+Konstruksi Bangunan Pelabuhan Perikanan
+Konstruksi Bangunan Sipil Fasilitas Olahraga
+Konstruksi Gedung Industri
+Konstruksi Gedung Kesehatan
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Penjahitan dan Pembuatan Pakaian Sesuai Pesanan
+Perdagangan Besar Bahan Bakar Padat, Cair dan Gas dan Produk YBDI
+Perdagangan Besar Barang Bekas dan Sisa-sisa Tak Terpakai
+Perdagangan Besar Logam dan Bijih Logam
+Pergudangan dan Penyimpanan
+Periklanan
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Produksi Es
+Real Estat Yang Dimiliki Sendiri Atau Disewa
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Lainnya
+Reparasi Peralatan Listrik Lainnya
+Reparasi Produk Logam Pabrikasi Lainnya
+Reparasi Produk Logam Siap Pasang Untuk Bangunan, Tangki, Tandon Air dan Generator Uap
+Reproduksi Media Rekaman Film dan Video
+Reproduksi Media Rekaman Suara dan Piranti Lunak
+Tempat Peribadatan
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Pendidikan
+Yayasan Sosial</v>
       </c>
       <c r="AB18" t="str">
         <v/>
@@ -6556,7 +8135,7 @@
         <v/>
       </c>
       <c r="AA19" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB19" t="str">
         <v/>
@@ -6698,7 +8277,7 @@
         <v/>
       </c>
       <c r="AA20" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="AB20" t="str">
         <v/>
@@ -7337,8 +8916,58 @@
       <c r="Z21" t="str">
         <v/>
       </c>
-      <c r="AA21" t="str">
-        <v/>
+      <c r="AA21" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Perancangan Khusus
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Industri Air Minum dan Air Mineral
+Kedai Makanan
+Kedai Minuman
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Perdagangan Eceran Khusus Peralatan Olahraga di Toko
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Pendidikan
+Yayasan Sosial</v>
       </c>
       <c r="AB21" t="str">
         <v/>
@@ -7558,8 +9187,159 @@
       <c r="Z22" t="str">
         <v/>
       </c>
-      <c r="AA22" t="str">
-        <v/>
+      <c r="AA22" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Budidaya Ayam Lokal dan Persilangannya
+Budidaya Ayam Ras Pedaging
+Budidaya Ayam Ras Petelur
+Budidaya Biota Air Laut Lainnya
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Tawar
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Fasilitas Umum dan Fasilitas Sosial Pemerintahan
+Industri Berbasis Daging Lumatan Surimi
+Industri Berbasis Lumatan Biota Air Lainnya
+Industri Karet Remah
+Industri Kimia Dasar Organik Yang Bersumber Dari Hasil Pertanian
+Industri Minyak Mentah Inti Kelapa Sawit
+Industri Minyak Mentah Kelapa
+Industri Minyak Mentah Kelapa Sawit
+Industri Pelumatan Buah-buahan dan Sayuran
+Industri Pembekuan Biota Air Lainnya
+Industri Pembekuan Buah-Buahan dan Sayuran
+Industri Pembekuan Ikan
+Industri Pemindangan Biota Air Lainnya
+Industri Pemindangan Ikan
+Industri Pemisahan/Fraksinasi Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Kelapa Sawit
+Industri Pemurnian Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pendinginan/Pengesan Biota Air Lainnya
+Industri Pendinginan/Pengesan Ikan
+Industri Pengasapan/Pemanggangan Biota Air Lainnya
+Industri Pengasapan/Pemanggangan Ikan
+Industri Pengasinan Buah-Buahan dan Sayuran
+Industri Pengeringan Buah-Buahan dan Sayuran
+Industri Penggaraman/Pengeringan Biota Air Lainnya
+Industri Penggaraman/Pengeringan Ikan
+Industri Pengolahan Rumput Laut
+Industri Pengolahan Sari Buah dan Sayuran
+Industri Pengolahan dan Pengawetan Buah-Buahan dan Sayuran Dalam Kaleng
+Industri Pengolahan dan Pengawetan Ikan dan Biota Air (Bukan Udang) Dalam Kaleng
+Industri Pengolahan dan Pengawetan Kedelai dan Kacang-Kacangan Lainnya Selain Tahu dan Tempe
+Industri Pengolahan dan Pengawetan Lainnya Buah-Buahan dan Sayuran Bukan Kacang-Kacangan
+Industri Pengolahan dan Pengawetan Lainnya Untuk Biota Air Lainnya
+Industri Pengolahan dan Pengawetan Lainnya Untuk Ikan
+Industri Pengolahan dan Pengawetan Produk Daging dan Daging Unggas
+Industri Pengolahan dan Pengawetan Udang Dalam Kaleng
+Industri Peragian/Fermentasi Biota Air Lainnya
+Industri Peragian/Fermentasi Ikan
+Industri Tahu Kedelai
+Industri Tempe Kedelai
+Jasa Pasca Panen
+Jasa Pasca Panen Budidaya Ikan Air Payau
+Jasa Pasca Panen Budidaya Ikan Air Tawar
+Jasa Pasca Panen Budidaya Ikan Laut
+Jasa Pelayanan Kesehatan Ternak
+Jasa Pemanenan
+Jasa Pemupukan, Penanaman Bibit/Benih dan Pengendalian Hama dan Gulma
+Jasa Pengetasan Telur
+Jasa Pengolahan Lahan
+Jasa Penunjang Pertanian Lainnya
+Jasa Penunjang Peternakan Lainnya
+Jasa Penyemprotan dan Penyerbukan Melalui Udara
+Jasa Perkawinan Ternak
+Jasa Produksi Budidaya Ikan Air Payau
+Jasa Produksi Budidaya Ikan Air Tawar
+Jasa Produksi Budidaya Ikan Laut
+Jasa Sarana Produksi Budidaya Ikan Air Payau
+Jasa Sarana Produksi Budidaya Ikan Air Tawar
+Jasa Sarana Produksi Budidaya Ikan Laut
+Kegiatan Rumah Potong dan Pengepakan Daging Bukan Unggas
+Kegiatan Rumah Potong dan Pengepakan Daging Unggas
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembesaran Crustacea Air Payau
+Pembesaran Crustacea Laut
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Kolam
+Pembesaran Ikan Air Tawar Di Sawah
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Tumbuhan Air Laut
+Pembesaran Tumbuhan Air Payau
+Pembibitan Ayam Lokal dan Persilangannya
+Pembibitan Ayam Ras
+Pembibitan Dan Budidaya Sapi Potong
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Pembibitan dan Budidaya Burung Merpati
+Pembibitan dan Budidaya Burung Puyuh
+Pembibitan dan Budidaya Burung Unta
+Pembibitan dan Budidaya Burung Walet
+Pembibitan dan Budidaya Cacing
+Pembibitan dan Budidaya Domba Perah
+Pembibitan dan Budidaya Domba Potong
+Pembibitan dan Budidaya Itik dan/atau Bebek
+Pembibitan dan Budidaya Kambing Perah
+Pembibitan dan Budidaya Kambing Potong
+Pembibitan dan Budidaya Kelinci
+Pembibitan dan Budidaya Kerbau Perah
+Pembibitan dan Budidaya Kerbau Potong
+Pembibitan dan Budidaya Lebah
+Pembibitan dan Budidaya Rusa
+Pembibitan dan Budidaya Sapi Perah
+Pembibitan dan Budidaya Ternak Unggas Lainnya
+Pemilihan Benih Tanaman Untuk Pengembangbiakan
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Pengusahaan Kokon/Kepompong Ulat Sutra
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Peternakan Babi
+Peternakan Kuda dan Sejenisnya
+Peternakan Unta dan Sejenisnya
+Produksi Bulu Domba Mentah/Raw Wool
+Rumah Tinggal
+Tempat Peribadatan</v>
       </c>
       <c r="AB22" t="str">
         <v/>
@@ -7833,8 +9613,9 @@
       <c r="Z23" t="str">
         <v/>
       </c>
-      <c r="AA23" t="str">
-        <v/>
+      <c r="AA23" t="str" xml:space="preserve">
+        <v xml:space="preserve">Konstruksi Bangunan Pelabuhan Bukan Perikanan
+Konstruksi Bangunan Pelabuhan Perikanan</v>
       </c>
       <c r="AB23" t="str">
         <v/>
@@ -8024,8 +9805,50 @@
       <c r="Z24" t="str">
         <v/>
       </c>
-      <c r="AA24" t="str">
-        <v/>
+      <c r="AA24" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Industri Air Minum dan Air Mineral
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium</v>
       </c>
       <c r="AB24" t="str">
         <v/>
@@ -9010,8 +10833,448 @@
       <c r="Z25" t="str">
         <v/>
       </c>
-      <c r="AA25" t="str">
-        <v/>
+      <c r="AA25" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Keamanan Swasta
+Aktivitas Panti Asuhan Pemerintah
+Aktivitas Panti Asuhan Swasta
+Aktivitas Penerbitan Lainnya
+Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Penyiaran dan Pemrograman Televisi Oleh Pemerintah
+Aktivitas Penyiaran dan Pemrograman Televisi Oleh Swasta
+Aktivitas Perancangan Khusus
+Aktivitas Sosial Di Dalam Panti Gelandangan Dan Pengemis
+Aktivitas Sosial Di Dalam Panti Lainnya YTDL
+Aktivitas Sosial Di Dalam Panti Sosial Karya Wanita
+Aktivitas Sosial Di Dalam Panti Untuk Anak Yang Berhadapan Dengan Hukum
+Aktivitas Sosial Di Dalam Panti Untuk Bina Remaja
+Aktivitas Sosial Di Dalam Panti Untuk Korban Penyalahgunaan Narkotika, Alkohol , Psikotropika Dan Zat Adiktif
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Daksa
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Grahita
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Laras
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Netra
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Rungu Wicara
+Aktivitas Sosial Di Dalam Panti Untuk Petirahan Anak
+Aktivitas Sosial Pemerintah Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial Swasta Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Swasta Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial di Dalam Panti untuk Perawatan dan Pemulihan Kesehatan
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Sewa
+Apartemen Hotel
+Badan Nasional Penanggulangan Bencana Dan Pemadam Kebakaran
+Budidaya Ayam Lokal dan Persilangannya
+Budidaya Ayam Ras Pedaging
+Budidaya Ayam Ras Petelur
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Tawar
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Hotel Bintang
+Hotel Melati
+Iindustri Kain Tenun Ikat
+Industri Air Kemasan
+Industri Air Minum Isi Ulang
+Industri Alas Kaki Lainnya
+Industri Alas Kaki Untuk Keperluan Sehari-hari
+Industri Alat Dapur dari Kayu, Rotan dan Bambu
+Industri Alat Musik Bukan Tradisional
+Industri Alat Musik Tradisional
+Industri Alat Olahraga
+Industri Alat Permainan
+Industri Bangunan Prafabrikasi dari Kayu
+Industri Bantal Dan Sejenisnya
+Industri Barang Anyaman dari Rotan dan Bambu
+Industri Barang Anyaman dari Tanaman Bukan Rotan dan Bambu
+Industri Barang Bangunan dari Kayu
+Industri Barang Dari Kertas dan Papan Kertas Lainnya YTDL
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Hewan
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Lainnya
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Pribadi
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Teknik Industri
+Industri Barang Dari Tali
+Industri Barang Jadi Rajutan dan Sulaman
+Industri Barang Jadi Tekstil Lainnya
+Industri Barang Jadi Tekstil Sulaman
+Industri Barang Jadi Tekstil Untuk Keperluan Rumah Tangga
+Industri Barang Tahan Api dari Tanah Liat/Keramik Lainnya
+Industri Barang dari Kayu, Rotan, Gabus Lainnya YTDL
+Industri Bata, Mortar, Semen, Dan Sejenisnya Yang Tahan Api
+Industri Batik
+Industri Batu Bata dari Tanah Liat/Keramik
+Industri Berbagai Macam Pati Palma
+Industri Berbasis Daging Lumatan Surimi
+Industri Berbasis Lumatan Biota Air Lainnya
+Industri Bubur Kertas
+Industri Bulu Tiruan Rajutan
+Industri Bulu Tiruan Tenunan
+Industri Bumbu Masak dan Penyedap Masakan
+Industri Bumbu Rokok Serta Kelengkapan Rokok Lainnya
+Industri Dodol
+Industri Furnitur dari Kayu
+Industri Furnitur dari Plastik
+Industri Furnitur dari Rotan dan atau Bambu
+Industri Genteng Dari Tanah Liat/Keramik
+Industri Glukosa dan Sejenisnya
+Industri Gula Merah
+Industri Gula Pasir
+Industri Kain Ban
+Industri Kain Pita
+Industri Kain Rajutan
+Industri Kain Sulaman
+Industri Kain Tulle Dan Kain Jaring
+Industri Kakao
+Industri Kapuk
+Industri Karpet dan Permadani
+Industri Karung Bukan Goni
+Industri Karung Goni
+Industri Kayu Bakar dan Pelet Kayu
+Industri Kayu Laminasi
+Industri Kayu Lapis
+Industri Kayu Lapis Laminasi, Termasuk Decorative Plywood
+Industri Kecap
+Industri Kemasan dan Kotak dari Kertas dan Karton
+Industri Kembang Gula
+Industri Kembang Gula Lainnya
+Industri Kerajinan Ukiran dari Kayu Bukan Mebeller
+Industri Kerajinan YTDL
+Industri Kertas Berharga
+Industri Kertas Budaya
+Industri Kertas Khusus
+Industri Kertas Lainnya
+Industri Kertas Tissue
+Industri Kertas dan Papan Kerta Bergelombang
+Industri Kerupuk, Keripik, Peyek dan Sejenisnya
+Industri Konsentrat Makanan Hewan
+Industri Kopra
+Industri Krimer Nabati
+Industri Kue Basah
+Industri Kulit Komposisi
+Industri Mainan Anak-anak
+Industri Makanan Bayi
+Industri Makanan Dari Cokelat dan Kembang Gula dari Coklat
+Industri Makanan Dari Kedelai dan Kacang-Kacangan Lainnya Bukan Kecap, Tempe dan Tahu
+Industri Makanan Sereal
+Industri Makanan dan Masakan Olahan
+Industri Makaroni, Mie dan Produk Sejenisnya
+Industri Malt
+Industri Manisan Buah-Buahan dan Sayuran Kering
+Industri Margarine
+Industri Minuman Beralkohol Hasil Destilasi
+Industri Minuman Beralkohol Hasil Fermentasi Anggur dan Hasil Pertanian Lainnya
+Industri Minuman Beralkohol Hasil Fermentasi Malt
+Industri Minuman Lainnya
+Industri Minuman Ringan
+Industri Minyak Dari Jagung dan Beras
+Industri Minyak Goreng Bukan Minyak Kelapa dan Minyak Kelapa Sawit
+Industri Minyak Goreng Kelapa
+Industri Minyak Goreng Kelapa Sawit
+Industri Minyak Ikan
+Industri Minyak Mentah Inti Kelapa Sawit
+Industri Minyak Mentah Kelapa
+Industri Minyak Mentah Kelapa Sawit
+Industri Minyak Mentah dan Lemak Hewani Selain Ikan
+Industri Minyak Mentah dan Lemak Nabati
+Industri Minyak Mentah dan Lemak Nabati dan Hewani Lainnya
+Industri Mortar atau Beton Siap Pakai
+Industri Non Woven
+Industri Pakaian Jadi (Konveksi) Dari Kulit
+Industri Pakaian Jadi (Konveksi) Dari Tekstil
+Industri Pakaian Jadi Sulaman/Bordir
+Industri Pakaian Jadi dan Barang Dari Kulit Berbulu
+Industri Pakaian Rajutan
+Industri Panel Kayu Lainnya
+Industri Partikel Kayu dan Sejenisnya
+Industri Pati Beras dan Jagung
+Industri Pati Ubi Kayu
+Industri Pati dan Produk Pati Lainnya
+Industri Pelet Kelapa
+Industri Pelumatan Buah-buahan dan Sayuran
+Industri Pemanis Dari Beras dan Jagung
+Industri Pembekuan Biota Air Lainnya
+Industri Pembekuan Buah-Buahan dan Sayuran
+Industri Pembekuan Ikan
+Industri Pemindangan Biota Air Lainnya
+Industri Pemindangan Ikan
+Industri Pemintalan Benang
+Industri Pemintalan Benang Jahit
+Industri Pemisahan/Fraksinasi Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Kelapa Sawit
+Industri Pemurnian Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pencelupan Kulit Bulu
+Industri Pencetakan 3D Printing
+Industri Pencetakan Khusus
+Industri Pencetakan Umum
+Industri Pendinginan/Pengesan Biota Air Lainnya
+Industri Pendinginan/Pengesan Ikan
+Industri Pengasapan/Pemanggangan Biota Air Lainnya
+Industri Pengasapan/Pemanggangan Ikan
+Industri Pengasinan Buah-Buahan dan Sayuran
+Industri Pengawetan Kayu
+Industri Pengawetan Kotak, Bambu dan Sejenisnya
+Industri Pengawetan Kulit
+Industri Pengeringan Buah-Buahan dan Sayuran
+Industri Pengeringan dan Pengolahan Tembakau
+Industri Penggaraman/Pengeringan Biota Air Lainnya
+Industri Penggaraman/Pengeringan Ikan
+Industri Penggergajian Kayu
+Industri Penggilingan Aneka Kacang
+Industri Penggilingan Aneka Umbi dan Sayuran
+Industri Penggilingan Gandum dan Serelia Lainnya
+Industri Penggilingan Padi dan Penyosohan Beras
+Industri Penggilingan dan Pembersihan Jagung
+Industri Pengolahan Es Krim
+Industri Pengolahan Es Sejenisnya Yang Dapat Dimakan
+Industri Pengolahan Garam
+Industri Pengolahan Gula Lainnya Bukan Sirop
+Industri Pengolahan Herbal
+Industri Pengolahan Kopi
+Industri Pengolahan Produk Dari Susu Lainnya
+Industri Pengolahan Rotan
+Industri Pengolahan Rumput Laut
+Industri Pengolahan Sari Buah dan Sayuran
+Industri Pengolahan Susu Bubuk dan Susu Kental
+Industri Pengolahan Susu Segar dan Krim
+Industri Pengolahan Tea
+Industri Pengolahan dan Pengawetan Buah-Buahan dan Sayuran Dalam Kaleng
+Industri Pengolahan dan Pengawetan Ikan dan Biota Air (Bukan Udang) Dalam Kaleng
+Industri Pengolahan dan Pengawetan Kedelai dan Kacang-Kacangan Lainnya Selain Tahu dan Tempe
+Industri Pengolahan dan Pengawetan Lainnya Buah-Buahan dan Sayuran Bukan Kacang-Kacangan
+Industri Pengolahan dan Pengawetan Lainnya Untuk Biota Air Lainnya
+Industri Pengolahan dan Pengawetan Lainnya Untuk Ikan
+Industri Pengolahan dan Pengawetan Produk Daging dan Daging Unggas
+Industri Pengolahan dan Pengawetan Udang Dalam Kaleng
+Industri Penyamakan Kulit
+Industri Penyempurnaan Benang
+Industri Penyempurnaan Kain
+Industri Peragian/Fermentasi Biota Air Lainnya
+Industri Peragian/Fermentasi Ikan
+Industri Percetakan Kain
+Industri Perlengkapan Pakaian Dari Kulit
+Industri Perlengkapan Pakaian Dari Tekstil
+Industri Perlengkapan Rumah Tangga Dari Porselen
+Industri Perlengkapan Rumah Tangga Dari Tanah Liat/Keramik
+Industri Persiapan Serat Tekstil
+Industri Pertenunan
+Industri Produk Makanan Lainnya
+Industri Produk Masak Lainnya
+Industri Produk Masak dari Kelapa
+Industri Produk Roti dan Kue
+Industri Rajutan Kaos Kaki dan Sejenisnya
+Industri Ransum Makanan Hewan
+Industri Rokok Lainnya
+Industri Rokok Putih
+Industri Sepatu Olahraga
+Industri Sepatu Teknik Lapangan/Keperluan Industri
+Industri Sigaret Kretek Mesin
+Industri Sigaret Kretek Tangan
+Industri Sirop
+Industri Tahu Kedelai
+Industri Tali
+Industri Tekstil Lainnya YTDL
+Industri Tempe Kedelai
+Industri Tepung Beras dan Tepung Jagung
+Industri Tepung Campuran dan Adonan Tepung
+Industri Tepung Terigu
+Industri Veneer
+Industri Wadah dari Kayu
+Industri Yang Menghasilkan Kain Keperluan Industri
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Jaminan Sosial Wajib
+Jasa Pasca Panen
+Jasa Pasca Panen Budidaya Ikan Air Payau
+Jasa Pasca Panen Budidaya Ikan Air Tawar
+Jasa Pasca Panen Budidaya Ikan Laut
+Jasa Pasca Panen Penangkapan Ikan Di Perairan Darat
+Jasa Pasca Panen Penangkapan Ikan di Laut
+Jasa Pelayanan Kesehatan Ternak
+Jasa Pemanenan
+Jasa Pemupukan, Penanaman Bibit/Benih dan Pengendalian Hama dan Gulma
+Jasa Pengetasan Telur
+Jasa Penggunaan Kawasan Hutan Di Luar Sektor Kehutanan
+Jasa Pengolahan Lahan
+Jasa Penunjang Pertanian Lainnya
+Jasa Penunjang Peternakan Lainnya
+Jasa Penyemprotan dan Penyerbukan Melalui Udara
+Jasa Perkawinan Ternak
+Jasa Produksi Budidaya Ikan Air Payau
+Jasa Produksi Budidaya Ikan Air Tawar
+Jasa Produksi Budidaya Ikan Laut
+Jasa Produksi Penangkapan Ikan Di Laut
+Jasa Produksi Penangkapan Ikan Di Perairan Darat
+Jasa Sarana Produksi Budidaya Ikan Air Payau
+Jasa Sarana Produksi Budidaya Ikan Air Tawar
+Jasa Sarana Produksi Budidaya Ikan Laut
+Jasa Sarana Produksi Penangkapan Ikan di Laut
+Jasa Sarana Produksi Penangkapan Ikan di Perairan Darat
+Kedai Makanan
+Kedai Minuman
+Kegiatan Jasa Penunjang Pencetakkan
+Kepolisian
+Konstruksi Gedung Industri
+Konstruksi Gedung Kesehatan
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Lembaga Peradilan
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembesaran Crustacea Air Payau
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Kolam
+Pembesaran Ikan Air Tawar Di Sawah
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Tumbuhan Air Payau
+Pembibitan Ayam Lokal dan Persilangannya
+Pembibitan Ayam Ras
+Pembibitan Dan Budidaya Sapi Potong
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Pembibitan dan Budidaya Burung Merpati
+Pembibitan dan Budidaya Burung Puyuh
+Pembibitan dan Budidaya Burung Unta
+Pembibitan dan Budidaya Burung Walet
+Pembibitan dan Budidaya Cacing
+Pembibitan dan Budidaya Domba Perah
+Pembibitan dan Budidaya Domba Potong
+Pembibitan dan Budidaya Itik dan/atau Bebek
+Pembibitan dan Budidaya Kambing Perah
+Pembibitan dan Budidaya Kambing Potong
+Pembibitan dan Budidaya Kelinci
+Pembibitan dan Budidaya Kerbau Perah
+Pembibitan dan Budidaya Kerbau Potong
+Pembibitan dan Budidaya Lebah
+Pembibitan dan Budidaya Rusa
+Pembibitan dan Budidaya Sapi Perah
+Pembibitan dan Budidaya Ternak Unggas Lainnya
+Penangkaran Ikan dan Coral/Karang
+Penerbitan Buku
+Penerbitan Direktori dan Mailing List
+Penerbitan Piranti Lunak
+Penerbitan Surat Kabar, Jurnal dan Buletin atau Majalah
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Penginapan Remaja
+Pengusahaaan Tenaga Panas Bumi
+Pengusahaan Kokon/Kepompong Ulat Sutra
+Pengusahaan Perbenihan Tanaman Kehutanan
+Penjahitan dan Pembuatan Pakaian Sesuai Pesanan
+Penyediaan Akomodasi Jangka Pendek Lainnya
+Penyediaan Akomodasi Lainnya
+Penyiaran Radio Oleh Pemerintah
+Penyiaran Radio Oleh Swasta
+Perdagangan Besar Bahan Bakar Padat, Cair dan Gas dan Produk YBDI
+Perdagangan Besar Bahan Baku Obat Tradisional Untuk Manusia dan Hewan
+Perdagangan Besar Bahan Farmasi Untuk Manusia dan Hewan
+Perdagangan Besar Barang Bekas dan Sisa-sisa Tak Terpakai
+Perdagangan Besar Barang Logam Untuk Bahan Konstruksi
+Perdagangan Besar Binatang Hidup
+Perdagangan Besar Buah Yang Mengandung Minyak
+Perdagangan Besar Cat
+Perdagangan Besar Daging Ayam dan Daging Ayam Olahan
+Perdagangan Besar Daging Sapi dan Daging Sapi Olahan
+Perdagangan Besar Daging dan Daging Olahan Lainnya
+Perdagangan Besar Hasil Perikanan
+Perdagangan Besar Hasil Pertanian dan Hewan Hidup Lainnya
+Perdagangan Besar Kopi, Tea dan Kakao
+Perdagangan Besar Kosmetik untuk Hewan
+Perdagangan Besar Kosmetik untuk Manusia
+Perdagangan Besar Kulit dan Kulit Jangat
+Perdagangan Besar Logam dan Bijih Logam
+Perdagangan Besar Mineral Bukan Logam
+Perdagangan Besar Minuman Beralkohol
+Perdagangan Besar Minuman Non Alkohol  Bukan Susu
+Perdagangan Besar Minyak dan Lemak Hewani
+Perdagangan Besar Minyak dan Lemak Nabati
+Perdagangan Besar Obat Farmasi Untuk Hewan
+Perdagangan Besar Obat Farmasi Untuk Manusia
+Perdagangan Besar Obat Tradisional Untuk Hewan
+Perdagangan Besar Obat Tradisional Untuk Manusia
+Perdagangan Besar Rokok dan Tembakau
+Perdagangan Besar Tembakau Rajangan
+Periklanan
+Pertahanan Sipil
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Peternakan Babi
+Peternakan Kuda dan Sejenisnya
+Peternakan Unta dan Sejenisnya
+Pondok Wisata
+Produksi Bulu Domba Mentah/Raw Wool
+Produksi Es
+Real Estat Atas Dasar Balas Jasa (Fee) atau Kontrak
+Real Estat Yang Dimiliki Sendiri Atau Disewa
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Lainnya
+Reparasi Peralatan Listrik Lainnya
+Reparasi Produk Logam Pabrikasi Lainnya
+Reproduksi Media Rekaman Film dan Video
+Reproduksi Media Rekaman Suara dan Piranti Lunak
+Restoran
+Rumah Minum/Kafe
+Rumah/Kedai Obat Tradisional
+Rumah/Warung Makan
+Taman Rekreasi
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Usaha Kehutanan Lainnya
+Villa
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Pendidikan
+Yayasan Sosial</v>
       </c>
       <c r="AB25" t="str">
         <v/>
@@ -9992,8 +12255,441 @@
       <c r="Z26" t="str">
         <v/>
       </c>
-      <c r="AA26" t="str">
-        <v/>
+      <c r="AA26" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Keamanan Swasta
+Aktivitas Panti Asuhan Pemerintah
+Aktivitas Panti Asuhan Swasta
+Aktivitas Penerbitan Lainnya
+Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Penyiaran dan Pemrograman Televisi Oleh Pemerintah
+Aktivitas Penyiaran dan Pemrograman Televisi Oleh Swasta
+Aktivitas Perancangan Khusus
+Aktivitas Sosial Di Dalam Panti Gelandangan Dan Pengemis
+Aktivitas Sosial Di Dalam Panti Lainnya YTDL
+Aktivitas Sosial Di Dalam Panti Sosial Karya Wanita
+Aktivitas Sosial Di Dalam Panti Untuk Anak Yang Berhadapan Dengan Hukum
+Aktivitas Sosial Di Dalam Panti Untuk Bina Remaja
+Aktivitas Sosial Di Dalam Panti Untuk Korban Penyalahgunaan Narkotika, Alkohol , Psikotropika Dan Zat Adiktif
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Daksa
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Grahita
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Laras
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Netra
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Rungu Wicara
+Aktivitas Sosial Di Dalam Panti Untuk Petirahan Anak
+Aktivitas Sosial Pemerintah Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial Swasta Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Swasta Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial di Dalam Panti untuk Perawatan dan Pemulihan Kesehatan
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Sewa
+Apartemen Hotel
+Badan Nasional Penanggulangan Bencana Dan Pemadam Kebakaran
+Budidaya Ayam Lokal dan Persilangannya
+Budidaya Ayam Ras Pedaging
+Budidaya Ayam Ras Petelur
+Budidaya Biota Air Payau Lainnya
+Budidaya Ikan Air Tawar Di Media Lainnya
+Budidaya Ikan Hias Air Tawar
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Hotel Bintang
+Hotel Melati
+Iindustri Kain Tenun Ikat
+Industri Air Kemasan
+Industri Air Minum Isi Ulang
+Industri Alas Kaki Lainnya
+Industri Alas Kaki Untuk Keperluan Sehari-hari
+Industri Alat Dapur dari Kayu, Rotan dan Bambu
+Industri Alat Musik Bukan Tradisional
+Industri Alat Musik Tradisional
+Industri Alat Olahraga
+Industri Alat Permainan
+Industri Bangunan Prafabrikasi dari Kayu
+Industri Bantal Dan Sejenisnya
+Industri Barang Anyaman dari Rotan dan Bambu
+Industri Barang Anyaman dari Tanaman Bukan Rotan dan Bambu
+Industri Barang Bangunan dari Kayu
+Industri Barang Dari Kertas dan Papan Kertas Lainnya YTDL
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Hewan
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Lainnya
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Pribadi
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Teknik Industri
+Industri Barang Dari Tali
+Industri Barang Jadi Rajutan dan Sulaman
+Industri Barang Jadi Tekstil Lainnya
+Industri Barang Jadi Tekstil Sulaman
+Industri Barang Jadi Tekstil Untuk Keperluan Rumah Tangga
+Industri Barang Tahan Api dari Tanah Liat/Keramik Lainnya
+Industri Barang dari Kayu, Rotan, Gabus Lainnya YTDL
+Industri Bata, Mortar, Semen, Dan Sejenisnya Yang Tahan Api
+Industri Batik
+Industri Batu Bata dari Tanah Liat/Keramik
+Industri Berbagai Macam Pati Palma
+Industri Berbasis Daging Lumatan Surimi
+Industri Berbasis Lumatan Biota Air Lainnya
+Industri Bubur Kertas
+Industri Bulu Tiruan Rajutan
+Industri Bulu Tiruan Tenunan
+Industri Bumbu Masak dan Penyedap Masakan
+Industri Bumbu Rokok Serta Kelengkapan Rokok Lainnya
+Industri Dodol
+Industri Furnitur dari Kayu
+Industri Furnitur dari Plastik
+Industri Furnitur dari Rotan dan atau Bambu
+Industri Genteng Dari Tanah Liat/Keramik
+Industri Glukosa dan Sejenisnya
+Industri Gula Merah
+Industri Gula Pasir
+Industri Kain Ban
+Industri Kain Pita
+Industri Kain Rajutan
+Industri Kain Sulaman
+Industri Kain Tulle Dan Kain Jaring
+Industri Kakao
+Industri Kapuk
+Industri Karpet dan Permadani
+Industri Karung Bukan Goni
+Industri Karung Goni
+Industri Kayu Bakar dan Pelet Kayu
+Industri Kayu Laminasi
+Industri Kayu Lapis
+Industri Kayu Lapis Laminasi, Termasuk Decorative Plywood
+Industri Kecap
+Industri Kemasan dan Kotak dari Kertas dan Karton
+Industri Kembang Gula
+Industri Kembang Gula Lainnya
+Industri Kerajinan Ukiran dari Kayu Bukan Mebeller
+Industri Kerajinan YTDL
+Industri Kertas Berharga
+Industri Kertas Budaya
+Industri Kertas Khusus
+Industri Kertas Lainnya
+Industri Kertas Tissue
+Industri Kertas dan Papan Kerta Bergelombang
+Industri Kerupuk, Keripik, Peyek dan Sejenisnya
+Industri Konsentrat Makanan Hewan
+Industri Kopra
+Industri Krimer Nabati
+Industri Kue Basah
+Industri Kulit Komposisi
+Industri Mainan Anak-anak
+Industri Makanan Bayi
+Industri Makanan Dari Cokelat dan Kembang Gula dari Coklat
+Industri Makanan Dari Kedelai dan Kacang-Kacangan Lainnya Bukan Kecap, Tempe dan Tahu
+Industri Makanan Sereal
+Industri Makanan dan Masakan Olahan
+Industri Makaroni, Mie dan Produk Sejenisnya
+Industri Malt
+Industri Manisan Buah-Buahan dan Sayuran Kering
+Industri Margarine
+Industri Minuman Beralkohol Hasil Destilasi
+Industri Minuman Beralkohol Hasil Fermentasi Anggur dan Hasil Pertanian Lainnya
+Industri Minuman Beralkohol Hasil Fermentasi Malt
+Industri Minuman Lainnya
+Industri Minuman Ringan
+Industri Minyak Dari Jagung dan Beras
+Industri Minyak Goreng Bukan Minyak Kelapa dan Minyak Kelapa Sawit
+Industri Minyak Goreng Kelapa
+Industri Minyak Goreng Kelapa Sawit
+Industri Minyak Ikan
+Industri Minyak Mentah Inti Kelapa Sawit
+Industri Minyak Mentah Kelapa
+Industri Minyak Mentah Kelapa Sawit
+Industri Minyak Mentah dan Lemak Hewani Selain Ikan
+Industri Minyak Mentah dan Lemak Nabati
+Industri Minyak Mentah dan Lemak Nabati dan Hewani Lainnya
+Industri Mortar atau Beton Siap Pakai
+Industri Non Woven
+Industri Pakaian Jadi (Konveksi) Dari Kulit
+Industri Pakaian Jadi (Konveksi) Dari Tekstil
+Industri Pakaian Jadi Sulaman/Bordir
+Industri Pakaian Jadi dan Barang Dari Kulit Berbulu
+Industri Pakaian Rajutan
+Industri Panel Kayu Lainnya
+Industri Partikel Kayu dan Sejenisnya
+Industri Pati Beras dan Jagung
+Industri Pati Ubi Kayu
+Industri Pati dan Produk Pati Lainnya
+Industri Pelet Kelapa
+Industri Pelumatan Buah-buahan dan Sayuran
+Industri Pemanis Dari Beras dan Jagung
+Industri Pembekuan Biota Air Lainnya
+Industri Pembekuan Buah-Buahan dan Sayuran
+Industri Pembekuan Ikan
+Industri Pemindangan Biota Air Lainnya
+Industri Pemindangan Ikan
+Industri Pemintalan Benang
+Industri Pemintalan Benang Jahit
+Industri Pemisahan/Fraksinasi Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Kelapa Sawit
+Industri Pemurnian Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pencelupan Kulit Bulu
+Industri Pencetakan 3D Printing
+Industri Pencetakan Khusus
+Industri Pencetakan Umum
+Industri Pendinginan/Pengesan Biota Air Lainnya
+Industri Pendinginan/Pengesan Ikan
+Industri Pengasapan/Pemanggangan Biota Air Lainnya
+Industri Pengasapan/Pemanggangan Ikan
+Industri Pengasinan Buah-Buahan dan Sayuran
+Industri Pengawetan Kayu
+Industri Pengawetan Kotak, Bambu dan Sejenisnya
+Industri Pengawetan Kulit
+Industri Pengeringan Buah-Buahan dan Sayuran
+Industri Pengeringan dan Pengolahan Tembakau
+Industri Penggaraman/Pengeringan Biota Air Lainnya
+Industri Penggaraman/Pengeringan Ikan
+Industri Penggergajian Kayu
+Industri Penggilingan Aneka Kacang
+Industri Penggilingan Aneka Umbi dan Sayuran
+Industri Penggilingan Gandum dan Serelia Lainnya
+Industri Penggilingan Padi dan Penyosohan Beras
+Industri Penggilingan dan Pembersihan Jagung
+Industri Pengolahan Es Krim
+Industri Pengolahan Es Sejenisnya Yang Dapat Dimakan
+Industri Pengolahan Garam
+Industri Pengolahan Gula Lainnya Bukan Sirop
+Industri Pengolahan Herbal
+Industri Pengolahan Kopi
+Industri Pengolahan Produk Dari Susu Lainnya
+Industri Pengolahan Rotan
+Industri Pengolahan Rumput Laut
+Industri Pengolahan Sari Buah dan Sayuran
+Industri Pengolahan Susu Bubuk dan Susu Kental
+Industri Pengolahan Susu Segar dan Krim
+Industri Pengolahan Tea
+Industri Pengolahan dan Pengawetan Buah-Buahan dan Sayuran Dalam Kaleng
+Industri Pengolahan dan Pengawetan Ikan dan Biota Air (Bukan Udang) Dalam Kaleng
+Industri Pengolahan dan Pengawetan Kedelai dan Kacang-Kacangan Lainnya Selain Tahu dan Tempe
+Industri Pengolahan dan Pengawetan Lainnya Buah-Buahan dan Sayuran Bukan Kacang-Kacangan
+Industri Pengolahan dan Pengawetan Lainnya Untuk Biota Air Lainnya
+Industri Pengolahan dan Pengawetan Lainnya Untuk Ikan
+Industri Pengolahan dan Pengawetan Produk Daging dan Daging Unggas
+Industri Pengolahan dan Pengawetan Udang Dalam Kaleng
+Industri Penyamakan Kulit
+Industri Penyempurnaan Benang
+Industri Penyempurnaan Kain
+Industri Peragian/Fermentasi Biota Air Lainnya
+Industri Peragian/Fermentasi Ikan
+Industri Percetakan Kain
+Industri Perlengkapan Pakaian Dari Kulit
+Industri Perlengkapan Pakaian Dari Tekstil
+Industri Persiapan Serat Tekstil
+Industri Pertenunan
+Industri Produk Makanan Lainnya
+Industri Produk Masak Lainnya
+Industri Produk Masak dari Kelapa
+Industri Produk Roti dan Kue
+Industri Rajutan Kaos Kaki dan Sejenisnya
+Industri Ransum Makanan Hewan
+Industri Rokok Lainnya
+Industri Rokok Putih
+Industri Sepatu Olahraga
+Industri Sepatu Teknik Lapangan/Keperluan Industri
+Industri Sigaret Kretek Mesin
+Industri Sigaret Kretek Tangan
+Industri Sirop
+Industri Tahu Kedelai
+Industri Tali
+Industri Tekstil Lainnya YTDL
+Industri Tempe Kedelai
+Industri Tepung Beras dan Tepung Jagung
+Industri Tepung Campuran dan Adonan Tepung
+Industri Tepung Terigu
+Industri Veneer
+Industri Wadah dari Kayu
+Industri Yang Menghasilkan Kain Keperluan Industri
+Jaminan Sosial Wajib
+Jasa Pasca Panen
+Jasa Pasca Panen Budidaya Ikan Air Payau
+Jasa Pasca Panen Budidaya Ikan Air Tawar
+Jasa Pasca Panen Budidaya Ikan Laut
+Jasa Pasca Panen Penangkapan Ikan Di Perairan Darat
+Jasa Pasca Panen Penangkapan Ikan di Laut
+Jasa Pelayanan Kesehatan Ternak
+Jasa Pemanenan
+Jasa Pemupukan, Penanaman Bibit/Benih dan Pengendalian Hama dan Gulma
+Jasa Pengetasan Telur
+Jasa Penggunaan Kawasan Hutan Di Luar Sektor Kehutanan
+Jasa Pengolahan Lahan
+Jasa Penunjang Pertanian Lainnya
+Jasa Penunjang Peternakan Lainnya
+Jasa Penyemprotan dan Penyerbukan Melalui Udara
+Jasa Perkawinan Ternak
+Jasa Produksi Budidaya Ikan Air Payau
+Jasa Produksi Budidaya Ikan Air Tawar
+Jasa Produksi Budidaya Ikan Laut
+Jasa Produksi Penangkapan Ikan Di Laut
+Jasa Produksi Penangkapan Ikan Di Perairan Darat
+Jasa Sarana Produksi Budidaya Ikan Air Payau
+Jasa Sarana Produksi Budidaya Ikan Air Tawar
+Jasa Sarana Produksi Budidaya Ikan Laut
+Jasa Sarana Produksi Penangkapan Ikan di Laut
+Jasa Sarana Produksi Penangkapan Ikan di Perairan Darat
+Kedai Makanan
+Kedai Minuman
+Kegiatan Jasa Penunjang Pencetakkan
+Kepolisian
+Konstruksi Gedung Industri
+Konstruksi Gedung Kesehatan
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Lembaga Peradilan
+Pembenihan Ikan Air Payau
+Pembenihan Ikan Air Tawar
+Pembesaran Crustacea Air Payau
+Pembesaran Ikan Air Tawar Di Karamba Jaring Apung
+Pembesaran Ikan Air Tawar Di Karamba Jaring Tancap
+Pembesaran Ikan Air Tawar Di Kolam
+Pembesaran Ikan Air Tawar Di Sawah
+Pembesaran Ikan Air Tawar di Karamba
+Pembesaran Mollusca Air Payau
+Pembesaran Pisces/Ikan Bersirip Air Payau
+Pembesaran Tumbuhan Air Payau
+Pembibitan Ayam Lokal dan Persilangannya
+Pembibitan Ayam Ras
+Pembibitan Dan Budidaya Sapi Potong
+Pembibitan dan Budidaya Aneka Ternak Lainnya
+Pembibitan dan Budidaya Burung Merpati
+Pembibitan dan Budidaya Burung Puyuh
+Pembibitan dan Budidaya Burung Unta
+Pembibitan dan Budidaya Burung Walet
+Pembibitan dan Budidaya Cacing
+Pembibitan dan Budidaya Domba Perah
+Pembibitan dan Budidaya Domba Potong
+Pembibitan dan Budidaya Itik dan/atau Bebek
+Pembibitan dan Budidaya Kambing Perah
+Pembibitan dan Budidaya Kambing Potong
+Pembibitan dan Budidaya Kelinci
+Pembibitan dan Budidaya Kerbau Perah
+Pembibitan dan Budidaya Kerbau Potong
+Pembibitan dan Budidaya Lebah
+Pembibitan dan Budidaya Rusa
+Pembibitan dan Budidaya Sapi Perah
+Pembibitan dan Budidaya Ternak Unggas Lainnya
+Penangkaran Ikan dan Coral/Karang
+Penerbitan Buku
+Penerbitan Direktori dan Mailing List
+Penerbitan Piranti Lunak
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Penginapan Remaja
+Pengusahaaan Tenaga Panas Bumi
+Pengusahaan Kokon/Kepompong Ulat Sutra
+Pengusahaan Perbenihan Tanaman Kehutanan
+Penjahitan dan Pembuatan Pakaian Sesuai Pesanan
+Penyediaan Akomodasi Jangka Pendek Lainnya
+Penyediaan Akomodasi Lainnya
+Penyiaran Radio Oleh Pemerintah
+Penyiaran Radio Oleh Swasta
+Perdagangan Besar Bahan Bakar Padat, Cair dan Gas dan Produk YBDI
+Perdagangan Besar Bahan Baku Obat Tradisional Untuk Manusia dan Hewan
+Perdagangan Besar Bahan Farmasi Untuk Manusia dan Hewan
+Perdagangan Besar Barang Bekas dan Sisa-sisa Tak Terpakai
+Perdagangan Besar Barang Logam Untuk Bahan Konstruksi
+Perdagangan Besar Binatang Hidup
+Perdagangan Besar Buah Yang Mengandung Minyak
+Perdagangan Besar Cat
+Perdagangan Besar Daging Ayam dan Daging Ayam Olahan
+Perdagangan Besar Daging Sapi dan Daging Sapi Olahan
+Perdagangan Besar Daging dan Daging Olahan Lainnya
+Perdagangan Besar Hasil Perikanan
+Perdagangan Besar Hasil Pertanian dan Hewan Hidup Lainnya
+Perdagangan Besar Kopi, Tea dan Kakao
+Perdagangan Besar Kosmetik untuk Hewan
+Perdagangan Besar Kosmetik untuk Manusia
+Perdagangan Besar Kulit dan Kulit Jangat
+Perdagangan Besar Logam dan Bijih Logam
+Perdagangan Besar Mineral Bukan Logam
+Perdagangan Besar Minuman Beralkohol
+Perdagangan Besar Minuman Non Alkohol  Bukan Susu
+Perdagangan Besar Minyak dan Lemak Hewani
+Perdagangan Besar Minyak dan Lemak Nabati
+Perdagangan Besar Obat Farmasi Untuk Hewan
+Perdagangan Besar Obat Farmasi Untuk Manusia
+Perdagangan Besar Obat Tradisional Untuk Hewan
+Perdagangan Besar Obat Tradisional Untuk Manusia
+Perdagangan Besar Rokok dan Tembakau
+Perdagangan Besar Tembakau Rajangan
+Periklanan
+Pertahanan Sipil
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Peternakan Babi
+Peternakan Kuda dan Sejenisnya
+Peternakan Unta dan Sejenisnya
+Pondok Wisata
+Produksi Bulu Domba Mentah/Raw Wool
+Produksi Es
+Real Estat Atas Dasar Balas Jasa (Fee) atau Kontrak
+Real Estat Yang Dimiliki Sendiri Atau Disewa
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Listrik Lainnya
+Reproduksi Media Rekaman Film dan Video
+Reproduksi Media Rekaman Suara dan Piranti Lunak
+Restoran
+Rumah Minum/Kafe
+Rumah/Kedai Obat Tradisional
+Rumah/Warung Makan
+Taman Rekreasi
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Usaha Kehutanan Lainnya
+Villa
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Pendidikan
+Yayasan Sosial</v>
       </c>
       <c r="AB26" t="str">
         <v/>
@@ -10923,8 +13619,363 @@
       <c r="Z27" t="str">
         <v/>
       </c>
-      <c r="AA27" t="str">
-        <v/>
+      <c r="AA27" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Keamanan Swasta
+Aktivitas Panti Asuhan Pemerintah
+Aktivitas Panti Asuhan Swasta
+Aktivitas Penerbitan Lainnya
+Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Penyiaran dan Pemrograman Televisi Oleh Pemerintah
+Aktivitas Penyiaran dan Pemrograman Televisi Oleh Swasta
+Aktivitas Perancangan Khusus
+Aktivitas Sosial Di Dalam Panti Gelandangan Dan Pengemis
+Aktivitas Sosial Di Dalam Panti Lainnya YTDL
+Aktivitas Sosial Di Dalam Panti Sosial Karya Wanita
+Aktivitas Sosial Di Dalam Panti Untuk Anak Yang Berhadapan Dengan Hukum
+Aktivitas Sosial Di Dalam Panti Untuk Bina Remaja
+Aktivitas Sosial Di Dalam Panti Untuk Korban Penyalahgunaan Narkotika, Alkohol , Psikotropika Dan Zat Adiktif
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Daksa
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Grahita
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Laras
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Netra
+Aktivitas Sosial Di Dalam Panti Untuk Penyandang Disabilitas Rungu Wicara
+Aktivitas Sosial Di Dalam Panti Untuk Petirahan Anak
+Aktivitas Sosial Pemerintah Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Pemerintah Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial Swasta Di Dalam Panti Untuk Lanjut Usia
+Aktivitas Sosial Swasta Tanpa Akomodasi Untuk Lanjut Usia Dan Penyandang Disabilitas
+Aktivitas Sosial di Dalam Panti untuk Perawatan dan Pemulihan Kesehatan
+Angkatan Darat
+Angkatan Laut
+Angkatan Udara
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Sewa
+Apartemen Hotel
+Badan Nasional Penanggulangan Bencana Dan Pemadam Kebakaran
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Hotel Bintang
+Hotel Melati
+Iindustri Kain Tenun Ikat
+Industri Air Kemasan
+Industri Air Minum Isi Ulang
+Industri Alas Kaki Lainnya
+Industri Alas Kaki Untuk Keperluan Sehari-hari
+Industri Alat Dapur dari Kayu, Rotan dan Bambu
+Industri Alat Musik Bukan Tradisional
+Industri Alat Musik Tradisional
+Industri Alat Olahraga
+Industri Alat Permainan
+Industri Bangunan Prafabrikasi dari Kayu
+Industri Bantal Dan Sejenisnya
+Industri Barang Anyaman dari Rotan dan Bambu
+Industri Barang Anyaman dari Tanaman Bukan Rotan dan Bambu
+Industri Barang Bangunan dari Kayu
+Industri Barang Dari Kertas dan Papan Kertas Lainnya YTDL
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Hewan
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Lainnya
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Pribadi
+Industri Barang Dari Kulit dan Kulit Komposisi Untuk Keperluan Teknik Industri
+Industri Barang Dari Tali
+Industri Barang Jadi Rajutan dan Sulaman
+Industri Barang Jadi Tekstil Lainnya
+Industri Barang Jadi Tekstil Sulaman
+Industri Barang Jadi Tekstil Untuk Keperluan Rumah Tangga
+Industri Barang dari Kayu, Rotan, Gabus Lainnya YTDL
+Industri Bata, Mortar, Semen, Dan Sejenisnya Yang Tahan Api
+Industri Batik
+Industri Berbagai Macam Pati Palma
+Industri Berbasis Daging Lumatan Surimi
+Industri Berbasis Lumatan Biota Air Lainnya
+Industri Bubur Kertas
+Industri Bulu Tiruan Rajutan
+Industri Bulu Tiruan Tenunan
+Industri Bumbu Masak dan Penyedap Masakan
+Industri Bumbu Rokok Serta Kelengkapan Rokok Lainnya
+Industri Dodol
+Industri Furnitur dari Kayu
+Industri Furnitur dari Plastik
+Industri Furnitur dari Rotan dan atau Bambu
+Industri Glukosa dan Sejenisnya
+Industri Gula Merah
+Industri Gula Pasir
+Industri Kain Ban
+Industri Kain Pita
+Industri Kain Rajutan
+Industri Kain Sulaman
+Industri Kain Tulle Dan Kain Jaring
+Industri Kakao
+Industri Kapuk
+Industri Karpet dan Permadani
+Industri Karung Bukan Goni
+Industri Karung Goni
+Industri Kayu Bakar dan Pelet Kayu
+Industri Kayu Laminasi
+Industri Kayu Lapis
+Industri Kayu Lapis Laminasi, Termasuk Decorative Plywood
+Industri Kecap
+Industri Kemasan dan Kotak dari Kertas dan Karton
+Industri Kembang Gula
+Industri Kembang Gula Lainnya
+Industri Kerajinan Ukiran dari Kayu Bukan Mebeller
+Industri Kerajinan YTDL
+Industri Kertas Berharga
+Industri Kertas Budaya
+Industri Kertas Khusus
+Industri Kertas Lainnya
+Industri Kertas Tissue
+Industri Kertas dan Papan Kerta Bergelombang
+Industri Kerupuk, Keripik, Peyek dan Sejenisnya
+Industri Konsentrat Makanan Hewan
+Industri Kopra
+Industri Krimer Nabati
+Industri Kue Basah
+Industri Kulit Komposisi
+Industri Mainan Anak-anak
+Industri Makanan Bayi
+Industri Makanan Dari Cokelat dan Kembang Gula dari Coklat
+Industri Makanan Dari Kedelai dan Kacang-Kacangan Lainnya Bukan Kecap, Tempe dan Tahu
+Industri Makanan Sereal
+Industri Makanan dan Masakan Olahan
+Industri Makaroni, Mie dan Produk Sejenisnya
+Industri Malt
+Industri Manisan Buah-Buahan dan Sayuran Kering
+Industri Margarine
+Industri Minuman Beralkohol Hasil Destilasi
+Industri Minuman Beralkohol Hasil Fermentasi Anggur dan Hasil Pertanian Lainnya
+Industri Minuman Beralkohol Hasil Fermentasi Malt
+Industri Minuman Lainnya
+Industri Minuman Ringan
+Industri Minyak Dari Jagung dan Beras
+Industri Minyak Goreng Bukan Minyak Kelapa dan Minyak Kelapa Sawit
+Industri Minyak Goreng Kelapa
+Industri Minyak Goreng Kelapa Sawit
+Industri Minyak Ikan
+Industri Minyak Mentah Inti Kelapa Sawit
+Industri Minyak Mentah Kelapa
+Industri Minyak Mentah Kelapa Sawit
+Industri Minyak Mentah dan Lemak Hewani Selain Ikan
+Industri Minyak Mentah dan Lemak Nabati
+Industri Minyak Mentah dan Lemak Nabati dan Hewani Lainnya
+Industri Mortar atau Beton Siap Pakai
+Industri Non Woven
+Industri Pakaian Jadi (Konveksi) Dari Kulit
+Industri Pakaian Jadi (Konveksi) Dari Tekstil
+Industri Pakaian Jadi Sulaman/Bordir
+Industri Pakaian Jadi dan Barang Dari Kulit Berbulu
+Industri Pakaian Rajutan
+Industri Panel Kayu Lainnya
+Industri Partikel Kayu dan Sejenisnya
+Industri Pati Beras dan Jagung
+Industri Pati Ubi Kayu
+Industri Pati dan Produk Pati Lainnya
+Industri Pelet Kelapa
+Industri Pelumatan Buah-buahan dan Sayuran
+Industri Pemanis Dari Beras dan Jagung
+Industri Pembekuan Biota Air Lainnya
+Industri Pembekuan Buah-Buahan dan Sayuran
+Industri Pembekuan Ikan
+Industri Pemindangan Biota Air Lainnya
+Industri Pemindangan Ikan
+Industri Pemintalan Benang
+Industri Pemintalan Benang Jahit
+Industri Pemisahan/Fraksinasi Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Inti Kelapa Sawit
+Industri Pemisahan/Fraksinasi Minyak Murni Kelapa Sawit
+Industri Pemurnian Minyak Mentah Kelapa Sawit dan Minyak Mentah Inti Kelapa Sawit
+Industri Pencelupan Kulit Bulu
+Industri Pencetakan 3D Printing
+Industri Pencetakan Khusus
+Industri Pencetakan Umum
+Industri Pendinginan/Pengesan Biota Air Lainnya
+Industri Pendinginan/Pengesan Ikan
+Industri Pengasapan/Pemanggangan Biota Air Lainnya
+Industri Pengasapan/Pemanggangan Ikan
+Industri Pengasinan Buah-Buahan dan Sayuran
+Industri Pengawetan Kayu
+Industri Pengawetan Kotak, Bambu dan Sejenisnya
+Industri Pengawetan Kulit
+Industri Pengeringan Buah-Buahan dan Sayuran
+Industri Pengeringan dan Pengolahan Tembakau
+Industri Penggaraman/Pengeringan Biota Air Lainnya
+Industri Penggaraman/Pengeringan Ikan
+Industri Penggergajian Kayu
+Industri Penggilingan Aneka Kacang
+Industri Penggilingan Aneka Umbi dan Sayuran
+Industri Penggilingan Gandum dan Serelia Lainnya
+Industri Penggilingan Padi dan Penyosohan Beras
+Industri Penggilingan dan Pembersihan Jagung
+Industri Pengolahan Es Krim
+Industri Pengolahan Es Sejenisnya Yang Dapat Dimakan
+Industri Pengolahan Garam
+Industri Pengolahan Gula Lainnya Bukan Sirop
+Industri Pengolahan Herbal
+Industri Pengolahan Kopi
+Industri Pengolahan Produk Dari Susu Lainnya
+Industri Pengolahan Rotan
+Industri Pengolahan Rumput Laut
+Industri Pengolahan Sari Buah dan Sayuran
+Industri Pengolahan Susu Bubuk dan Susu Kental
+Industri Pengolahan Susu Segar dan Krim
+Industri Pengolahan Tea
+Industri Pengolahan dan Pengawetan Buah-Buahan dan Sayuran Dalam Kaleng
+Industri Pengolahan dan Pengawetan Ikan dan Biota Air (Bukan Udang) Dalam Kaleng
+Industri Pengolahan dan Pengawetan Kedelai dan Kacang-Kacangan Lainnya Selain Tahu dan Tempe
+Industri Pengolahan dan Pengawetan Lainnya Buah-Buahan dan Sayuran Bukan Kacang-Kacangan
+Industri Pengolahan dan Pengawetan Lainnya Untuk Biota Air Lainnya
+Industri Pengolahan dan Pengawetan Lainnya Untuk Ikan
+Industri Pengolahan dan Pengawetan Produk Daging dan Daging Unggas
+Industri Pengolahan dan Pengawetan Udang Dalam Kaleng
+Industri Penyamakan Kulit
+Industri Penyempurnaan Benang
+Industri Penyempurnaan Kain
+Industri Peragian/Fermentasi Biota Air Lainnya
+Industri Peragian/Fermentasi Ikan
+Industri Percetakan Kain
+Industri Perlengkapan Pakaian Dari Kulit
+Industri Perlengkapan Pakaian Dari Tekstil
+Industri Persiapan Serat Tekstil
+Industri Pertenunan
+Industri Produk Makanan Lainnya
+Industri Produk Masak Lainnya
+Industri Produk Masak dari Kelapa
+Industri Produk Roti dan Kue
+Industri Rajutan Kaos Kaki dan Sejenisnya
+Industri Ransum Makanan Hewan
+Industri Rokok Lainnya
+Industri Rokok Putih
+Industri Sepatu Olahraga
+Industri Sepatu Teknik Lapangan/Keperluan Industri
+Industri Sigaret Kretek Mesin
+Industri Sigaret Kretek Tangan
+Industri Sirop
+Industri Tahu Kedelai
+Industri Tali
+Industri Tekstil Lainnya YTDL
+Industri Tempe Kedelai
+Industri Tepung Beras dan Tepung Jagung
+Industri Tepung Campuran dan Adonan Tepung
+Industri Tepung Terigu
+Industri Veneer
+Industri Wadah dari Kayu
+Industri Yang Menghasilkan Kain Keperluan Industri
+Jaminan Sosial Wajib
+Kedai Makanan
+Kedai Minuman
+Kegiatan Jasa Penunjang Pencetakkan
+Kepolisian
+Konstruksi Gedung Industri
+Konstruksi Gedung Kesehatan
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Lembaga Peradilan
+Penerbitan Buku
+Penerbitan Direktori dan Mailing List
+Penerbitan Piranti Lunak
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Penginapan Remaja
+Pengusahaaan Tenaga Panas Bumi
+Penjahitan dan Pembuatan Pakaian Sesuai Pesanan
+Penyediaan Akomodasi Jangka Pendek Lainnya
+Penyediaan Akomodasi Lainnya
+Penyiaran Radio Oleh Pemerintah
+Penyiaran Radio Oleh Swasta
+Perdagangan Besar Bahan Bakar Padat, Cair dan Gas dan Produk YBDI
+Perdagangan Besar Bahan Baku Obat Tradisional Untuk Manusia dan Hewan
+Perdagangan Besar Bahan Farmasi Untuk Manusia dan Hewan
+Perdagangan Besar Barang Bekas dan Sisa-sisa Tak Terpakai
+Perdagangan Besar Barang Logam Untuk Bahan Konstruksi
+Perdagangan Besar Binatang Hidup
+Perdagangan Besar Buah Yang Mengandung Minyak
+Perdagangan Besar Cat
+Perdagangan Besar Daging Ayam dan Daging Ayam Olahan
+Perdagangan Besar Daging Sapi dan Daging Sapi Olahan
+Perdagangan Besar Daging dan Daging Olahan Lainnya
+Perdagangan Besar Hasil Perikanan
+Perdagangan Besar Hasil Pertanian dan Hewan Hidup Lainnya
+Perdagangan Besar Kopi, Tea dan Kakao
+Perdagangan Besar Kosmetik untuk Hewan
+Perdagangan Besar Kosmetik untuk Manusia
+Perdagangan Besar Kulit dan Kulit Jangat
+Perdagangan Besar Logam dan Bijih Logam
+Perdagangan Besar Mineral Bukan Logam
+Perdagangan Besar Minuman Beralkohol
+Perdagangan Besar Minuman Non Alkohol  Bukan Susu
+Perdagangan Besar Minyak dan Lemak Hewani
+Perdagangan Besar Minyak dan Lemak Nabati
+Perdagangan Besar Obat Farmasi Untuk Hewan
+Perdagangan Besar Obat Farmasi Untuk Manusia
+Perdagangan Besar Obat Tradisional Untuk Hewan
+Perdagangan Besar Obat Tradisional Untuk Manusia
+Perdagangan Besar Rokok dan Tembakau
+Perdagangan Besar Tembakau Rajangan
+Periklanan
+Pertahanan Sipil
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Pondok Wisata
+Produksi Es
+Real Estat Atas Dasar Balas Jasa (Fee) atau Kontrak
+Real Estat Yang Dimiliki Sendiri Atau Disewa
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reproduksi Media Rekaman Film dan Video
+Reproduksi Media Rekaman Suara dan Piranti Lunak
+Restoran
+Rumah Minum/Kafe
+Rumah/Kedai Obat Tradisional
+Rumah/Warung Makan
+Taman Rekreasi
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Villa
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Pendidikan
+Yayasan Sosial</v>
       </c>
       <c r="AB27" t="str">
         <v/>
@@ -11103,8 +14154,50 @@
       <c r="Z28" t="str">
         <v/>
       </c>
-      <c r="AA28" t="str">
-        <v/>
+      <c r="AA28" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Industri Air Minum dan Air Mineral
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium</v>
       </c>
       <c r="AB28" t="str">
         <v/>
@@ -11643,8 +14736,123 @@
       <c r="Z29" t="str">
         <v/>
       </c>
-      <c r="AA29" t="str">
-        <v/>
+      <c r="AA29" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Perancangan Khusus
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Laut Dalam Negeri Liner dan Tramper untuk Penumpang
+Angkutan Laut Dalam Negeri Perintis Untuk Penumpang
+Angkutan Laut Dalam Negeri Untuk Wisata
+Angkutan Laut Luar Negeri Liner dan Tramper Untuk Penumpang
+Angkutan Laut Luar Negeri Untuk Wisata
+Angkutan Laut Perairan Pelabuhan Dalam Negeri Untuk Penumpang
+Angkutan Sewa
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Industri Air Minum dan Air Mineral
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Kontruksi Gedung Penginapan
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) Selain di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Beras
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau (Barang-barang Kelontong) Bukan Di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Buah-buahan
+Perdagangan Eceran Daging dan Ikan Olahan
+Perdagangan Eceran Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Hasil Perikanan
+Perdagangan Eceran Hasil Pertanian Lainnya
+Perdagangan Eceran Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Beras
+Perdagangan Eceran Kaki Lima dan Los Pasar Daging Olahan dan Ikan Olahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Buah-buahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Perikanan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Makanan dan Minuman YTDL
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Padi dan Palawija
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Sayur-sayuran
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Tanaman Hias dan Hasil Pertanian Lainnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Kopi, Gula Pasir, Gula Merah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Minuman
+Perdagangan Eceran Kaki Lima dan Los Pasar Pakan Ternak, Pakan Unggas dan Pakan Ikan
+Perdagangan Eceran Kaki Lima dan Los Pasar Rokok dan Tembakau
+Perdagangan Eceran Kaki Lima dan Los Pasar Roti, Kue Kering, Kue Basah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Tahu, Tempe, Tauco dan Oncom
+Perdagangan Eceran Kaki Lima dan Los Pasar Tekstil
+Perdagangan Eceran Keliling Komoditi Makanan, Minuman atau Tembakau Hasil Industri Pengolahan
+Perdagangan Eceran Keliling Perlengkapan Rumah Tangga dan Perlengkapan Dapur
+Perdagangan Eceran Khusus Rokok dan Tembakau di Toko
+Perdagangan Eceran Kopi, Gula Pasir dan Gula Merah
+Perdagangan Eceran Makanan Lainnya
+Perdagangan Eceran Minuman Beralkohol
+Perdagangan Eceran Minuman Tidak Beralkohol
+Perdagangan Eceran Minyak Pelumas di Toko
+Perdagangan Eceran Padi dan Palawija
+Perdagangan Eceran Roti, Kue Kering, serta Kue Basah dan Sejenisnya
+Perdagangan Eceran Sayuran
+Perdagangan Eceran Tahu, Tempe, Tauco dan Oncom
+Periklanan
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Produksi Es
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Lokomotif dan Gerbong Kereta
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Lainnya
+Reparasi Peralatan Listrik Lainnya
+Reparasi Pesawat Terbang
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Sosial</v>
       </c>
       <c r="AB29" t="str">
         <v/>
@@ -12183,8 +15391,117 @@
       <c r="Z30" t="str">
         <v/>
       </c>
-      <c r="AA30" t="str">
-        <v/>
+      <c r="AA30" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Perancangan Khusus
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Sewa
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Industri Air Minum dan Air Mineral
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Kontruksi Gedung Penginapan
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) Selain di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Beras
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau (Barang-barang Kelontong) Bukan Di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Buah-buahan
+Perdagangan Eceran Daging dan Ikan Olahan
+Perdagangan Eceran Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Hasil Perikanan
+Perdagangan Eceran Hasil Pertanian Lainnya
+Perdagangan Eceran Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Beras
+Perdagangan Eceran Kaki Lima dan Los Pasar Daging Olahan dan Ikan Olahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Buah-buahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Perikanan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Makanan dan Minuman YTDL
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Padi dan Palawija
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Sayur-sayuran
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Tanaman Hias dan Hasil Pertanian Lainnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Kopi, Gula Pasir, Gula Merah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Minuman
+Perdagangan Eceran Kaki Lima dan Los Pasar Pakan Ternak, Pakan Unggas dan Pakan Ikan
+Perdagangan Eceran Kaki Lima dan Los Pasar Rokok dan Tembakau
+Perdagangan Eceran Kaki Lima dan Los Pasar Roti, Kue Kering, Kue Basah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Tahu, Tempe, Tauco dan Oncom
+Perdagangan Eceran Kaki Lima dan Los Pasar Tekstil
+Perdagangan Eceran Keliling Komoditi Makanan, Minuman atau Tembakau Hasil Industri Pengolahan
+Perdagangan Eceran Keliling Perlengkapan Rumah Tangga dan Perlengkapan Dapur
+Perdagangan Eceran Khusus Rokok dan Tembakau di Toko
+Perdagangan Eceran Kopi, Gula Pasir dan Gula Merah
+Perdagangan Eceran Makanan Lainnya
+Perdagangan Eceran Minuman Beralkohol
+Perdagangan Eceran Minuman Tidak Beralkohol
+Perdagangan Eceran Minyak Pelumas di Toko
+Perdagangan Eceran Padi dan Palawija
+Perdagangan Eceran Roti, Kue Kering, serta Kue Basah dan Sejenisnya
+Perdagangan Eceran Sayuran
+Perdagangan Eceran Tahu, Tempe, Tauco dan Oncom
+Periklanan
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Produksi Es
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Lokomotif dan Gerbong Kereta
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Lainnya
+Reparasi Peralatan Listrik Lainnya
+Reparasi Pesawat Terbang
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Sosial</v>
       </c>
       <c r="AB30" t="str">
         <v/>
@@ -12724,8 +16041,117 @@
       <c r="Z31" t="str">
         <v/>
       </c>
-      <c r="AA31" t="str">
-        <v/>
+      <c r="AA31" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Perancangan Khusus
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Sewa
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Industri Air Minum dan Air Mineral
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Kontruksi Gedung Penginapan
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) Selain di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Beras
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau (Barang-barang Kelontong) Bukan Di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Buah-buahan
+Perdagangan Eceran Daging dan Ikan Olahan
+Perdagangan Eceran Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Hasil Perikanan
+Perdagangan Eceran Hasil Pertanian Lainnya
+Perdagangan Eceran Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Beras
+Perdagangan Eceran Kaki Lima dan Los Pasar Daging Olahan dan Ikan Olahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Buah-buahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Perikanan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Makanan dan Minuman YTDL
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Padi dan Palawija
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Sayur-sayuran
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Tanaman Hias dan Hasil Pertanian Lainnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Kopi, Gula Pasir, Gula Merah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Minuman
+Perdagangan Eceran Kaki Lima dan Los Pasar Pakan Ternak, Pakan Unggas dan Pakan Ikan
+Perdagangan Eceran Kaki Lima dan Los Pasar Rokok dan Tembakau
+Perdagangan Eceran Kaki Lima dan Los Pasar Roti, Kue Kering, Kue Basah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Tahu, Tempe, Tauco dan Oncom
+Perdagangan Eceran Kaki Lima dan Los Pasar Tekstil
+Perdagangan Eceran Keliling Komoditi Makanan, Minuman atau Tembakau Hasil Industri Pengolahan
+Perdagangan Eceran Keliling Perlengkapan Rumah Tangga dan Perlengkapan Dapur
+Perdagangan Eceran Khusus Rokok dan Tembakau di Toko
+Perdagangan Eceran Kopi, Gula Pasir dan Gula Merah
+Perdagangan Eceran Makanan Lainnya
+Perdagangan Eceran Minuman Beralkohol
+Perdagangan Eceran Minuman Tidak Beralkohol
+Perdagangan Eceran Minyak Pelumas di Toko
+Perdagangan Eceran Padi dan Palawija
+Perdagangan Eceran Roti, Kue Kering, serta Kue Basah dan Sejenisnya
+Perdagangan Eceran Sayuran
+Perdagangan Eceran Tahu, Tempe, Tauco dan Oncom
+Periklanan
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Produksi Es
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Lokomotif dan Gerbong Kereta
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Lainnya
+Reparasi Peralatan Listrik Lainnya
+Reparasi Pesawat Terbang
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Sosial</v>
       </c>
       <c r="AB31" t="str">
         <v/>
@@ -13259,8 +16685,117 @@
       <c r="Z32" t="str">
         <v/>
       </c>
-      <c r="AA32" t="str">
-        <v/>
+      <c r="AA32" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Aktivitas Perancangan Khusus
+Angkutan Bermotor Untuk Barang Khusus
+Angkutan Bermotor Untuk Barang Umum
+Angkutan Sewa
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Industri Air Minum dan Air Mineral
+Instalasi/Pemasangan Mesin dan Peralatan Industri
+Kontruksi Gedung Penginapan
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) Selain di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Bahan Bakar Minyak, Bahan Bakar Gas (BBG), dan Liquified Petroleum Gas (LPG) di Sarana Pengisian Bahan Bakar Transportasi Darat, Laut dan Udara
+Perdagangan Eceran Beras
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau (Barang-barang Kelontong) Bukan Di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Bukan Makanan, Minuman atau Tembakau di Toserba
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Berbagai Macam Barang Yang Utamanya Makanan, Minuman Atau Tembakau Di Minimarket/Supermarket/Hypermarket
+Perdagangan Eceran Buah-buahan
+Perdagangan Eceran Daging dan Ikan Olahan
+Perdagangan Eceran Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Hasil Perikanan
+Perdagangan Eceran Hasil Pertanian Lainnya
+Perdagangan Eceran Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Beras
+Perdagangan Eceran Kaki Lima dan Los Pasar Daging Olahan dan Ikan Olahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Buah-buahan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Kehutanan dan Perburuan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Perikanan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Hasil Peternakan
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Makanan dan Minuman YTDL
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Padi dan Palawija
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Sayur-sayuran
+Perdagangan Eceran Kaki Lima dan Los Pasar Komoditi Tanaman Hias dan Hasil Pertanian Lainnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Kopi, Gula Pasir, Gula Merah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Minuman
+Perdagangan Eceran Kaki Lima dan Los Pasar Pakan Ternak, Pakan Unggas dan Pakan Ikan
+Perdagangan Eceran Kaki Lima dan Los Pasar Rokok dan Tembakau
+Perdagangan Eceran Kaki Lima dan Los Pasar Roti, Kue Kering, Kue Basah dan Sejenisnya
+Perdagangan Eceran Kaki Lima dan Los Pasar Tahu, Tempe, Tauco dan Oncom
+Perdagangan Eceran Kaki Lima dan Los Pasar Tekstil
+Perdagangan Eceran Keliling Komoditi Makanan, Minuman atau Tembakau Hasil Industri Pengolahan
+Perdagangan Eceran Keliling Perlengkapan Rumah Tangga dan Perlengkapan Dapur
+Perdagangan Eceran Khusus Rokok dan Tembakau di Toko
+Perdagangan Eceran Kopi, Gula Pasir dan Gula Merah
+Perdagangan Eceran Makanan Lainnya
+Perdagangan Eceran Minuman Beralkohol
+Perdagangan Eceran Minuman Tidak Beralkohol
+Perdagangan Eceran Minyak Pelumas di Toko
+Perdagangan Eceran Padi dan Palawija
+Perdagangan Eceran Roti, Kue Kering, serta Kue Basah dan Sejenisnya
+Perdagangan Eceran Sayuran
+Perdagangan Eceran Tahu, Tempe, Tauco dan Oncom
+Periklanan
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium
+Produksi Es
+Reparasi Alat Angkutan Lainnya, Bukan Kendaraan Bermotor
+Reparasi Alat Ukur, Alat Uji dan Peralatan Navigasi dan Pengontrol
+Reparasi Baterai dan Akumulator Listrik
+Reparasi Kapal, Perahu dan Bangunan Terapung
+Reparasi Lokomotif dan Gerbong Kereta
+Reparasi Mesin Untuk Keperluan Khusus
+Reparasi Mesin Untuk Keperluan Umum
+Reparasi Motor Listrik, Generator dan Transformation
+Reparasi Peralatan Fotografi dan Optik
+Reparasi Peralatan Iradiasi, Elektromedis dan Elektroterapi
+Reparasi Peralatan Lainnya
+Reparasi Peralatan Listrik Lainnya
+Reparasi Pesawat Terbang
+Treatment dan Pembuangan Limbah dan Sampah Tidak Berbahaya
+Yayasan Keagamaan
+Yayasan Kemanusiaan
+Yayasan Sosial</v>
       </c>
       <c r="AB32" t="str">
         <v/>
@@ -13466,8 +17001,12 @@
       <c r="Z33" t="str">
         <v/>
       </c>
-      <c r="AA33" t="str">
-        <v/>
+      <c r="AA33" t="str" xml:space="preserve">
+        <v xml:space="preserve">Konstruksi Gedung Lainnya
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Periklanan
+Pertanian Pengembangbiakan Tanaman
+Pertanian Tanaman Hias</v>
       </c>
       <c r="AB33" t="str">
         <v/>
@@ -13672,8 +17211,12 @@
       <c r="Z34" t="str">
         <v/>
       </c>
-      <c r="AA34" t="str">
-        <v/>
+      <c r="AA34" t="str" xml:space="preserve">
+        <v xml:space="preserve">Konstruksi Gedung Lainnya
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Periklanan
+Pertanian Pengembangbiakan Tanaman
+Pertanian Tanaman Hias</v>
       </c>
       <c r="AB34" t="str">
         <v/>
@@ -13879,8 +17422,12 @@
       <c r="Z35" t="str">
         <v/>
       </c>
-      <c r="AA35" t="str">
-        <v/>
+      <c r="AA35" t="str" xml:space="preserve">
+        <v xml:space="preserve">Konstruksi Gedung Lainnya
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Periklanan
+Pertanian Pengembangbiakan Tanaman
+Pertanian Tanaman Hias</v>
       </c>
       <c r="AB35" t="str">
         <v/>
@@ -14047,8 +17594,10 @@
       <c r="Z36" t="str">
         <v/>
       </c>
-      <c r="AA36" t="str">
-        <v/>
+      <c r="AA36" t="str" xml:space="preserve">
+        <v xml:space="preserve">Periklanan
+Pertanian Pengembangbiakan Tanaman
+Pertanian Tanaman Hias</v>
       </c>
       <c r="AB36" t="str">
         <v/>
@@ -14242,8 +17791,12 @@
       <c r="Z37" t="str">
         <v/>
       </c>
-      <c r="AA37" t="str">
-        <v/>
+      <c r="AA37" t="str" xml:space="preserve">
+        <v xml:space="preserve">Konstruksi Gedung Lainnya
+Konstruksi Gedung Tempat Hiburan dan Olahraga
+Periklanan
+Pertanian Pengembangbiakan Tanaman
+Pertanian Tanaman Hias</v>
       </c>
       <c r="AB37" t="str">
         <v/>
@@ -14424,8 +17977,60 @@
       <c r="Z38" t="str">
         <v/>
       </c>
-      <c r="AA38" t="str">
-        <v/>
+      <c r="AA38" t="str" xml:space="preserve">
+        <v xml:space="preserve">Aktivitas Penunjang Pertambangan Dan Penggalian Lainnya
+Aktivitas Penunjang Pertambangan Minyak Bumi dan Gas Alam
+Ekstraksi Garam
+Ekstraksi Tanah Gemuk
+Jasa Pasca Panen
+Jasa Pelayanan Kesehatan Ternak
+Jasa Pemanenan
+Jasa Pemupukan, Penanaman Bibit/Benih dan Pengendalian Hama dan Gulma
+Jasa Pengetasan Telur
+Jasa Pengolahan Lahan
+Jasa Penunjang Pertanian Lainnya
+Jasa Penunjang Peternakan Lainnya
+Jasa Penyemprotan dan Penyerbukan Melalui Udara
+Jasa Perkawinan Ternak
+Pemilihan Benih Tanaman Untuk Pengembangbiakan
+Penggalian Asbes
+Penggalian Batu Apung
+Penggalian Batu Hias dan Batu Bangunan
+Penggalian Batu Kapur/Gamping
+Penggalian Batu, Pasir Dan Tanah Liat Lainnya
+Penggalian Feldspar dan Kalsit
+Penggalian Gips
+Penggalian Kerikil/Sirtu
+Penggalian Kuarsa/Pasir Kuarsa
+Penggalian Pasir
+Penggalian Tanah dan Tanah Liat
+Penggalian Tras
+Pengusahaaan Tenaga Panas Bumi
+Pertambangan Aspal Alam
+Pertambangan Bahan Galian Lainnya Yang Tidak Mengandung Bijih Besi
+Pertambangan Batu Bara
+Pertambangan Batu Mulia
+Pertambangan Belerang
+Pertambangan Bijih Bauksit
+Pertambangan Bijih Besi
+Pertambangan Bijih Logam Mulia Lainnya
+Pertambangan Bijih Mangan
+Pertambangan Bijih Nikel
+Pertambangan Bijih Tembaga
+Pertambangan Bijih Timah
+Pertambangan Bijih Timah Hitam
+Pertambangan Bijih Uranium Dan Torium
+Pertambangan Dan Penggalian Lainnya YTDL
+Pertambangan Emas dan Perak
+Pertambangan Fosfat
+Pertambangan Gas Alam
+Pertambangan Lignit
+Pertambangan Mineral, Bahan Kimia dan Bahan Pupuk Lainya
+Pertambangan Minyak Bumi
+Pertambangan Nitrat
+Pertambangan Pasir Besi
+Pertambangan Potash
+Pertambangan Yodium</v>
       </c>
       <c r="AB38" t="str">
         <v/>

</xml_diff>